<commit_message>
revised todo with ariana info
</commit_message>
<xml_diff>
--- a/Silver_Todo.xlsx
+++ b/Silver_Todo.xlsx
@@ -8,16 +8,15 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\dwg11\Silver\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DD3DB568-3017-4D22-8B1E-0F7A87ED0008}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6AB71872-1F2A-43D2-8B84-C6F3A107D1CF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="25820" windowHeight="15500" tabRatio="788" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="25820" windowHeight="15500" tabRatio="788" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Overview and Credits" sheetId="2" r:id="rId1"/>
     <sheet name="Todos" sheetId="15" r:id="rId2"/>
-    <sheet name="Lance1 Team (Intended to lose)" sheetId="16" r:id="rId3"/>
-    <sheet name="ChrisTeams" sheetId="13" r:id="rId4"/>
-    <sheet name="GiovanniTeams" sheetId="14" r:id="rId5"/>
+    <sheet name="ChrisTeams" sheetId="13" r:id="rId3"/>
+    <sheet name="ArianaGiovanniTeams" sheetId="14" r:id="rId4"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -37,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="635" uniqueCount="309">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="702" uniqueCount="339">
   <si>
     <t>Pallet Town</t>
   </si>
@@ -318,12 +317,6 @@
     <t>Lv 5</t>
   </si>
   <si>
-    <t>In Celadon:</t>
-  </si>
-  <si>
-    <t>In Silph:</t>
-  </si>
-  <si>
     <t>In Cerulean Cave:</t>
   </si>
   <si>
@@ -420,9 +413,6 @@
     <t>Refuses to give the badge. Have to go to Tohjo Falls, where you can find an old 8th badge from Giovanni, and bypass the waterfall with a secret passage</t>
   </si>
   <si>
-    <t>something with lance…</t>
-  </si>
-  <si>
     <t>One-way ledge prevents backtracking</t>
   </si>
   <si>
@@ -465,9 +455,6 @@
     <t>Cerulean Cave</t>
   </si>
   <si>
-    <t xml:space="preserve">Discover Giovanni in the gym, fight #1, can't go north, learn that there's a plot to take out the power in Kanto, Blue comes up after defeating Gio </t>
-  </si>
-  <si>
     <t>Friendship event?</t>
   </si>
   <si>
@@ -516,24 +503,9 @@
     <t>intro flashes mewtwo instead of wooper</t>
   </si>
   <si>
-    <t>Lance</t>
-  </si>
-  <si>
     <t>Dragonair</t>
   </si>
   <si>
-    <t>Lv 35</t>
-  </si>
-  <si>
-    <t>Aerodactyl</t>
-  </si>
-  <si>
-    <t>Charizard</t>
-  </si>
-  <si>
-    <t>Rock slide</t>
-  </si>
-  <si>
     <t>Wing attack</t>
   </si>
   <si>
@@ -549,48 +521,21 @@
     <t>Leer</t>
   </si>
   <si>
-    <t>Hyper Beam</t>
-  </si>
-  <si>
-    <t>Thunder Wave</t>
-  </si>
-  <si>
     <t>force a loss to lance at LoR?</t>
   </si>
   <si>
-    <t>Lv 37</t>
-  </si>
-  <si>
-    <t>Lv 39</t>
-  </si>
-  <si>
-    <t>Lv 41</t>
-  </si>
-  <si>
-    <t>Lv 43</t>
-  </si>
-  <si>
-    <t>Lv 45</t>
-  </si>
-  <si>
     <t>Hydro Pump</t>
   </si>
   <si>
     <t>Thunderbolt</t>
   </si>
   <si>
-    <t>Agility</t>
-  </si>
-  <si>
     <t>Ice Beam</t>
   </si>
   <si>
     <t>Earthquake</t>
   </si>
   <si>
-    <t>Blizzard</t>
-  </si>
-  <si>
     <t>Fire Blast</t>
   </si>
   <si>
@@ -906,9 +851,6 @@
     <t>Psychic</t>
   </si>
   <si>
-    <t>Rockets cleared out, given a zubat</t>
-  </si>
-  <si>
     <t>Talk to Mr Pokemon, get a pokedex and an exp share</t>
   </si>
   <si>
@@ -924,21 +866,12 @@
     <t>discover another room, secret lair with some computers, etc., and referencing plans to start new rocket with international people, which will let you bypass waterfall, reference power outage</t>
   </si>
   <si>
-    <t>reason to visit??</t>
-  </si>
-  <si>
-    <t>need to see player right before entering murkrow room</t>
-  </si>
-  <si>
     <t>Radio tower takeover</t>
   </si>
   <si>
     <t xml:space="preserve">Steal a magnemite from the magnet line, 'these are the strongest mons to build the rail with'. </t>
   </si>
   <si>
-    <t>rival battle. Steal an abra from the game corner while the rockets are around</t>
-  </si>
-  <si>
     <t>just do a blackout</t>
   </si>
   <si>
@@ -964,6 +897,162 @@
   </si>
   <si>
     <t>Use Chris front sprite for rival</t>
+  </si>
+  <si>
+    <t>Call from Giovanni talking about legendary pokemon</t>
+  </si>
+  <si>
+    <t xml:space="preserve">need to see player right before entering murkrow room. Talk to Ariana: "&lt;silver&gt; do you still resent me? I </t>
+  </si>
+  <si>
+    <t>reason to visit -- Ariana is there, tries to play on his insecurity "&lt;silver&gt;, I see a lot of myself in you. I saw you get beat down by Lance. If you want to actually be strong, you have to join us."</t>
+  </si>
+  <si>
+    <t>rival battle. Steal an abra from the game corner while the rockets are around. "&lt;silver&gt;, I know who you are. You look the same as the day your father took you away from me. You were always so sensitive. Are you mad at me for not giving you enough care? Team Rocket is coming back, and you're going to join. You'll never be anything without us!"</t>
+  </si>
+  <si>
+    <t>Ariana and Proton talking; Rockets cleared out, Ariana talks, "no… could it really be you? He told me that he sent you away…Battle me and show me who you are!"</t>
+  </si>
+  <si>
+    <t>Ariana</t>
+  </si>
+  <si>
+    <t>Ekans</t>
+  </si>
+  <si>
+    <t>Oddish</t>
+  </si>
+  <si>
+    <t>Murkrow</t>
+  </si>
+  <si>
+    <t>Arbok</t>
+  </si>
+  <si>
+    <t>Gloom</t>
+  </si>
+  <si>
+    <t>Radio Tower</t>
+  </si>
+  <si>
+    <t>Vileplume</t>
+  </si>
+  <si>
+    <t>Glare</t>
+  </si>
+  <si>
+    <t>Wrap</t>
+  </si>
+  <si>
+    <t>Poison Sting</t>
+  </si>
+  <si>
+    <t>Sweet Scent</t>
+  </si>
+  <si>
+    <t>Absorb</t>
+  </si>
+  <si>
+    <t>Acid</t>
+  </si>
+  <si>
+    <t>Peck</t>
+  </si>
+  <si>
+    <t>Haze</t>
+  </si>
+  <si>
+    <t>Pursuit</t>
+  </si>
+  <si>
+    <t>Night Shade</t>
+  </si>
+  <si>
+    <t>Mega Drain</t>
+  </si>
+  <si>
+    <t>Wing Attack</t>
+  </si>
+  <si>
+    <t>Astonish</t>
+  </si>
+  <si>
+    <t>Grimer</t>
+  </si>
+  <si>
+    <t>Muk</t>
+  </si>
+  <si>
+    <t>Poison Gas</t>
+  </si>
+  <si>
+    <t>Disable</t>
+  </si>
+  <si>
+    <t>Harden</t>
+  </si>
+  <si>
+    <t>Pound</t>
+  </si>
+  <si>
+    <t>Sludge</t>
+  </si>
+  <si>
+    <t>Minimize</t>
+  </si>
+  <si>
+    <t>Crunch</t>
+  </si>
+  <si>
+    <t>Mewtwo</t>
+  </si>
+  <si>
+    <t>Nidoking</t>
+  </si>
+  <si>
+    <t>Nidoqueen</t>
+  </si>
+  <si>
+    <t>Rhydon</t>
+  </si>
+  <si>
+    <t>Kangaskhan</t>
+  </si>
+  <si>
+    <t>Persian</t>
+  </si>
+  <si>
+    <t>Houndoom</t>
+  </si>
+  <si>
+    <t>Crobat</t>
+  </si>
+  <si>
+    <t>Tauros</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Discover Giovanni in the gym, fight #1, can't go north, learn that there's a plot to take out the power in Kanto, Blue comes up after defeating Gio, this encounter Gio trades with Silver to "show him how much stronger he'd be with me", </t>
+  </si>
+  <si>
+    <t>Dugtrio</t>
+  </si>
+  <si>
+    <t>Marowak</t>
+  </si>
+  <si>
+    <t>Exeggutor</t>
+  </si>
+  <si>
+    <t>Parasect</t>
+  </si>
+  <si>
+    <t>In Viridian:</t>
+  </si>
+  <si>
+    <t>Scyther</t>
+  </si>
+  <si>
+    <t>In Safari Zone:</t>
   </si>
 </sst>
 </file>
@@ -1192,7 +1281,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="43">
+  <cellXfs count="45">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -1291,6 +1380,12 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -2364,8 +2459,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4D4D23E0-802A-4842-9CD9-587C61A270C2}">
   <dimension ref="A1:E142"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A65" workbookViewId="0">
-      <selection activeCell="G79" sqref="G79"/>
+    <sheetView topLeftCell="A36" workbookViewId="0">
+      <selection activeCell="C57" sqref="C57"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
@@ -2380,21 +2475,21 @@
         <v>87</v>
       </c>
       <c r="B1" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="C1" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" s="32" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
@@ -2402,7 +2497,7 @@
         <v>29</v>
       </c>
       <c r="C3" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
@@ -2420,7 +2515,7 @@
         <v>78</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
@@ -2433,7 +2528,7 @@
         <v>32</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>290</v>
+        <v>271</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.25">
@@ -2447,7 +2542,7 @@
         <v>34</v>
       </c>
       <c r="C10" t="s">
-        <v>291</v>
+        <v>272</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.25">
@@ -2455,7 +2550,7 @@
         <v>47</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.25">
@@ -2464,7 +2559,7 @@
       </c>
       <c r="B12" s="1"/>
       <c r="C12" s="1" t="s">
-        <v>292</v>
+        <v>273</v>
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.25">
@@ -2487,7 +2582,7 @@
         <v>39</v>
       </c>
       <c r="C16" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.25">
@@ -2495,7 +2590,7 @@
         <v>40</v>
       </c>
       <c r="C17" s="1" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.25">
@@ -2503,7 +2598,7 @@
         <v>41</v>
       </c>
       <c r="C18" s="1" t="s">
-        <v>289</v>
+        <v>291</v>
       </c>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.25">
@@ -2511,7 +2606,7 @@
         <v>42</v>
       </c>
       <c r="C19" s="1" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="E19" s="1"/>
     </row>
@@ -2520,7 +2615,7 @@
         <v>43</v>
       </c>
       <c r="C20" s="1" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.25">
@@ -2528,7 +2623,7 @@
         <v>44</v>
       </c>
       <c r="C21" s="1" t="s">
-        <v>298</v>
+        <v>277</v>
       </c>
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.25">
@@ -2550,13 +2645,16 @@
       <c r="A25" s="7" t="s">
         <v>79</v>
       </c>
+      <c r="C25" t="s">
+        <v>287</v>
+      </c>
     </row>
     <row r="26" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A26" s="7" t="s">
         <v>48</v>
       </c>
       <c r="C26" s="1" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
     </row>
     <row r="27" spans="1:5" x14ac:dyDescent="0.25">
@@ -2564,7 +2662,7 @@
         <v>49</v>
       </c>
       <c r="C27" s="1" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
     </row>
     <row r="28" spans="1:5" x14ac:dyDescent="0.25">
@@ -2572,7 +2670,7 @@
         <v>68</v>
       </c>
       <c r="C28" s="1" t="s">
-        <v>294</v>
+        <v>275</v>
       </c>
     </row>
     <row r="29" spans="1:5" x14ac:dyDescent="0.25">
@@ -2590,7 +2688,7 @@
         <v>53</v>
       </c>
       <c r="C31" s="1" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
     </row>
     <row r="32" spans="1:5" x14ac:dyDescent="0.25">
@@ -2613,7 +2711,7 @@
         <v>57</v>
       </c>
       <c r="C35" s="1" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
     </row>
     <row r="36" spans="1:3" x14ac:dyDescent="0.25">
@@ -2625,9 +2723,7 @@
       <c r="A37" s="7" t="s">
         <v>76</v>
       </c>
-      <c r="C37" s="1" t="s">
-        <v>127</v>
-      </c>
+      <c r="C37" s="1"/>
     </row>
     <row r="38" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A38" s="7" t="s">
@@ -2644,7 +2740,7 @@
         <v>60</v>
       </c>
       <c r="C40" t="s">
-        <v>295</v>
+        <v>289</v>
       </c>
     </row>
     <row r="41" spans="1:3" x14ac:dyDescent="0.25">
@@ -2652,7 +2748,7 @@
         <v>61</v>
       </c>
       <c r="C41" t="s">
-        <v>296</v>
+        <v>288</v>
       </c>
     </row>
     <row r="42" spans="1:3" x14ac:dyDescent="0.25">
@@ -2660,12 +2756,12 @@
         <v>56</v>
       </c>
     </row>
-    <row r="43" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:3" ht="50" x14ac:dyDescent="0.25">
       <c r="A43" s="7" t="s">
-        <v>297</v>
-      </c>
-      <c r="C43" t="s">
-        <v>299</v>
+        <v>276</v>
+      </c>
+      <c r="C43" s="43" t="s">
+        <v>290</v>
       </c>
     </row>
     <row r="44" spans="1:3" x14ac:dyDescent="0.25">
@@ -2678,12 +2774,12 @@
         <v>63</v>
       </c>
     </row>
-    <row r="46" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:3" ht="25" x14ac:dyDescent="0.25">
       <c r="A46" s="7" t="s">
         <v>64</v>
       </c>
-      <c r="C46" s="1" t="s">
-        <v>126</v>
+      <c r="C46" s="44" t="s">
+        <v>124</v>
       </c>
     </row>
     <row r="47" spans="1:3" x14ac:dyDescent="0.25">
@@ -2716,7 +2812,7 @@
         <v>28</v>
       </c>
       <c r="C52" s="1" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
     </row>
     <row r="53" spans="1:3" x14ac:dyDescent="0.25">
@@ -2724,7 +2820,7 @@
         <v>80</v>
       </c>
       <c r="C53" t="s">
-        <v>293</v>
+        <v>274</v>
       </c>
     </row>
     <row r="54" spans="1:3" ht="13" x14ac:dyDescent="0.25">
@@ -2740,15 +2836,15 @@
         <v>3</v>
       </c>
       <c r="C56" s="1" t="s">
-        <v>128</v>
+        <v>125</v>
       </c>
     </row>
     <row r="57" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A57" s="7" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="C57" s="1" t="s">
-        <v>142</v>
+        <v>331</v>
       </c>
     </row>
     <row r="58" spans="1:3" x14ac:dyDescent="0.25">
@@ -2773,12 +2869,12 @@
         <v>5</v>
       </c>
       <c r="C61" s="1" t="s">
-        <v>143</v>
+        <v>139</v>
       </c>
     </row>
     <row r="62" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A62" s="7" t="s">
-        <v>144</v>
+        <v>140</v>
       </c>
     </row>
     <row r="63" spans="1:3" x14ac:dyDescent="0.25">
@@ -2798,10 +2894,10 @@
     </row>
     <row r="66" spans="1:3" ht="13" x14ac:dyDescent="0.25">
       <c r="A66" s="33" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="C66" s="1" t="s">
-        <v>129</v>
+        <v>126</v>
       </c>
     </row>
     <row r="67" spans="1:3" x14ac:dyDescent="0.25">
@@ -2816,23 +2912,23 @@
     </row>
     <row r="69" spans="1:3" ht="13" x14ac:dyDescent="0.25">
       <c r="A69" s="33" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
       <c r="C69" s="1" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
     </row>
     <row r="70" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A70" s="7" t="s">
-        <v>131</v>
+        <v>128</v>
       </c>
     </row>
     <row r="71" spans="1:3" ht="13" x14ac:dyDescent="0.3">
       <c r="A71" s="19" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="C71" s="1" t="s">
-        <v>132</v>
+        <v>129</v>
       </c>
     </row>
     <row r="72" spans="1:3" x14ac:dyDescent="0.25">
@@ -2843,10 +2939,10 @@
     </row>
     <row r="73" spans="1:3" ht="13" x14ac:dyDescent="0.25">
       <c r="A73" s="33" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="C73" s="1" t="s">
-        <v>137</v>
+        <v>134</v>
       </c>
     </row>
     <row r="74" spans="1:3" x14ac:dyDescent="0.25">
@@ -2857,34 +2953,34 @@
     </row>
     <row r="75" spans="1:3" ht="13" x14ac:dyDescent="0.25">
       <c r="A75" s="33" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="C75" s="1" t="s">
-        <v>136</v>
+        <v>133</v>
       </c>
     </row>
     <row r="76" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A76" s="1" t="s">
-        <v>133</v>
+        <v>130</v>
       </c>
     </row>
     <row r="77" spans="1:3" ht="13" x14ac:dyDescent="0.25">
       <c r="A77" s="34" t="s">
-        <v>130</v>
+        <v>127</v>
       </c>
     </row>
     <row r="78" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A78" s="1" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
       <c r="C78" s="1"/>
     </row>
     <row r="79" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A79" s="1" t="s">
+        <v>132</v>
+      </c>
+      <c r="C79" s="1" t="s">
         <v>135</v>
-      </c>
-      <c r="C79" s="1" t="s">
-        <v>138</v>
       </c>
     </row>
     <row r="80" spans="1:3" x14ac:dyDescent="0.25">
@@ -2895,10 +2991,10 @@
     </row>
     <row r="81" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A81" s="1" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="C81" s="1" t="s">
-        <v>139</v>
+        <v>136</v>
       </c>
     </row>
     <row r="82" spans="1:3" x14ac:dyDescent="0.25">
@@ -2908,10 +3004,10 @@
     </row>
     <row r="83" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A83" s="1" t="s">
-        <v>140</v>
+        <v>137</v>
       </c>
       <c r="B83" s="1" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
     </row>
     <row r="84" spans="1:3" x14ac:dyDescent="0.25">
@@ -2921,134 +3017,134 @@
     </row>
     <row r="85" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A85" s="1" t="s">
-        <v>141</v>
+        <v>138</v>
       </c>
     </row>
     <row r="87" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A87" t="s">
-        <v>172</v>
+        <v>161</v>
       </c>
       <c r="B87" t="s">
-        <v>300</v>
+        <v>278</v>
       </c>
     </row>
     <row r="88" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A88" s="1" t="s">
-        <v>147</v>
+        <v>143</v>
       </c>
       <c r="B88" s="1" t="s">
-        <v>305</v>
+        <v>283</v>
       </c>
     </row>
     <row r="89" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A89" s="1" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="B89" t="s">
-        <v>305</v>
+        <v>283</v>
       </c>
     </row>
     <row r="90" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A90" s="1" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="B90" t="s">
-        <v>304</v>
+        <v>282</v>
       </c>
     </row>
     <row r="91" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A91" s="1" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
     </row>
     <row r="92" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A92" s="1" t="s">
-        <v>308</v>
+        <v>286</v>
       </c>
     </row>
     <row r="93" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A93" s="1" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="B93" t="s">
-        <v>307</v>
+        <v>285</v>
       </c>
     </row>
     <row r="94" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A94" s="1" t="s">
-        <v>145</v>
+        <v>141</v>
       </c>
     </row>
     <row r="95" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A95" s="1" t="s">
-        <v>146</v>
+        <v>142</v>
       </c>
       <c r="B95" t="s">
-        <v>305</v>
+        <v>283</v>
       </c>
     </row>
     <row r="96" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A96" s="1" t="s">
-        <v>148</v>
+        <v>144</v>
       </c>
       <c r="B96" t="s">
-        <v>305</v>
+        <v>283</v>
       </c>
     </row>
     <row r="97" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A97" s="1" t="s">
-        <v>149</v>
+        <v>145</v>
       </c>
       <c r="B97" t="s">
-        <v>305</v>
+        <v>283</v>
       </c>
     </row>
     <row r="98" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A98" s="1" t="s">
-        <v>150</v>
+        <v>146</v>
       </c>
       <c r="B98" t="s">
-        <v>305</v>
+        <v>283</v>
       </c>
     </row>
     <row r="99" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A99" s="1" t="s">
+        <v>147</v>
+      </c>
+      <c r="B99" t="s">
         <v>151</v>
-      </c>
-      <c r="B99" t="s">
-        <v>155</v>
       </c>
     </row>
     <row r="100" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A100" s="1" t="s">
-        <v>152</v>
+        <v>148</v>
       </c>
       <c r="B100" t="s">
-        <v>303</v>
+        <v>281</v>
       </c>
     </row>
     <row r="101" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A101" s="1" t="s">
-        <v>153</v>
+        <v>149</v>
       </c>
       <c r="B101" t="s">
-        <v>154</v>
+        <v>150</v>
       </c>
     </row>
     <row r="102" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A102" s="1" t="s">
-        <v>158</v>
+        <v>154</v>
       </c>
       <c r="B102" t="s">
-        <v>302</v>
+        <v>280</v>
       </c>
     </row>
     <row r="103" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A103" s="1" t="s">
-        <v>301</v>
+        <v>279</v>
       </c>
       <c r="B103" t="s">
-        <v>306</v>
+        <v>284</v>
       </c>
     </row>
     <row r="112" spans="1:2" x14ac:dyDescent="0.25">
@@ -3096,7 +3192,7 @@
         <v>8</v>
       </c>
       <c r="C120" s="1" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
     </row>
     <row r="121" spans="1:3" x14ac:dyDescent="0.25">
@@ -3104,7 +3200,7 @@
         <v>9</v>
       </c>
       <c r="C121" s="1" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
     </row>
     <row r="122" spans="1:3" x14ac:dyDescent="0.25">
@@ -3132,7 +3228,7 @@
         <v>5</v>
       </c>
       <c r="C126" s="1" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
     </row>
     <row r="127" spans="1:3" x14ac:dyDescent="0.25">
@@ -3227,157 +3323,12 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{48146755-4111-4B0B-B0B2-DA4A11AE4A9F}">
-  <dimension ref="A1:I6"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="3" max="3" width="13.7265625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="9.36328125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="12.36328125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="11.453125" bestFit="1" customWidth="1"/>
-    <col min="8" max="9" width="10.7265625" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="C1" t="s">
-        <v>161</v>
-      </c>
-      <c r="D1" t="s">
-        <v>166</v>
-      </c>
-      <c r="F1" t="s">
-        <v>167</v>
-      </c>
-      <c r="G1" t="s">
-        <v>168</v>
-      </c>
-      <c r="H1" t="s">
-        <v>170</v>
-      </c>
-      <c r="I1" t="s">
-        <v>169</v>
-      </c>
-    </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>159</v>
-      </c>
-      <c r="C2" t="s">
-        <v>173</v>
-      </c>
-      <c r="D2" t="s">
-        <v>160</v>
-      </c>
-      <c r="F2" t="s">
-        <v>171</v>
-      </c>
-      <c r="G2" t="s">
-        <v>170</v>
-      </c>
-      <c r="H2" t="s">
-        <v>179</v>
-      </c>
-      <c r="I2" t="s">
-        <v>180</v>
-      </c>
-    </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="C3" t="s">
-        <v>174</v>
-      </c>
-      <c r="D3" t="s">
-        <v>162</v>
-      </c>
-      <c r="F3" t="s">
-        <v>164</v>
-      </c>
-      <c r="G3" t="s">
-        <v>165</v>
-      </c>
-      <c r="H3" t="s">
-        <v>182</v>
-      </c>
-      <c r="I3" t="s">
-        <v>170</v>
-      </c>
-    </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="C4" t="s">
-        <v>175</v>
-      </c>
-      <c r="D4" t="s">
-        <v>163</v>
-      </c>
-      <c r="F4" t="s">
-        <v>167</v>
-      </c>
-      <c r="G4" t="s">
-        <v>168</v>
-      </c>
-      <c r="H4" t="s">
-        <v>169</v>
-      </c>
-      <c r="I4" t="s">
-        <v>170</v>
-      </c>
-    </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="C5" t="s">
-        <v>176</v>
-      </c>
-      <c r="D5" t="s">
-        <v>160</v>
-      </c>
-      <c r="F5" t="s">
-        <v>171</v>
-      </c>
-      <c r="G5" t="s">
-        <v>170</v>
-      </c>
-      <c r="H5" t="s">
-        <v>181</v>
-      </c>
-      <c r="I5" t="s">
-        <v>180</v>
-      </c>
-    </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="C6" t="s">
-        <v>177</v>
-      </c>
-      <c r="D6" t="s">
-        <v>160</v>
-      </c>
-      <c r="F6" t="s">
-        <v>183</v>
-      </c>
-      <c r="G6" t="s">
-        <v>184</v>
-      </c>
-      <c r="H6" t="s">
-        <v>179</v>
-      </c>
-      <c r="I6" t="s">
-        <v>170</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DB3E0C82-6EA9-4690-9C5F-8CA3CDECAC6B}">
   <dimension ref="A1:T39"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane xSplit="1" topLeftCell="C1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="G6" sqref="G6"/>
+      <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
+      <selection pane="topRight" activeCell="A27" sqref="A27:A32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
@@ -3406,7 +3357,7 @@
     </row>
     <row r="2" spans="1:20" x14ac:dyDescent="0.25">
       <c r="C2" s="40" t="s">
-        <v>185</v>
+        <v>167</v>
       </c>
       <c r="D2" s="41"/>
       <c r="E2" s="41"/>
@@ -3414,7 +3365,7 @@
       <c r="G2" s="41"/>
       <c r="H2" s="42"/>
       <c r="I2" s="40" t="s">
-        <v>186</v>
+        <v>168</v>
       </c>
       <c r="J2" s="41"/>
       <c r="K2" s="41"/>
@@ -3422,7 +3373,7 @@
       <c r="M2" s="41"/>
       <c r="N2" s="42"/>
       <c r="O2" s="40" t="s">
-        <v>187</v>
+        <v>169</v>
       </c>
       <c r="P2" s="41"/>
       <c r="Q2" s="41"/>
@@ -3432,10 +3383,10 @@
     </row>
     <row r="3" spans="1:20" ht="13" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>226</v>
+        <v>208</v>
       </c>
       <c r="B3" s="19" t="s">
-        <v>189</v>
+        <v>171</v>
       </c>
       <c r="C3">
         <v>5</v>
@@ -3444,34 +3395,34 @@
         <v>74</v>
       </c>
       <c r="E3" t="s">
-        <v>188</v>
+        <v>170</v>
       </c>
       <c r="F3" t="s">
-        <v>169</v>
+        <v>160</v>
       </c>
       <c r="I3">
         <v>5</v>
       </c>
       <c r="J3" t="s">
-        <v>157</v>
+        <v>153</v>
       </c>
       <c r="K3" t="s">
-        <v>225</v>
+        <v>207</v>
       </c>
       <c r="L3" t="s">
-        <v>262</v>
+        <v>244</v>
       </c>
       <c r="O3" t="s">
         <v>92</v>
       </c>
       <c r="P3" t="s">
-        <v>156</v>
+        <v>152</v>
       </c>
       <c r="Q3" t="s">
-        <v>225</v>
+        <v>207</v>
       </c>
       <c r="R3" t="s">
-        <v>169</v>
+        <v>160</v>
       </c>
     </row>
     <row r="4" spans="1:20" x14ac:dyDescent="0.25">
@@ -3497,10 +3448,10 @@
     </row>
     <row r="5" spans="1:20" ht="13" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>226</v>
+        <v>208</v>
       </c>
       <c r="B5" s="19" t="s">
-        <v>263</v>
+        <v>245</v>
       </c>
       <c r="C5">
         <v>16</v>
@@ -3509,164 +3460,164 @@
         <v>74</v>
       </c>
       <c r="E5" t="s">
-        <v>224</v>
+        <v>206</v>
       </c>
       <c r="F5" t="s">
-        <v>223</v>
+        <v>205</v>
       </c>
       <c r="G5" s="1" t="s">
-        <v>169</v>
+        <v>160</v>
       </c>
       <c r="H5" s="39" t="s">
-        <v>188</v>
+        <v>170</v>
       </c>
       <c r="I5">
         <v>16</v>
       </c>
       <c r="J5" t="s">
-        <v>194</v>
+        <v>176</v>
       </c>
       <c r="K5" t="s">
-        <v>233</v>
+        <v>215</v>
       </c>
       <c r="L5" t="s">
-        <v>231</v>
+        <v>213</v>
       </c>
       <c r="M5" t="s">
-        <v>232</v>
+        <v>214</v>
       </c>
       <c r="N5" s="39" t="s">
-        <v>225</v>
+        <v>207</v>
       </c>
       <c r="O5">
         <v>14</v>
       </c>
       <c r="P5" t="s">
-        <v>193</v>
+        <v>175</v>
       </c>
       <c r="Q5" t="s">
-        <v>234</v>
+        <v>216</v>
       </c>
       <c r="R5" t="s">
-        <v>235</v>
+        <v>217</v>
       </c>
       <c r="S5" t="s">
-        <v>225</v>
+        <v>207</v>
       </c>
       <c r="T5" s="37" t="s">
-        <v>169</v>
+        <v>160</v>
       </c>
     </row>
     <row r="6" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>227</v>
+        <v>209</v>
       </c>
       <c r="B6" t="s">
-        <v>274</v>
+        <v>256</v>
       </c>
       <c r="C6">
         <v>12</v>
       </c>
       <c r="D6" t="s">
-        <v>191</v>
+        <v>173</v>
       </c>
       <c r="E6" t="s">
-        <v>218</v>
+        <v>200</v>
       </c>
       <c r="F6" t="s">
-        <v>262</v>
+        <v>244</v>
       </c>
       <c r="G6" t="s">
-        <v>219</v>
+        <v>201</v>
       </c>
       <c r="I6">
         <v>12</v>
       </c>
       <c r="J6" t="s">
-        <v>191</v>
+        <v>173</v>
       </c>
       <c r="K6" t="s">
-        <v>218</v>
+        <v>200</v>
       </c>
       <c r="L6" t="s">
-        <v>221</v>
+        <v>203</v>
       </c>
       <c r="M6" t="s">
-        <v>219</v>
+        <v>201</v>
       </c>
       <c r="N6" s="37" t="s">
-        <v>262</v>
+        <v>244</v>
       </c>
       <c r="O6">
         <v>12</v>
       </c>
       <c r="P6" t="s">
-        <v>191</v>
+        <v>173</v>
       </c>
       <c r="Q6" t="s">
-        <v>218</v>
+        <v>200</v>
       </c>
       <c r="R6" t="s">
-        <v>221</v>
+        <v>203</v>
       </c>
       <c r="S6" t="s">
-        <v>219</v>
+        <v>201</v>
       </c>
       <c r="T6" s="37" t="s">
-        <v>262</v>
+        <v>244</v>
       </c>
     </row>
     <row r="7" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>228</v>
+        <v>210</v>
       </c>
       <c r="C7">
         <v>16</v>
       </c>
       <c r="D7" t="s">
-        <v>192</v>
+        <v>174</v>
       </c>
       <c r="E7" t="s">
-        <v>222</v>
+        <v>204</v>
       </c>
       <c r="F7" t="s">
-        <v>247</v>
+        <v>229</v>
       </c>
       <c r="G7" t="s">
-        <v>234</v>
+        <v>216</v>
       </c>
       <c r="I7">
         <v>16</v>
       </c>
       <c r="J7" t="s">
-        <v>195</v>
+        <v>177</v>
       </c>
       <c r="K7" t="s">
-        <v>223</v>
+        <v>205</v>
       </c>
       <c r="L7" t="s">
-        <v>236</v>
+        <v>218</v>
       </c>
       <c r="M7" t="s">
-        <v>237</v>
+        <v>219</v>
       </c>
       <c r="O7">
         <v>18</v>
       </c>
       <c r="P7" t="s">
-        <v>196</v>
+        <v>178</v>
       </c>
       <c r="Q7" s="1" t="s">
-        <v>275</v>
+        <v>257</v>
       </c>
       <c r="R7" s="1" t="s">
-        <v>276</v>
+        <v>258</v>
       </c>
       <c r="S7" s="1" t="s">
-        <v>233</v>
+        <v>215</v>
       </c>
       <c r="T7" s="39" t="s">
-        <v>225</v>
+        <v>207</v>
       </c>
     </row>
     <row r="8" spans="1:20" s="36" customFormat="1" x14ac:dyDescent="0.25">
@@ -3676,243 +3627,243 @@
     </row>
     <row r="9" spans="1:20" ht="13" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
-        <v>226</v>
+        <v>208</v>
       </c>
       <c r="B9" s="19" t="s">
-        <v>197</v>
+        <v>179</v>
       </c>
       <c r="C9">
         <v>22</v>
       </c>
       <c r="D9" t="s">
-        <v>190</v>
+        <v>172</v>
       </c>
       <c r="E9" s="1" t="s">
-        <v>167</v>
+        <v>158</v>
       </c>
       <c r="F9" s="1" t="s">
+        <v>204</v>
+      </c>
+      <c r="G9" s="1" t="s">
+        <v>160</v>
+      </c>
+      <c r="H9" s="39" t="s">
         <v>222</v>
-      </c>
-      <c r="G9" s="1" t="s">
-        <v>169</v>
-      </c>
-      <c r="H9" s="39" t="s">
-        <v>240</v>
       </c>
       <c r="I9">
         <v>22</v>
       </c>
       <c r="J9" t="s">
-        <v>194</v>
+        <v>176</v>
       </c>
       <c r="K9" s="1" t="s">
-        <v>233</v>
+        <v>215</v>
       </c>
       <c r="L9" s="1" t="s">
-        <v>231</v>
+        <v>213</v>
       </c>
       <c r="M9" s="1" t="s">
-        <v>216</v>
+        <v>198</v>
       </c>
       <c r="N9" s="39" t="s">
-        <v>240</v>
+        <v>222</v>
       </c>
       <c r="O9">
         <v>22</v>
       </c>
       <c r="P9" t="s">
-        <v>193</v>
+        <v>175</v>
       </c>
       <c r="Q9" s="1" t="s">
-        <v>234</v>
+        <v>216</v>
       </c>
       <c r="R9" s="1" t="s">
-        <v>235</v>
+        <v>217</v>
       </c>
       <c r="S9" s="1" t="s">
-        <v>216</v>
+        <v>198</v>
       </c>
       <c r="T9" s="39" t="s">
-        <v>240</v>
+        <v>222</v>
       </c>
     </row>
     <row r="10" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>229</v>
+        <v>211</v>
       </c>
       <c r="B10" s="1"/>
       <c r="C10">
         <v>20</v>
       </c>
       <c r="D10" t="s">
-        <v>199</v>
+        <v>181</v>
       </c>
       <c r="E10" t="s">
+        <v>202</v>
+      </c>
+      <c r="F10" t="s">
         <v>220</v>
       </c>
-      <c r="F10" t="s">
-        <v>238</v>
-      </c>
       <c r="G10" t="s">
-        <v>218</v>
+        <v>200</v>
       </c>
       <c r="H10" s="37" t="s">
-        <v>198</v>
+        <v>180</v>
       </c>
       <c r="I10">
         <v>20</v>
       </c>
       <c r="J10" t="s">
-        <v>199</v>
+        <v>181</v>
       </c>
       <c r="K10" t="s">
+        <v>202</v>
+      </c>
+      <c r="L10" t="s">
         <v>220</v>
       </c>
-      <c r="L10" t="s">
-        <v>238</v>
-      </c>
       <c r="M10" t="s">
-        <v>218</v>
+        <v>200</v>
       </c>
       <c r="N10" s="37" t="s">
-        <v>198</v>
+        <v>180</v>
       </c>
       <c r="O10">
         <v>20</v>
       </c>
       <c r="P10" t="s">
-        <v>199</v>
+        <v>181</v>
       </c>
       <c r="Q10" t="s">
+        <v>202</v>
+      </c>
+      <c r="R10" t="s">
         <v>220</v>
       </c>
-      <c r="R10" t="s">
-        <v>238</v>
-      </c>
       <c r="S10" t="s">
-        <v>218</v>
+        <v>200</v>
       </c>
       <c r="T10" s="37" t="s">
-        <v>198</v>
+        <v>180</v>
       </c>
     </row>
     <row r="11" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>228</v>
+        <v>210</v>
       </c>
       <c r="C11">
         <v>20</v>
       </c>
       <c r="D11" t="s">
-        <v>192</v>
+        <v>174</v>
       </c>
       <c r="E11" t="s">
-        <v>222</v>
+        <v>204</v>
       </c>
       <c r="F11" t="s">
-        <v>247</v>
+        <v>229</v>
       </c>
       <c r="G11" t="s">
-        <v>234</v>
+        <v>216</v>
       </c>
       <c r="H11" s="37" t="s">
-        <v>169</v>
+        <v>160</v>
       </c>
       <c r="I11">
         <v>20</v>
       </c>
       <c r="J11" t="s">
-        <v>201</v>
+        <v>183</v>
       </c>
       <c r="K11" s="1" t="s">
-        <v>223</v>
+        <v>205</v>
       </c>
       <c r="L11" s="1" t="s">
-        <v>236</v>
+        <v>218</v>
       </c>
       <c r="M11" s="1" t="s">
-        <v>264</v>
+        <v>246</v>
       </c>
       <c r="N11" s="39" t="s">
-        <v>265</v>
+        <v>247</v>
       </c>
       <c r="O11">
         <v>20</v>
       </c>
       <c r="P11" t="s">
-        <v>196</v>
+        <v>178</v>
       </c>
       <c r="Q11" s="1" t="s">
-        <v>275</v>
+        <v>257</v>
       </c>
       <c r="R11" s="1" t="s">
-        <v>276</v>
+        <v>258</v>
       </c>
       <c r="S11" s="1" t="s">
-        <v>233</v>
+        <v>215</v>
       </c>
       <c r="T11" s="39" t="s">
-        <v>225</v>
+        <v>207</v>
       </c>
     </row>
     <row r="12" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>230</v>
+        <v>212</v>
       </c>
       <c r="B12" s="1"/>
       <c r="C12">
         <v>18</v>
       </c>
       <c r="D12" t="s">
-        <v>200</v>
+        <v>182</v>
       </c>
       <c r="E12" t="s">
-        <v>255</v>
+        <v>237</v>
       </c>
       <c r="F12" t="s">
-        <v>169</v>
+        <v>160</v>
       </c>
       <c r="G12" t="s">
-        <v>256</v>
+        <v>238</v>
       </c>
       <c r="H12" s="37" t="s">
-        <v>257</v>
+        <v>239</v>
       </c>
       <c r="I12">
         <v>18</v>
       </c>
       <c r="J12" t="s">
-        <v>202</v>
+        <v>184</v>
       </c>
       <c r="K12" s="1" t="s">
-        <v>234</v>
+        <v>216</v>
       </c>
       <c r="L12" s="1" t="s">
-        <v>257</v>
+        <v>239</v>
       </c>
       <c r="M12" s="1" t="s">
-        <v>268</v>
+        <v>250</v>
       </c>
       <c r="N12" s="39" t="s">
-        <v>169</v>
+        <v>160</v>
       </c>
       <c r="O12">
         <v>18</v>
       </c>
       <c r="P12" t="s">
-        <v>203</v>
+        <v>185</v>
       </c>
       <c r="Q12" s="1" t="s">
-        <v>282</v>
+        <v>264</v>
       </c>
       <c r="R12" s="1" t="s">
-        <v>283</v>
+        <v>265</v>
       </c>
       <c r="S12" s="1" t="s">
-        <v>284</v>
+        <v>266</v>
       </c>
       <c r="T12" s="39" t="s">
-        <v>285</v>
+        <v>267</v>
       </c>
     </row>
     <row r="13" spans="1:20" s="36" customFormat="1" x14ac:dyDescent="0.25">
@@ -3922,300 +3873,300 @@
     </row>
     <row r="14" spans="1:20" ht="13" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
-        <v>226</v>
+        <v>208</v>
       </c>
       <c r="B14" s="19" t="s">
-        <v>204</v>
+        <v>186</v>
       </c>
       <c r="C14">
         <v>32</v>
       </c>
       <c r="D14" t="s">
-        <v>213</v>
+        <v>195</v>
       </c>
       <c r="E14" t="s">
-        <v>198</v>
+        <v>180</v>
       </c>
       <c r="F14" s="1" t="s">
-        <v>167</v>
+        <v>158</v>
       </c>
       <c r="G14" s="1" t="s">
+        <v>204</v>
+      </c>
+      <c r="H14" s="39" t="s">
         <v>222</v>
-      </c>
-      <c r="H14" s="39" t="s">
-        <v>240</v>
       </c>
       <c r="I14">
         <v>32</v>
       </c>
       <c r="J14" t="s">
-        <v>214</v>
+        <v>196</v>
       </c>
       <c r="K14" t="s">
-        <v>198</v>
+        <v>180</v>
       </c>
       <c r="L14" s="1" t="s">
-        <v>231</v>
+        <v>213</v>
       </c>
       <c r="M14" s="1" t="s">
-        <v>241</v>
+        <v>223</v>
       </c>
       <c r="N14" s="39" t="s">
-        <v>240</v>
+        <v>222</v>
       </c>
       <c r="O14">
         <v>36</v>
       </c>
       <c r="P14" t="s">
-        <v>215</v>
+        <v>197</v>
       </c>
       <c r="Q14" t="s">
-        <v>198</v>
+        <v>180</v>
       </c>
       <c r="R14" s="1" t="s">
-        <v>245</v>
+        <v>227</v>
       </c>
       <c r="S14" s="1" t="s">
-        <v>246</v>
+        <v>228</v>
       </c>
       <c r="T14" s="39" t="s">
-        <v>240</v>
+        <v>222</v>
       </c>
     </row>
     <row r="15" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>229</v>
+        <v>211</v>
       </c>
       <c r="C15">
         <v>32</v>
       </c>
       <c r="D15" t="s">
-        <v>199</v>
+        <v>181</v>
       </c>
       <c r="E15" t="s">
-        <v>198</v>
+        <v>180</v>
       </c>
       <c r="F15" t="s">
-        <v>238</v>
+        <v>220</v>
       </c>
       <c r="G15" t="s">
-        <v>218</v>
+        <v>200</v>
       </c>
       <c r="H15" s="39" t="s">
-        <v>239</v>
+        <v>221</v>
       </c>
       <c r="I15">
         <v>32</v>
       </c>
       <c r="J15" t="s">
-        <v>199</v>
+        <v>181</v>
       </c>
       <c r="K15" t="s">
-        <v>198</v>
+        <v>180</v>
       </c>
       <c r="L15" t="s">
-        <v>238</v>
+        <v>220</v>
       </c>
       <c r="M15" t="s">
-        <v>218</v>
+        <v>200</v>
       </c>
       <c r="N15" s="39" t="s">
-        <v>239</v>
+        <v>221</v>
       </c>
       <c r="O15">
         <v>28</v>
       </c>
       <c r="P15" t="s">
-        <v>199</v>
+        <v>181</v>
       </c>
       <c r="Q15" t="s">
-        <v>198</v>
+        <v>180</v>
       </c>
       <c r="R15" t="s">
-        <v>238</v>
+        <v>220</v>
       </c>
       <c r="S15" t="s">
-        <v>218</v>
+        <v>200</v>
       </c>
       <c r="T15" s="39" t="s">
-        <v>239</v>
+        <v>221</v>
       </c>
     </row>
     <row r="16" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>228</v>
+        <v>210</v>
       </c>
       <c r="C16">
         <v>32</v>
       </c>
       <c r="D16" t="s">
-        <v>211</v>
+        <v>193</v>
       </c>
       <c r="E16" t="s">
-        <v>222</v>
+        <v>204</v>
       </c>
       <c r="F16" t="s">
+        <v>198</v>
+      </c>
+      <c r="G16" t="s">
         <v>216</v>
       </c>
-      <c r="G16" t="s">
-        <v>234</v>
-      </c>
       <c r="H16" s="37" t="s">
-        <v>169</v>
+        <v>160</v>
       </c>
       <c r="I16">
         <v>32</v>
       </c>
       <c r="J16" t="s">
-        <v>201</v>
+        <v>183</v>
       </c>
       <c r="K16" s="1" t="s">
-        <v>266</v>
+        <v>248</v>
       </c>
       <c r="L16" s="1" t="s">
-        <v>236</v>
+        <v>218</v>
       </c>
       <c r="M16" s="1" t="s">
-        <v>264</v>
+        <v>246</v>
       </c>
       <c r="N16" s="39" t="s">
-        <v>246</v>
+        <v>228</v>
       </c>
       <c r="O16">
         <v>32</v>
       </c>
       <c r="P16" t="s">
-        <v>210</v>
+        <v>192</v>
       </c>
       <c r="Q16" s="1" t="s">
-        <v>277</v>
+        <v>259</v>
       </c>
       <c r="R16" s="1" t="s">
-        <v>278</v>
+        <v>260</v>
       </c>
       <c r="S16" s="1" t="s">
-        <v>233</v>
+        <v>215</v>
       </c>
       <c r="T16" s="39" t="s">
-        <v>279</v>
+        <v>261</v>
       </c>
     </row>
     <row r="17" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>230</v>
+        <v>212</v>
       </c>
       <c r="C17">
         <v>30</v>
       </c>
       <c r="D17" t="s">
-        <v>205</v>
+        <v>187</v>
       </c>
       <c r="E17" t="s">
-        <v>255</v>
+        <v>237</v>
       </c>
       <c r="F17" t="s">
-        <v>169</v>
+        <v>160</v>
       </c>
       <c r="G17" t="s">
-        <v>256</v>
+        <v>238</v>
       </c>
       <c r="H17" s="37" t="s">
-        <v>257</v>
+        <v>239</v>
       </c>
       <c r="I17">
         <v>30</v>
       </c>
       <c r="J17" t="s">
-        <v>206</v>
+        <v>188</v>
       </c>
       <c r="K17" s="1" t="s">
-        <v>267</v>
+        <v>249</v>
       </c>
       <c r="L17" s="1" t="s">
-        <v>257</v>
+        <v>239</v>
       </c>
       <c r="M17" s="1" t="s">
-        <v>268</v>
+        <v>250</v>
       </c>
       <c r="N17" s="39" t="s">
-        <v>235</v>
+        <v>217</v>
       </c>
       <c r="O17">
         <v>30</v>
       </c>
       <c r="P17" t="s">
-        <v>207</v>
+        <v>189</v>
       </c>
       <c r="Q17" s="1" t="s">
-        <v>271</v>
+        <v>253</v>
       </c>
       <c r="R17" s="1" t="s">
-        <v>257</v>
+        <v>239</v>
       </c>
       <c r="S17" s="1" t="s">
-        <v>284</v>
+        <v>266</v>
       </c>
       <c r="T17" s="39" t="s">
-        <v>286</v>
+        <v>268</v>
       </c>
     </row>
     <row r="18" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>248</v>
+        <v>230</v>
       </c>
       <c r="C18">
         <v>30</v>
       </c>
       <c r="D18" t="s">
-        <v>166</v>
+        <v>157</v>
       </c>
       <c r="E18" t="s">
-        <v>167</v>
+        <v>158</v>
       </c>
       <c r="F18" t="s">
-        <v>208</v>
+        <v>190</v>
       </c>
       <c r="G18" t="s">
-        <v>168</v>
+        <v>159</v>
       </c>
       <c r="H18" s="37" t="s">
-        <v>259</v>
+        <v>241</v>
       </c>
       <c r="I18">
         <v>30</v>
       </c>
       <c r="J18" t="s">
-        <v>166</v>
+        <v>157</v>
       </c>
       <c r="K18" t="s">
-        <v>167</v>
+        <v>158</v>
       </c>
       <c r="L18" t="s">
-        <v>208</v>
+        <v>190</v>
       </c>
       <c r="M18" t="s">
-        <v>168</v>
+        <v>159</v>
       </c>
       <c r="N18" s="37" t="s">
-        <v>259</v>
+        <v>241</v>
       </c>
       <c r="O18">
         <v>30</v>
       </c>
       <c r="P18" t="s">
-        <v>166</v>
+        <v>157</v>
       </c>
       <c r="Q18" t="s">
-        <v>167</v>
+        <v>158</v>
       </c>
       <c r="R18" t="s">
-        <v>208</v>
+        <v>190</v>
       </c>
       <c r="S18" t="s">
-        <v>168</v>
+        <v>159</v>
       </c>
       <c r="T18" s="37" t="s">
-        <v>259</v>
+        <v>241</v>
       </c>
     </row>
     <row r="19" spans="1:20" s="36" customFormat="1" x14ac:dyDescent="0.25">
@@ -4225,7 +4176,7 @@
     </row>
     <row r="20" spans="1:20" ht="12.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
-        <v>226</v>
+        <v>208</v>
       </c>
       <c r="B20" s="19" t="s">
         <v>28</v>
@@ -4234,350 +4185,350 @@
         <v>38</v>
       </c>
       <c r="D20" t="s">
-        <v>213</v>
+        <v>195</v>
       </c>
       <c r="E20" s="1" t="s">
-        <v>198</v>
+        <v>180</v>
       </c>
       <c r="F20" s="1" t="s">
-        <v>167</v>
+        <v>158</v>
       </c>
       <c r="G20" s="1" t="s">
-        <v>222</v>
+        <v>204</v>
       </c>
       <c r="H20" s="39" t="s">
-        <v>246</v>
+        <v>228</v>
       </c>
       <c r="I20">
         <v>38</v>
       </c>
       <c r="J20" t="s">
-        <v>214</v>
+        <v>196</v>
       </c>
       <c r="K20" s="1" t="s">
-        <v>198</v>
+        <v>180</v>
       </c>
       <c r="L20" s="1" t="s">
-        <v>241</v>
+        <v>223</v>
       </c>
       <c r="M20" s="1" t="s">
-        <v>231</v>
+        <v>213</v>
       </c>
       <c r="N20" s="39" t="s">
-        <v>242</v>
+        <v>224</v>
       </c>
       <c r="O20">
         <v>38</v>
       </c>
       <c r="P20" t="s">
-        <v>215</v>
+        <v>197</v>
       </c>
       <c r="Q20" s="1" t="s">
-        <v>198</v>
+        <v>180</v>
       </c>
       <c r="R20" s="1" t="s">
-        <v>245</v>
+        <v>227</v>
       </c>
       <c r="S20" s="1" t="s">
-        <v>246</v>
+        <v>228</v>
       </c>
       <c r="T20" s="39" t="s">
-        <v>242</v>
+        <v>224</v>
       </c>
     </row>
     <row r="21" spans="1:20" ht="12.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>229</v>
+        <v>211</v>
       </c>
       <c r="C21">
         <v>36</v>
       </c>
       <c r="D21" t="s">
-        <v>199</v>
+        <v>181</v>
       </c>
       <c r="E21" t="s">
-        <v>198</v>
+        <v>180</v>
       </c>
       <c r="F21" t="s">
-        <v>238</v>
+        <v>220</v>
       </c>
       <c r="G21" t="s">
-        <v>218</v>
+        <v>200</v>
       </c>
       <c r="H21" s="39" t="s">
-        <v>239</v>
+        <v>221</v>
       </c>
       <c r="I21">
         <v>36</v>
       </c>
       <c r="J21" t="s">
-        <v>199</v>
+        <v>181</v>
       </c>
       <c r="K21" t="s">
-        <v>198</v>
+        <v>180</v>
       </c>
       <c r="L21" t="s">
-        <v>238</v>
+        <v>220</v>
       </c>
       <c r="M21" t="s">
-        <v>218</v>
+        <v>200</v>
       </c>
       <c r="N21" s="39" t="s">
-        <v>239</v>
+        <v>221</v>
       </c>
       <c r="O21">
         <v>36</v>
       </c>
       <c r="P21" t="s">
-        <v>199</v>
+        <v>181</v>
       </c>
       <c r="Q21" t="s">
-        <v>198</v>
+        <v>180</v>
       </c>
       <c r="R21" t="s">
-        <v>238</v>
+        <v>220</v>
       </c>
       <c r="S21" t="s">
-        <v>218</v>
+        <v>200</v>
       </c>
       <c r="T21" s="39" t="s">
-        <v>239</v>
+        <v>221</v>
       </c>
     </row>
     <row r="22" spans="1:20" ht="12.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>252</v>
+        <v>234</v>
       </c>
       <c r="C22">
         <v>35</v>
       </c>
       <c r="D22" t="s">
-        <v>211</v>
+        <v>193</v>
       </c>
       <c r="E22" t="s">
-        <v>222</v>
+        <v>204</v>
       </c>
       <c r="F22" t="s">
+        <v>198</v>
+      </c>
+      <c r="G22" t="s">
         <v>216</v>
       </c>
-      <c r="G22" t="s">
-        <v>234</v>
-      </c>
       <c r="H22" s="37" t="s">
-        <v>254</v>
+        <v>236</v>
       </c>
       <c r="I22">
         <v>35</v>
       </c>
       <c r="J22" t="s">
-        <v>201</v>
+        <v>183</v>
       </c>
       <c r="K22" s="1" t="s">
-        <v>266</v>
+        <v>248</v>
       </c>
       <c r="L22" s="1" t="s">
-        <v>182</v>
+        <v>165</v>
       </c>
       <c r="M22" s="1" t="s">
-        <v>236</v>
+        <v>218</v>
       </c>
       <c r="N22" s="39" t="s">
-        <v>237</v>
+        <v>219</v>
       </c>
       <c r="O22">
         <v>35</v>
       </c>
       <c r="P22" t="s">
-        <v>210</v>
+        <v>192</v>
       </c>
       <c r="Q22" s="1" t="s">
-        <v>277</v>
+        <v>259</v>
       </c>
       <c r="R22" s="1" t="s">
-        <v>278</v>
+        <v>260</v>
       </c>
       <c r="S22" s="1" t="s">
-        <v>233</v>
+        <v>215</v>
       </c>
       <c r="T22" s="39" t="s">
-        <v>279</v>
+        <v>261</v>
       </c>
     </row>
     <row r="23" spans="1:20" ht="12.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>251</v>
+        <v>233</v>
       </c>
       <c r="C23">
         <v>36</v>
       </c>
       <c r="D23" t="s">
-        <v>205</v>
+        <v>187</v>
       </c>
       <c r="E23" t="s">
-        <v>255</v>
+        <v>237</v>
       </c>
       <c r="F23" t="s">
-        <v>258</v>
+        <v>240</v>
       </c>
       <c r="G23" t="s">
-        <v>256</v>
+        <v>238</v>
       </c>
       <c r="H23" s="37" t="s">
-        <v>257</v>
+        <v>239</v>
       </c>
       <c r="I23">
         <v>35</v>
       </c>
       <c r="J23" t="s">
-        <v>206</v>
+        <v>188</v>
       </c>
       <c r="K23" s="1" t="s">
-        <v>267</v>
+        <v>249</v>
       </c>
       <c r="L23" s="1" t="s">
-        <v>257</v>
+        <v>239</v>
       </c>
       <c r="M23" s="1" t="s">
-        <v>269</v>
+        <v>251</v>
       </c>
       <c r="N23" s="39" t="s">
-        <v>235</v>
+        <v>217</v>
       </c>
       <c r="O23">
         <v>35</v>
       </c>
       <c r="P23" t="s">
-        <v>207</v>
+        <v>189</v>
       </c>
       <c r="Q23" s="1" t="s">
-        <v>271</v>
+        <v>253</v>
       </c>
       <c r="R23" s="1" t="s">
-        <v>257</v>
+        <v>239</v>
       </c>
       <c r="S23" s="1" t="s">
-        <v>284</v>
+        <v>266</v>
       </c>
       <c r="T23" s="39" t="s">
-        <v>286</v>
+        <v>268</v>
       </c>
     </row>
     <row r="24" spans="1:20" ht="12.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>248</v>
+        <v>230</v>
       </c>
       <c r="C24">
         <v>33</v>
       </c>
       <c r="D24" t="s">
-        <v>166</v>
+        <v>157</v>
       </c>
       <c r="E24" t="s">
-        <v>167</v>
+        <v>158</v>
       </c>
       <c r="F24" t="s">
-        <v>208</v>
+        <v>190</v>
       </c>
       <c r="G24" t="s">
-        <v>261</v>
+        <v>243</v>
       </c>
       <c r="H24" s="37" t="s">
-        <v>260</v>
+        <v>242</v>
       </c>
       <c r="I24">
         <v>35</v>
       </c>
       <c r="J24" t="s">
-        <v>166</v>
+        <v>157</v>
       </c>
       <c r="K24" t="s">
-        <v>167</v>
+        <v>158</v>
       </c>
       <c r="L24" t="s">
-        <v>208</v>
+        <v>190</v>
       </c>
       <c r="M24" t="s">
-        <v>261</v>
+        <v>243</v>
       </c>
       <c r="N24" s="37" t="s">
-        <v>260</v>
+        <v>242</v>
       </c>
       <c r="O24">
         <v>35</v>
       </c>
       <c r="P24" t="s">
-        <v>166</v>
+        <v>157</v>
       </c>
       <c r="Q24" t="s">
-        <v>167</v>
+        <v>158</v>
       </c>
       <c r="R24" t="s">
-        <v>208</v>
+        <v>190</v>
       </c>
       <c r="S24" t="s">
-        <v>261</v>
+        <v>243</v>
       </c>
       <c r="T24" s="37" t="s">
-        <v>260</v>
+        <v>242</v>
       </c>
     </row>
     <row r="25" spans="1:20" ht="12.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>249</v>
+        <v>231</v>
       </c>
       <c r="C25">
         <v>35</v>
       </c>
       <c r="D25" t="s">
-        <v>160</v>
+        <v>155</v>
       </c>
       <c r="E25" t="s">
-        <v>209</v>
+        <v>191</v>
       </c>
       <c r="F25" t="s">
-        <v>217</v>
+        <v>199</v>
       </c>
       <c r="G25" t="s">
-        <v>270</v>
+        <v>252</v>
       </c>
       <c r="H25" s="39" t="s">
-        <v>272</v>
+        <v>254</v>
       </c>
       <c r="I25">
         <v>35</v>
       </c>
       <c r="J25" t="s">
-        <v>160</v>
+        <v>155</v>
       </c>
       <c r="K25" t="s">
-        <v>209</v>
+        <v>191</v>
       </c>
       <c r="L25" t="s">
-        <v>217</v>
+        <v>199</v>
       </c>
       <c r="M25" t="s">
-        <v>270</v>
+        <v>252</v>
       </c>
       <c r="N25" s="39" t="s">
-        <v>272</v>
+        <v>254</v>
       </c>
       <c r="O25">
         <v>35</v>
       </c>
       <c r="P25" t="s">
-        <v>160</v>
+        <v>155</v>
       </c>
       <c r="Q25" t="s">
-        <v>209</v>
+        <v>191</v>
       </c>
       <c r="R25" t="s">
-        <v>217</v>
+        <v>199</v>
       </c>
       <c r="S25" t="s">
-        <v>270</v>
+        <v>252</v>
       </c>
       <c r="T25" s="39" t="s">
-        <v>272</v>
+        <v>254</v>
       </c>
     </row>
     <row r="26" spans="1:20" s="36" customFormat="1" ht="12.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -4587,359 +4538,359 @@
     </row>
     <row r="27" spans="1:20" ht="13" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
-        <v>226</v>
+        <v>208</v>
       </c>
       <c r="B27" s="19" t="s">
-        <v>140</v>
+        <v>137</v>
       </c>
       <c r="C27">
         <v>45</v>
       </c>
       <c r="D27" s="1" t="s">
-        <v>213</v>
+        <v>195</v>
       </c>
       <c r="E27" s="1" t="s">
-        <v>198</v>
+        <v>180</v>
       </c>
       <c r="F27" s="1" t="s">
-        <v>246</v>
+        <v>228</v>
       </c>
       <c r="G27" s="1" t="s">
-        <v>178</v>
+        <v>162</v>
       </c>
       <c r="H27" s="39" t="s">
-        <v>181</v>
+        <v>164</v>
       </c>
       <c r="I27">
         <v>45</v>
       </c>
       <c r="J27" s="1" t="s">
-        <v>214</v>
+        <v>196</v>
       </c>
       <c r="K27" t="s">
-        <v>198</v>
+        <v>180</v>
       </c>
       <c r="L27" s="1" t="s">
-        <v>241</v>
+        <v>223</v>
       </c>
       <c r="M27" s="1" t="s">
-        <v>243</v>
+        <v>225</v>
       </c>
       <c r="N27" s="39" t="s">
-        <v>242</v>
+        <v>224</v>
       </c>
       <c r="O27">
         <v>45</v>
       </c>
       <c r="P27" s="1" t="s">
-        <v>215</v>
+        <v>197</v>
       </c>
       <c r="Q27" s="1" t="s">
-        <v>198</v>
+        <v>180</v>
       </c>
       <c r="R27" s="1" t="s">
-        <v>246</v>
+        <v>228</v>
       </c>
       <c r="S27" s="1" t="s">
-        <v>242</v>
+        <v>224</v>
       </c>
       <c r="T27" s="39" t="s">
-        <v>244</v>
+        <v>226</v>
       </c>
     </row>
     <row r="28" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>250</v>
+        <v>232</v>
       </c>
       <c r="C28">
         <v>43</v>
       </c>
       <c r="D28" t="s">
-        <v>199</v>
+        <v>181</v>
       </c>
       <c r="E28" t="s">
-        <v>198</v>
+        <v>180</v>
       </c>
       <c r="F28" t="s">
-        <v>238</v>
+        <v>220</v>
       </c>
       <c r="G28" t="s">
-        <v>218</v>
+        <v>200</v>
       </c>
       <c r="H28" s="39" t="s">
-        <v>239</v>
+        <v>221</v>
       </c>
       <c r="I28">
         <v>43</v>
       </c>
       <c r="J28" t="s">
-        <v>199</v>
+        <v>181</v>
       </c>
       <c r="K28" t="s">
-        <v>198</v>
+        <v>180</v>
       </c>
       <c r="L28" t="s">
-        <v>238</v>
+        <v>220</v>
       </c>
       <c r="M28" t="s">
-        <v>218</v>
+        <v>200</v>
       </c>
       <c r="N28" s="39" t="s">
-        <v>239</v>
+        <v>221</v>
       </c>
       <c r="O28">
         <v>43</v>
       </c>
       <c r="P28" t="s">
-        <v>199</v>
+        <v>181</v>
       </c>
       <c r="Q28" t="s">
-        <v>198</v>
+        <v>180</v>
       </c>
       <c r="R28" t="s">
-        <v>238</v>
+        <v>220</v>
       </c>
       <c r="S28" t="s">
-        <v>218</v>
+        <v>200</v>
       </c>
       <c r="T28" s="39" t="s">
-        <v>239</v>
+        <v>221</v>
       </c>
     </row>
     <row r="29" spans="1:20" ht="12.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>252</v>
+        <v>234</v>
       </c>
       <c r="C29">
         <v>42</v>
       </c>
       <c r="D29" t="s">
-        <v>211</v>
+        <v>193</v>
       </c>
       <c r="E29" t="s">
-        <v>222</v>
+        <v>204</v>
       </c>
       <c r="F29" t="s">
-        <v>216</v>
+        <v>198</v>
       </c>
       <c r="G29" t="s">
-        <v>184</v>
+        <v>166</v>
       </c>
       <c r="H29" s="37" t="s">
-        <v>254</v>
+        <v>236</v>
       </c>
       <c r="I29">
         <v>42</v>
       </c>
       <c r="J29" t="s">
-        <v>201</v>
+        <v>183</v>
       </c>
       <c r="K29" s="1" t="s">
-        <v>266</v>
+        <v>248</v>
       </c>
       <c r="L29" s="1" t="s">
-        <v>182</v>
+        <v>165</v>
       </c>
       <c r="M29" s="1" t="s">
+        <v>218</v>
+      </c>
+      <c r="N29" s="39" t="s">
         <v>236</v>
-      </c>
-      <c r="N29" s="39" t="s">
-        <v>254</v>
       </c>
       <c r="O29">
         <v>44</v>
       </c>
       <c r="P29" t="s">
-        <v>210</v>
+        <v>192</v>
       </c>
       <c r="Q29" s="1" t="s">
-        <v>280</v>
+        <v>262</v>
       </c>
       <c r="R29" s="1" t="s">
-        <v>281</v>
+        <v>263</v>
       </c>
       <c r="S29" s="1" t="s">
-        <v>278</v>
+        <v>260</v>
       </c>
       <c r="T29" s="39" t="s">
-        <v>279</v>
+        <v>261</v>
       </c>
     </row>
     <row r="30" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>251</v>
+        <v>233</v>
       </c>
       <c r="C30">
         <v>47</v>
       </c>
       <c r="D30" t="s">
-        <v>205</v>
+        <v>187</v>
       </c>
       <c r="E30" t="s">
-        <v>179</v>
+        <v>163</v>
       </c>
       <c r="F30" t="s">
-        <v>258</v>
+        <v>240</v>
       </c>
       <c r="G30" t="s">
-        <v>256</v>
+        <v>238</v>
       </c>
       <c r="H30" s="37" t="s">
-        <v>257</v>
+        <v>239</v>
       </c>
       <c r="I30">
         <v>47</v>
       </c>
       <c r="J30" t="s">
-        <v>206</v>
+        <v>188</v>
       </c>
       <c r="K30" s="1" t="s">
-        <v>244</v>
+        <v>226</v>
       </c>
       <c r="L30" s="1" t="s">
-        <v>257</v>
+        <v>239</v>
       </c>
       <c r="M30" s="1" t="s">
-        <v>269</v>
+        <v>251</v>
       </c>
       <c r="N30" s="39" t="s">
-        <v>255</v>
+        <v>237</v>
       </c>
       <c r="O30">
         <v>47</v>
       </c>
       <c r="P30" t="s">
-        <v>207</v>
+        <v>189</v>
       </c>
       <c r="Q30" s="1" t="s">
-        <v>287</v>
+        <v>269</v>
       </c>
       <c r="R30" s="1" t="s">
-        <v>288</v>
+        <v>270</v>
       </c>
       <c r="S30" s="1" t="s">
-        <v>284</v>
+        <v>266</v>
       </c>
       <c r="T30" s="39" t="s">
-        <v>241</v>
+        <v>223</v>
       </c>
     </row>
     <row r="31" spans="1:20" ht="12.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
-        <v>248</v>
+        <v>230</v>
       </c>
       <c r="C31">
         <v>41</v>
       </c>
       <c r="D31" t="s">
-        <v>166</v>
+        <v>157</v>
       </c>
       <c r="E31" t="s">
-        <v>167</v>
+        <v>158</v>
       </c>
       <c r="F31" t="s">
-        <v>208</v>
+        <v>190</v>
       </c>
       <c r="G31" t="s">
-        <v>261</v>
+        <v>243</v>
       </c>
       <c r="H31" s="37" t="s">
-        <v>260</v>
+        <v>242</v>
       </c>
       <c r="I31">
         <v>41</v>
       </c>
       <c r="J31" t="s">
-        <v>166</v>
+        <v>157</v>
       </c>
       <c r="K31" t="s">
-        <v>167</v>
+        <v>158</v>
       </c>
       <c r="L31" t="s">
-        <v>208</v>
+        <v>190</v>
       </c>
       <c r="M31" t="s">
-        <v>261</v>
+        <v>243</v>
       </c>
       <c r="N31" s="37" t="s">
-        <v>260</v>
+        <v>242</v>
       </c>
       <c r="O31">
         <v>41</v>
       </c>
       <c r="P31" t="s">
-        <v>166</v>
+        <v>157</v>
       </c>
       <c r="Q31" t="s">
-        <v>167</v>
+        <v>158</v>
       </c>
       <c r="R31" t="s">
-        <v>208</v>
+        <v>190</v>
       </c>
       <c r="S31" t="s">
-        <v>261</v>
+        <v>243</v>
       </c>
       <c r="T31" s="37" t="s">
-        <v>260</v>
+        <v>242</v>
       </c>
     </row>
     <row r="32" spans="1:20" ht="12.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
-        <v>253</v>
+        <v>235</v>
       </c>
       <c r="C32">
         <v>45</v>
       </c>
       <c r="D32" t="s">
-        <v>212</v>
+        <v>194</v>
       </c>
       <c r="E32" t="s">
-        <v>209</v>
+        <v>191</v>
       </c>
       <c r="F32" t="s">
-        <v>217</v>
+        <v>199</v>
       </c>
       <c r="G32" t="s">
-        <v>270</v>
+        <v>252</v>
       </c>
       <c r="H32" s="39" t="s">
-        <v>273</v>
+        <v>255</v>
       </c>
       <c r="I32">
         <v>45</v>
       </c>
       <c r="J32" t="s">
-        <v>212</v>
+        <v>194</v>
       </c>
       <c r="K32" t="s">
-        <v>209</v>
+        <v>191</v>
       </c>
       <c r="L32" t="s">
-        <v>217</v>
+        <v>199</v>
       </c>
       <c r="M32" t="s">
-        <v>270</v>
+        <v>252</v>
       </c>
       <c r="N32" s="39" t="s">
-        <v>273</v>
+        <v>255</v>
       </c>
       <c r="O32">
         <v>45</v>
       </c>
       <c r="P32" t="s">
-        <v>212</v>
+        <v>194</v>
       </c>
       <c r="Q32" t="s">
-        <v>209</v>
+        <v>191</v>
       </c>
       <c r="R32" t="s">
-        <v>217</v>
+        <v>199</v>
       </c>
       <c r="S32" t="s">
-        <v>270</v>
+        <v>252</v>
       </c>
       <c r="T32" s="39" t="s">
-        <v>273</v>
+        <v>255</v>
       </c>
     </row>
     <row r="33" ht="12.5" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -4960,35 +4911,440 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5CCA6904-CCBA-4CF4-893E-058C20254CB5}">
-  <dimension ref="A2:A8"/>
+  <dimension ref="A1:K38"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H20" sqref="H20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="15.1796875" bestFit="1" customWidth="1"/>
+    <col min="3" max="7" width="15.6328125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>292</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11" ht="13" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>41</v>
+      </c>
+      <c r="B3">
+        <v>12</v>
+      </c>
+      <c r="C3" t="s">
+        <v>293</v>
+      </c>
+      <c r="D3" t="s">
+        <v>301</v>
+      </c>
+      <c r="E3" t="s">
+        <v>160</v>
+      </c>
+      <c r="F3" t="s">
+        <v>302</v>
+      </c>
+      <c r="G3" s="19" t="s">
+        <v>308</v>
+      </c>
+      <c r="K3" t="s">
+        <v>208</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="B4">
+        <v>12</v>
+      </c>
+      <c r="C4" t="s">
+        <v>294</v>
+      </c>
+      <c r="D4" t="s">
+        <v>304</v>
+      </c>
+      <c r="E4" t="s">
+        <v>303</v>
+      </c>
+      <c r="K4" t="s">
+        <v>209</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="B5">
+        <v>11</v>
+      </c>
+      <c r="C5" t="s">
+        <v>313</v>
+      </c>
+      <c r="D5" t="s">
+        <v>315</v>
+      </c>
+      <c r="E5" t="s">
+        <v>316</v>
+      </c>
+      <c r="F5" t="s">
+        <v>317</v>
+      </c>
+      <c r="G5" t="s">
+        <v>318</v>
+      </c>
+      <c r="K5" t="s">
+        <v>210</v>
+      </c>
+    </row>
+    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>61</v>
+      </c>
+      <c r="B7">
+        <v>23</v>
+      </c>
+      <c r="C7" t="s">
+        <v>296</v>
+      </c>
+      <c r="D7" t="s">
+        <v>300</v>
+      </c>
+      <c r="E7" t="s">
+        <v>204</v>
+      </c>
+      <c r="F7" t="s">
+        <v>301</v>
+      </c>
+      <c r="G7" t="s">
+        <v>302</v>
+      </c>
+      <c r="K7" t="s">
+        <v>208</v>
+      </c>
+    </row>
+    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="B8">
+        <v>23</v>
+      </c>
+      <c r="C8" t="s">
+        <v>297</v>
+      </c>
+      <c r="D8" t="s">
+        <v>303</v>
+      </c>
+      <c r="E8" t="s">
+        <v>310</v>
+      </c>
+      <c r="F8" t="s">
+        <v>305</v>
+      </c>
+      <c r="G8" t="s">
+        <v>257</v>
+      </c>
+      <c r="K8" t="s">
+        <v>211</v>
+      </c>
+    </row>
+    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="B9">
+        <v>25</v>
+      </c>
+      <c r="C9" t="s">
+        <v>295</v>
+      </c>
+      <c r="D9" t="s">
+        <v>306</v>
+      </c>
+      <c r="E9" t="s">
+        <v>307</v>
+      </c>
+      <c r="F9" t="s">
+        <v>308</v>
+      </c>
+      <c r="G9" t="s">
+        <v>309</v>
+      </c>
+      <c r="K9" s="1" t="s">
+        <v>234</v>
+      </c>
+    </row>
+    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="B10">
+        <v>25</v>
+      </c>
+      <c r="C10" t="s">
+        <v>313</v>
+      </c>
+      <c r="D10" t="s">
+        <v>319</v>
+      </c>
+      <c r="E10" t="s">
+        <v>320</v>
+      </c>
+      <c r="F10" t="s">
+        <v>316</v>
+      </c>
+      <c r="G10" t="s">
+        <v>247</v>
+      </c>
+      <c r="K10" t="s">
+        <v>212</v>
+      </c>
+    </row>
+    <row r="12" spans="1:11" ht="13" x14ac:dyDescent="0.3">
+      <c r="A12" t="s">
+        <v>298</v>
+      </c>
+      <c r="B12">
+        <v>32</v>
+      </c>
+      <c r="C12" t="s">
+        <v>296</v>
+      </c>
+      <c r="D12" t="s">
+        <v>300</v>
+      </c>
+      <c r="E12" s="19" t="s">
+        <v>321</v>
+      </c>
+      <c r="F12" t="s">
+        <v>301</v>
+      </c>
+      <c r="G12" t="s">
+        <v>302</v>
+      </c>
+      <c r="K12" t="s">
+        <v>208</v>
+      </c>
+    </row>
+    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="B13">
+        <v>32</v>
+      </c>
+      <c r="C13" t="s">
+        <v>299</v>
+      </c>
+      <c r="D13" t="s">
+        <v>303</v>
+      </c>
+      <c r="E13" t="s">
+        <v>310</v>
+      </c>
+      <c r="F13" t="s">
+        <v>305</v>
+      </c>
+      <c r="G13" t="s">
+        <v>257</v>
+      </c>
+      <c r="K13" t="s">
+        <v>211</v>
+      </c>
+    </row>
+    <row r="14" spans="1:11" ht="13" x14ac:dyDescent="0.3">
+      <c r="B14">
+        <v>32</v>
+      </c>
+      <c r="C14" t="s">
+        <v>295</v>
+      </c>
+      <c r="D14" s="19" t="s">
+        <v>311</v>
+      </c>
+      <c r="E14" t="s">
+        <v>312</v>
+      </c>
+      <c r="F14" t="s">
+        <v>308</v>
+      </c>
+      <c r="G14" t="s">
+        <v>309</v>
+      </c>
+      <c r="K14" s="1" t="s">
+        <v>234</v>
+      </c>
+    </row>
+    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="B15">
+        <v>32</v>
+      </c>
+      <c r="C15" t="s">
+        <v>314</v>
+      </c>
+      <c r="D15" t="s">
+        <v>319</v>
+      </c>
+      <c r="E15" t="s">
+        <v>320</v>
+      </c>
+      <c r="F15" t="s">
+        <v>240</v>
+      </c>
+      <c r="G15" t="s">
+        <v>249</v>
+      </c>
+      <c r="K15" s="1" t="s">
+        <v>233</v>
+      </c>
+    </row>
+    <row r="16" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="K16" t="s">
+        <v>230</v>
+      </c>
+    </row>
+    <row r="19" spans="1:11" ht="13" x14ac:dyDescent="0.3">
+      <c r="A19" s="1" t="s">
+        <v>336</v>
+      </c>
+      <c r="C19" s="1" t="s">
+        <v>328</v>
+      </c>
+      <c r="D19" s="19" t="s">
+        <v>321</v>
+      </c>
+      <c r="K19" t="s">
+        <v>208</v>
+      </c>
+    </row>
+    <row r="20" spans="1:11" ht="13" x14ac:dyDescent="0.3">
+      <c r="C20" s="1" t="s">
+        <v>329</v>
+      </c>
+      <c r="D20" s="19" t="s">
+        <v>156</v>
+      </c>
+      <c r="K20" t="s">
+        <v>211</v>
+      </c>
+    </row>
+    <row r="21" spans="1:11" ht="13" x14ac:dyDescent="0.3">
+      <c r="C21" s="1" t="s">
+        <v>330</v>
+      </c>
+      <c r="D21" s="19" t="s">
+        <v>308</v>
+      </c>
+      <c r="K21" t="s">
+        <v>234</v>
+      </c>
+    </row>
+    <row r="22" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="E22" s="1"/>
+      <c r="K22" t="s">
+        <v>233</v>
+      </c>
+    </row>
+    <row r="23" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="K23" t="s">
+        <v>230</v>
+      </c>
+    </row>
+    <row r="24" spans="1:11" ht="13" x14ac:dyDescent="0.3">
+      <c r="D24" s="19"/>
+      <c r="K24" t="s">
+        <v>231</v>
+      </c>
+    </row>
+    <row r="26" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A26" s="1" t="s">
+        <v>338</v>
+      </c>
+      <c r="C26" s="1" t="s">
+        <v>333</v>
+      </c>
+      <c r="K26" t="s">
+        <v>208</v>
+      </c>
+    </row>
+    <row r="27" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="C27" s="1" t="s">
+        <v>334</v>
+      </c>
+      <c r="K27" t="s">
+        <v>232</v>
+      </c>
+    </row>
+    <row r="28" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="C28" s="1" t="s">
+        <v>335</v>
+      </c>
+      <c r="K28" t="s">
+        <v>234</v>
+      </c>
+    </row>
+    <row r="29" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="C29" s="1" t="s">
+        <v>326</v>
+      </c>
+      <c r="K29" t="s">
+        <v>233</v>
+      </c>
+    </row>
+    <row r="30" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="C30" s="1" t="s">
+        <v>337</v>
+      </c>
+      <c r="K30" t="s">
+        <v>230</v>
+      </c>
+    </row>
+    <row r="31" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="K31" t="s">
+        <v>235</v>
+      </c>
+    </row>
+    <row r="33" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A33" t="s">
         <v>93</v>
       </c>
-    </row>
-    <row r="5" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
-        <v>94</v>
-      </c>
-    </row>
-    <row r="8" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
-        <v>95</v>
+      <c r="C33" t="s">
+        <v>322</v>
+      </c>
+      <c r="K33" t="s">
+        <v>208</v>
+      </c>
+    </row>
+    <row r="34" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="C34" t="s">
+        <v>323</v>
+      </c>
+      <c r="K34" t="s">
+        <v>232</v>
+      </c>
+    </row>
+    <row r="35" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="C35" t="s">
+        <v>324</v>
+      </c>
+      <c r="K35" t="s">
+        <v>234</v>
+      </c>
+    </row>
+    <row r="36" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="C36" t="s">
+        <v>325</v>
+      </c>
+      <c r="K36" t="s">
+        <v>233</v>
+      </c>
+    </row>
+    <row r="37" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="C37" t="s">
+        <v>327</v>
+      </c>
+      <c r="K37" t="s">
+        <v>230</v>
+      </c>
+    </row>
+    <row r="38" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="C38" s="1" t="s">
+        <v>332</v>
+      </c>
+      <c r="K38" t="s">
+        <v>235</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
new parties, new giovanni, cleaned up PLC maps
</commit_message>
<xml_diff>
--- a/Silver_Todo.xlsx
+++ b/Silver_Todo.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\dwg11\Silver\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6AB71872-1F2A-43D2-8B84-C6F3A107D1CF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9B6F08DB-4A47-4C21-A5A3-8061E0F25605}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="25820" windowHeight="15500" tabRatio="788" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="25820" windowHeight="15500" tabRatio="788" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Overview and Credits" sheetId="2" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="702" uniqueCount="339">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="773" uniqueCount="378">
   <si>
     <t>Pallet Town</t>
   </si>
@@ -1046,13 +1046,130 @@
     <t>Parasect</t>
   </si>
   <si>
-    <t>In Viridian:</t>
-  </si>
-  <si>
-    <t>Scyther</t>
-  </si>
-  <si>
     <t>In Safari Zone:</t>
+  </si>
+  <si>
+    <t>Machamp</t>
+  </si>
+  <si>
+    <t>Porygon2</t>
+  </si>
+  <si>
+    <t>Recover</t>
+  </si>
+  <si>
+    <t>Tri Attack</t>
+  </si>
+  <si>
+    <t>Swords Dance</t>
+  </si>
+  <si>
+    <t>Pinsir</t>
+  </si>
+  <si>
+    <t>In Silph:</t>
+  </si>
+  <si>
+    <t>Frustration</t>
+  </si>
+  <si>
+    <t>In Viridian: No battle, just trades</t>
+  </si>
+  <si>
+    <t>Bonemerang</t>
+  </si>
+  <si>
+    <t>Focus Energy</t>
+  </si>
+  <si>
+    <t>Egg Bomb</t>
+  </si>
+  <si>
+    <t>Moonlight</t>
+  </si>
+  <si>
+    <t>Slash</t>
+  </si>
+  <si>
+    <t>Leech Life</t>
+  </si>
+  <si>
+    <t>Reversal</t>
+  </si>
+  <si>
+    <t>Mega Punch</t>
+  </si>
+  <si>
+    <t>Guillotine</t>
+  </si>
+  <si>
+    <t>Submission</t>
+  </si>
+  <si>
+    <t>Swagger</t>
+  </si>
+  <si>
+    <t>HP Bug</t>
+  </si>
+  <si>
+    <t>Faint Attack</t>
+  </si>
+  <si>
+    <t>Confuse Ray</t>
+  </si>
+  <si>
+    <t>Mean Look</t>
+  </si>
+  <si>
+    <t>Zap Cannon</t>
+  </si>
+  <si>
+    <t>Lock-On</t>
+  </si>
+  <si>
+    <t>Cross Chop</t>
+  </si>
+  <si>
+    <t>Scary Face</t>
+  </si>
+  <si>
+    <t>Thunder</t>
+  </si>
+  <si>
+    <t>Double Kick</t>
+  </si>
+  <si>
+    <t>Rock Slide</t>
+  </si>
+  <si>
+    <t>Fury Attack</t>
+  </si>
+  <si>
+    <t>Sand-attack</t>
+  </si>
+  <si>
+    <t>Ho-Oh</t>
+  </si>
+  <si>
+    <t>Detect</t>
+  </si>
+  <si>
+    <t xml:space="preserve">only way to gain happiness is through elder at dden, who will then max out the happiness. </t>
+  </si>
+  <si>
+    <t>extra rare candy at entrance</t>
+  </si>
+  <si>
+    <t>cal team, gio tem</t>
+  </si>
+  <si>
+    <t>m/f?</t>
+  </si>
+  <si>
+    <t>t.d.</t>
+  </si>
+  <si>
+    <t>intro text for giovanni</t>
   </si>
 </sst>
 </file>
@@ -1372,6 +1489,12 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1381,18 +1504,29 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="1">
+  <dxfs count="3">
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="1"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <fill>
         <patternFill>
@@ -2459,8 +2593,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4D4D23E0-802A-4842-9CD9-587C61A270C2}">
   <dimension ref="A1:E142"/>
   <sheetViews>
-    <sheetView topLeftCell="A36" workbookViewId="0">
-      <selection activeCell="C57" sqref="C57"/>
+    <sheetView tabSelected="1" topLeftCell="A57" workbookViewId="0">
+      <selection activeCell="B105" sqref="B105"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
@@ -2760,7 +2894,7 @@
       <c r="A43" s="7" t="s">
         <v>276</v>
       </c>
-      <c r="C43" s="43" t="s">
+      <c r="C43" s="40" t="s">
         <v>290</v>
       </c>
     </row>
@@ -2778,7 +2912,7 @@
       <c r="A46" s="7" t="s">
         <v>64</v>
       </c>
-      <c r="C46" s="44" t="s">
+      <c r="C46" s="41" t="s">
         <v>124</v>
       </c>
     </row>
@@ -2786,6 +2920,9 @@
       <c r="A47" s="7" t="s">
         <v>65</v>
       </c>
+      <c r="C47" t="s">
+        <v>373</v>
+      </c>
     </row>
     <row r="48" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A48" s="8" t="s">
@@ -3033,7 +3170,7 @@
         <v>143</v>
       </c>
       <c r="B88" s="1" t="s">
-        <v>283</v>
+        <v>280</v>
       </c>
     </row>
     <row r="89" spans="1:3" x14ac:dyDescent="0.25">
@@ -3041,7 +3178,7 @@
         <v>107</v>
       </c>
       <c r="B89" t="s">
-        <v>283</v>
+        <v>280</v>
       </c>
     </row>
     <row r="90" spans="1:3" x14ac:dyDescent="0.25">
@@ -3056,11 +3193,17 @@
       <c r="A91" s="1" t="s">
         <v>109</v>
       </c>
+      <c r="B91" t="s">
+        <v>376</v>
+      </c>
     </row>
     <row r="92" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A92" s="1" t="s">
         <v>286</v>
       </c>
+      <c r="B92" t="s">
+        <v>376</v>
+      </c>
     </row>
     <row r="93" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A93" s="1" t="s">
@@ -3074,6 +3217,9 @@
       <c r="A94" s="1" t="s">
         <v>141</v>
       </c>
+      <c r="B94" t="s">
+        <v>375</v>
+      </c>
     </row>
     <row r="95" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A95" s="1" t="s">
@@ -3088,7 +3234,7 @@
         <v>144</v>
       </c>
       <c r="B96" t="s">
-        <v>283</v>
+        <v>374</v>
       </c>
     </row>
     <row r="97" spans="1:2" x14ac:dyDescent="0.25">
@@ -3147,6 +3293,16 @@
         <v>284</v>
       </c>
     </row>
+    <row r="104" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A104" s="1" t="s">
+        <v>372</v>
+      </c>
+    </row>
+    <row r="105" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A105" s="1" t="s">
+        <v>377</v>
+      </c>
+    </row>
     <row r="112" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A112" s="7" t="s">
         <v>18</v>
@@ -3313,8 +3469,13 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="A112:A142 A77 A72:A75 A1:A70">
-    <cfRule type="containsBlanks" dxfId="0" priority="1">
+    <cfRule type="containsBlanks" dxfId="2" priority="2">
       <formula>LEN(TRIM(A1))=0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A1:C1048576">
+    <cfRule type="cellIs" dxfId="0" priority="1" operator="equal">
+      <formula>"done"</formula>
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -3356,30 +3517,30 @@
       </c>
     </row>
     <row r="2" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="C2" s="40" t="s">
+      <c r="C2" s="42" t="s">
         <v>167</v>
       </c>
-      <c r="D2" s="41"/>
-      <c r="E2" s="41"/>
-      <c r="F2" s="41"/>
-      <c r="G2" s="41"/>
-      <c r="H2" s="42"/>
-      <c r="I2" s="40" t="s">
+      <c r="D2" s="43"/>
+      <c r="E2" s="43"/>
+      <c r="F2" s="43"/>
+      <c r="G2" s="43"/>
+      <c r="H2" s="44"/>
+      <c r="I2" s="42" t="s">
         <v>168</v>
       </c>
-      <c r="J2" s="41"/>
-      <c r="K2" s="41"/>
-      <c r="L2" s="41"/>
-      <c r="M2" s="41"/>
-      <c r="N2" s="42"/>
-      <c r="O2" s="40" t="s">
+      <c r="J2" s="43"/>
+      <c r="K2" s="43"/>
+      <c r="L2" s="43"/>
+      <c r="M2" s="43"/>
+      <c r="N2" s="44"/>
+      <c r="O2" s="42" t="s">
         <v>169</v>
       </c>
-      <c r="P2" s="41"/>
-      <c r="Q2" s="41"/>
-      <c r="R2" s="41"/>
-      <c r="S2" s="41"/>
-      <c r="T2" s="42"/>
+      <c r="P2" s="43"/>
+      <c r="Q2" s="43"/>
+      <c r="R2" s="43"/>
+      <c r="S2" s="43"/>
+      <c r="T2" s="44"/>
     </row>
     <row r="3" spans="1:20" ht="13" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
@@ -4913,10 +5074,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5CCA6904-CCBA-4CF4-893E-058C20254CB5}">
-  <dimension ref="A1:K38"/>
+  <dimension ref="A1:K39"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H20" sqref="H20"/>
+    <sheetView topLeftCell="A5" workbookViewId="0">
+      <selection activeCell="P17" sqref="P17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
@@ -5107,8 +5268,8 @@
       <c r="E12" s="19" t="s">
         <v>321</v>
       </c>
-      <c r="F12" t="s">
-        <v>301</v>
+      <c r="F12" s="19" t="s">
+        <v>240</v>
       </c>
       <c r="G12" t="s">
         <v>302</v>
@@ -5117,18 +5278,18 @@
         <v>208</v>
       </c>
     </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:11" ht="13" x14ac:dyDescent="0.3">
       <c r="B13">
         <v>32</v>
       </c>
       <c r="C13" t="s">
         <v>299</v>
       </c>
-      <c r="D13" t="s">
-        <v>303</v>
-      </c>
-      <c r="E13" t="s">
-        <v>310</v>
+      <c r="D13" s="19" t="s">
+        <v>341</v>
+      </c>
+      <c r="E13" s="19" t="s">
+        <v>349</v>
       </c>
       <c r="F13" t="s">
         <v>305</v>
@@ -5153,8 +5314,8 @@
       <c r="E14" t="s">
         <v>312</v>
       </c>
-      <c r="F14" t="s">
-        <v>308</v>
+      <c r="F14" s="19" t="s">
+        <v>358</v>
       </c>
       <c r="G14" t="s">
         <v>309</v>
@@ -5191,49 +5352,129 @@
         <v>230</v>
       </c>
     </row>
-    <row r="19" spans="1:11" ht="13" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A17" s="1" t="s">
+        <v>345</v>
+      </c>
+      <c r="D17">
+        <f>COUNTIF(D19:G38, "?")</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="19" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A19" s="1" t="s">
         <v>336</v>
       </c>
+      <c r="B19">
+        <v>45</v>
+      </c>
       <c r="C19" s="1" t="s">
-        <v>328</v>
-      </c>
-      <c r="D19" s="19" t="s">
-        <v>321</v>
+        <v>333</v>
+      </c>
+      <c r="D19" s="1" t="s">
+        <v>346</v>
+      </c>
+      <c r="E19" s="1" t="s">
+        <v>347</v>
+      </c>
+      <c r="F19" s="1" t="s">
+        <v>241</v>
+      </c>
+      <c r="G19" s="1" t="s">
+        <v>255</v>
       </c>
       <c r="K19" t="s">
         <v>208</v>
       </c>
     </row>
     <row r="20" spans="1:11" ht="13" x14ac:dyDescent="0.3">
+      <c r="B20">
+        <v>45</v>
+      </c>
       <c r="C20" s="1" t="s">
-        <v>329</v>
-      </c>
-      <c r="D20" s="19" t="s">
-        <v>156</v>
+        <v>334</v>
+      </c>
+      <c r="D20" s="1" t="s">
+        <v>348</v>
+      </c>
+      <c r="E20" s="1" t="s">
+        <v>303</v>
+      </c>
+      <c r="F20" s="1" t="s">
+        <v>270</v>
+      </c>
+      <c r="G20" s="19" t="s">
+        <v>349</v>
       </c>
       <c r="K20" t="s">
-        <v>211</v>
+        <v>232</v>
       </c>
     </row>
     <row r="21" spans="1:11" ht="13" x14ac:dyDescent="0.3">
+      <c r="B21">
+        <v>45</v>
+      </c>
       <c r="C21" s="1" t="s">
-        <v>330</v>
+        <v>335</v>
       </c>
       <c r="D21" s="19" t="s">
-        <v>308</v>
+        <v>341</v>
+      </c>
+      <c r="E21" s="1" t="s">
+        <v>350</v>
+      </c>
+      <c r="F21" s="1" t="s">
+        <v>351</v>
+      </c>
+      <c r="G21" s="1" t="s">
+        <v>258</v>
       </c>
       <c r="K21" t="s">
         <v>234</v>
       </c>
     </row>
     <row r="22" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="E22" s="1"/>
+      <c r="B22">
+        <v>45</v>
+      </c>
+      <c r="C22" s="1" t="s">
+        <v>326</v>
+      </c>
+      <c r="D22" s="1" t="s">
+        <v>239</v>
+      </c>
+      <c r="E22" s="1" t="s">
+        <v>352</v>
+      </c>
+      <c r="F22" s="1" t="s">
+        <v>204</v>
+      </c>
+      <c r="G22" s="1" t="s">
+        <v>353</v>
+      </c>
       <c r="K22" t="s">
         <v>233</v>
       </c>
     </row>
     <row r="23" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="B23">
+        <v>45</v>
+      </c>
+      <c r="C23" s="1" t="s">
+        <v>342</v>
+      </c>
+      <c r="D23" s="1" t="s">
+        <v>341</v>
+      </c>
+      <c r="E23" s="1" t="s">
+        <v>354</v>
+      </c>
+      <c r="F23" s="1" t="s">
+        <v>355</v>
+      </c>
+      <c r="G23" s="1" t="s">
+        <v>357</v>
+      </c>
       <c r="K23" t="s">
         <v>230</v>
       </c>
@@ -5241,47 +5482,122 @@
     <row r="24" spans="1:11" ht="13" x14ac:dyDescent="0.3">
       <c r="D24" s="19"/>
       <c r="K24" t="s">
-        <v>231</v>
-      </c>
-    </row>
-    <row r="26" spans="1:11" x14ac:dyDescent="0.25">
+        <v>235</v>
+      </c>
+    </row>
+    <row r="26" spans="1:11" ht="13" x14ac:dyDescent="0.3">
       <c r="A26" s="1" t="s">
-        <v>338</v>
+        <v>343</v>
+      </c>
+      <c r="B26">
+        <v>48</v>
       </c>
       <c r="C26" s="1" t="s">
-        <v>333</v>
+        <v>328</v>
+      </c>
+      <c r="D26" s="19" t="s">
+        <v>321</v>
+      </c>
+      <c r="E26" s="19" t="s">
+        <v>226</v>
+      </c>
+      <c r="F26" s="1" t="s">
+        <v>250</v>
+      </c>
+      <c r="G26" s="1" t="s">
+        <v>229</v>
       </c>
       <c r="K26" t="s">
         <v>208</v>
       </c>
     </row>
-    <row r="27" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:11" ht="13" x14ac:dyDescent="0.3">
+      <c r="B27">
+        <v>52</v>
+      </c>
       <c r="C27" s="1" t="s">
-        <v>334</v>
+        <v>329</v>
+      </c>
+      <c r="D27" s="19" t="s">
+        <v>156</v>
+      </c>
+      <c r="E27" s="19" t="s">
+        <v>358</v>
+      </c>
+      <c r="F27" s="1" t="s">
+        <v>360</v>
+      </c>
+      <c r="G27" s="1" t="s">
+        <v>359</v>
       </c>
       <c r="K27" t="s">
         <v>232</v>
       </c>
     </row>
-    <row r="28" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:11" ht="13" x14ac:dyDescent="0.3">
+      <c r="B28">
+        <v>50</v>
+      </c>
       <c r="C28" s="1" t="s">
-        <v>335</v>
+        <v>330</v>
+      </c>
+      <c r="D28" s="19" t="s">
+        <v>308</v>
+      </c>
+      <c r="E28" s="1" t="s">
+        <v>344</v>
+      </c>
+      <c r="F28" s="1" t="s">
+        <v>206</v>
+      </c>
+      <c r="G28" s="1" t="s">
+        <v>236</v>
       </c>
       <c r="K28" t="s">
         <v>234</v>
       </c>
     </row>
     <row r="29" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="B29">
+        <v>50</v>
+      </c>
       <c r="C29" s="1" t="s">
-        <v>326</v>
+        <v>338</v>
+      </c>
+      <c r="D29" s="1" t="s">
+        <v>339</v>
+      </c>
+      <c r="E29" s="1" t="s">
+        <v>340</v>
+      </c>
+      <c r="F29" s="1" t="s">
+        <v>361</v>
+      </c>
+      <c r="G29" s="1" t="s">
+        <v>362</v>
       </c>
       <c r="K29" t="s">
         <v>233</v>
       </c>
     </row>
     <row r="30" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="B30">
+        <v>50</v>
+      </c>
       <c r="C30" s="1" t="s">
         <v>337</v>
+      </c>
+      <c r="D30" s="1" t="s">
+        <v>363</v>
+      </c>
+      <c r="E30" s="1" t="s">
+        <v>364</v>
+      </c>
+      <c r="F30" s="1" t="s">
+        <v>249</v>
+      </c>
+      <c r="G30" s="1" t="s">
+        <v>223</v>
       </c>
       <c r="K30" t="s">
         <v>230</v>
@@ -5296,51 +5612,146 @@
       <c r="A33" t="s">
         <v>93</v>
       </c>
+      <c r="B33">
+        <v>66</v>
+      </c>
       <c r="C33" t="s">
         <v>322</v>
       </c>
+      <c r="D33" s="1" t="s">
+        <v>270</v>
+      </c>
+      <c r="E33" s="1" t="s">
+        <v>249</v>
+      </c>
+      <c r="F33" s="1" t="s">
+        <v>237</v>
+      </c>
+      <c r="G33" s="1" t="s">
+        <v>203</v>
+      </c>
       <c r="K33" t="s">
         <v>208</v>
       </c>
     </row>
     <row r="34" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="B34">
+        <v>60</v>
+      </c>
       <c r="C34" t="s">
         <v>323</v>
       </c>
+      <c r="D34" s="1" t="s">
+        <v>365</v>
+      </c>
+      <c r="E34" s="1" t="s">
+        <v>165</v>
+      </c>
+      <c r="F34" s="1" t="s">
+        <v>160</v>
+      </c>
+      <c r="G34" s="1" t="s">
+        <v>366</v>
+      </c>
       <c r="K34" t="s">
         <v>232</v>
       </c>
     </row>
     <row r="35" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="B35">
+        <v>60</v>
+      </c>
       <c r="C35" t="s">
         <v>324</v>
       </c>
+      <c r="D35" s="1" t="s">
+        <v>164</v>
+      </c>
+      <c r="E35" s="1" t="s">
+        <v>165</v>
+      </c>
+      <c r="F35" s="1" t="s">
+        <v>160</v>
+      </c>
+      <c r="G35" s="1" t="s">
+        <v>366</v>
+      </c>
       <c r="K35" t="s">
         <v>234</v>
       </c>
     </row>
     <row r="36" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="B36">
+        <v>62</v>
+      </c>
       <c r="C36" t="s">
         <v>325</v>
       </c>
+      <c r="D36" s="1" t="s">
+        <v>165</v>
+      </c>
+      <c r="E36" s="1" t="s">
+        <v>367</v>
+      </c>
+      <c r="F36" s="1" t="s">
+        <v>364</v>
+      </c>
+      <c r="G36" s="1" t="s">
+        <v>368</v>
+      </c>
       <c r="K36" t="s">
         <v>233</v>
       </c>
     </row>
     <row r="37" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="B37">
+        <v>65</v>
+      </c>
       <c r="C37" t="s">
         <v>327</v>
       </c>
+      <c r="D37" s="1" t="s">
+        <v>350</v>
+      </c>
+      <c r="E37" s="1" t="s">
+        <v>240</v>
+      </c>
+      <c r="F37" s="1" t="s">
+        <v>371</v>
+      </c>
+      <c r="G37" s="1" t="s">
+        <v>356</v>
+      </c>
       <c r="K37" t="s">
         <v>230</v>
       </c>
     </row>
-    <row r="38" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:11" ht="13" x14ac:dyDescent="0.3">
+      <c r="B38">
+        <v>60</v>
+      </c>
       <c r="C38" s="1" t="s">
         <v>332</v>
       </c>
+      <c r="D38" s="1" t="s">
+        <v>165</v>
+      </c>
+      <c r="E38" s="1" t="s">
+        <v>369</v>
+      </c>
+      <c r="F38" s="1" t="s">
+        <v>350</v>
+      </c>
+      <c r="G38" s="19" t="s">
+        <v>240</v>
+      </c>
       <c r="K38" t="s">
         <v>235</v>
+      </c>
+    </row>
+    <row r="39" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="K39" s="1" t="s">
+        <v>370</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
added giovanni OW sprite and giovanni trainer sprite
</commit_message>
<xml_diff>
--- a/Silver_Todo.xlsx
+++ b/Silver_Todo.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\dwg11\Silver\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9B6F08DB-4A47-4C21-A5A3-8061E0F25605}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E470D5E7-6BAC-42FD-AEAE-2CF9901EC843}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="25820" windowHeight="15500" tabRatio="788" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="25820" windowHeight="15500" tabRatio="788" firstSheet="1" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Overview and Credits" sheetId="2" r:id="rId1"/>
@@ -884,9 +884,6 @@
     <t>if needed? May revise f/b and OW sprite to have this option?</t>
   </si>
   <si>
-    <t>gfx\trainers\oak is where pokemon prof is, only time that it is used</t>
-  </si>
-  <si>
     <t>tutorial</t>
   </si>
   <si>
@@ -974,9 +971,6 @@
     <t>Wing Attack</t>
   </si>
   <si>
-    <t>Astonish</t>
-  </si>
-  <si>
     <t>Grimer</t>
   </si>
   <si>
@@ -1170,6 +1164,12 @@
   </si>
   <si>
     <t>intro text for giovanni</t>
+  </si>
+  <si>
+    <t>Add a new trainer class · pret/pokecrystal Wiki (github.com)</t>
+  </si>
+  <si>
+    <t>palfix needed at gfx/trainers/giovanni.png</t>
   </si>
 </sst>
 </file>
@@ -1398,7 +1398,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="45">
+  <cellXfs count="46">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -1504,12 +1504,13 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="3">
+  <dxfs count="2">
     <dxf>
       <font>
         <color rgb="FF006100"/>
@@ -1517,13 +1518,6 @@
       <fill>
         <patternFill>
           <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="1"/>
         </patternFill>
       </fill>
     </dxf>
@@ -2593,8 +2587,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4D4D23E0-802A-4842-9CD9-587C61A270C2}">
   <dimension ref="A1:E142"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A57" workbookViewId="0">
-      <selection activeCell="B105" sqref="B105"/>
+    <sheetView tabSelected="1" topLeftCell="A63" workbookViewId="0">
+      <selection activeCell="B91" sqref="B91"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
@@ -2732,7 +2726,7 @@
         <v>41</v>
       </c>
       <c r="C18" s="1" t="s">
-        <v>291</v>
+        <v>290</v>
       </c>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.25">
@@ -2780,7 +2774,7 @@
         <v>79</v>
       </c>
       <c r="C25" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
     </row>
     <row r="26" spans="1:5" x14ac:dyDescent="0.25">
@@ -2874,7 +2868,7 @@
         <v>60</v>
       </c>
       <c r="C40" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
     </row>
     <row r="41" spans="1:3" x14ac:dyDescent="0.25">
@@ -2882,7 +2876,7 @@
         <v>61</v>
       </c>
       <c r="C41" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
     </row>
     <row r="42" spans="1:3" x14ac:dyDescent="0.25">
@@ -2895,7 +2889,7 @@
         <v>276</v>
       </c>
       <c r="C43" s="40" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
     </row>
     <row r="44" spans="1:3" x14ac:dyDescent="0.25">
@@ -2921,7 +2915,7 @@
         <v>65</v>
       </c>
       <c r="C47" t="s">
-        <v>373</v>
+        <v>371</v>
       </c>
     </row>
     <row r="48" spans="1:3" x14ac:dyDescent="0.25">
@@ -2981,7 +2975,7 @@
         <v>114</v>
       </c>
       <c r="C57" s="1" t="s">
-        <v>331</v>
+        <v>329</v>
       </c>
     </row>
     <row r="58" spans="1:3" x14ac:dyDescent="0.25">
@@ -3185,8 +3179,11 @@
       <c r="A90" s="1" t="s">
         <v>108</v>
       </c>
-      <c r="B90" t="s">
-        <v>282</v>
+      <c r="B90" s="45" t="s">
+        <v>376</v>
+      </c>
+      <c r="C90" t="s">
+        <v>377</v>
       </c>
     </row>
     <row r="91" spans="1:3" x14ac:dyDescent="0.25">
@@ -3194,15 +3191,15 @@
         <v>109</v>
       </c>
       <c r="B91" t="s">
-        <v>376</v>
+        <v>374</v>
       </c>
     </row>
     <row r="92" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A92" s="1" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
       <c r="B92" t="s">
-        <v>376</v>
+        <v>374</v>
       </c>
     </row>
     <row r="93" spans="1:3" x14ac:dyDescent="0.25">
@@ -3210,7 +3207,7 @@
         <v>113</v>
       </c>
       <c r="B93" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
     </row>
     <row r="94" spans="1:3" x14ac:dyDescent="0.25">
@@ -3218,7 +3215,7 @@
         <v>141</v>
       </c>
       <c r="B94" t="s">
-        <v>375</v>
+        <v>373</v>
       </c>
     </row>
     <row r="95" spans="1:3" x14ac:dyDescent="0.25">
@@ -3226,7 +3223,7 @@
         <v>142</v>
       </c>
       <c r="B95" t="s">
-        <v>283</v>
+        <v>282</v>
       </c>
     </row>
     <row r="96" spans="1:3" x14ac:dyDescent="0.25">
@@ -3234,7 +3231,7 @@
         <v>144</v>
       </c>
       <c r="B96" t="s">
-        <v>374</v>
+        <v>372</v>
       </c>
     </row>
     <row r="97" spans="1:2" x14ac:dyDescent="0.25">
@@ -3242,7 +3239,7 @@
         <v>145</v>
       </c>
       <c r="B97" t="s">
-        <v>283</v>
+        <v>282</v>
       </c>
     </row>
     <row r="98" spans="1:2" x14ac:dyDescent="0.25">
@@ -3250,7 +3247,7 @@
         <v>146</v>
       </c>
       <c r="B98" t="s">
-        <v>283</v>
+        <v>282</v>
       </c>
     </row>
     <row r="99" spans="1:2" x14ac:dyDescent="0.25">
@@ -3290,17 +3287,17 @@
         <v>279</v>
       </c>
       <c r="B103" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
     </row>
     <row r="104" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A104" s="1" t="s">
-        <v>372</v>
+        <v>370</v>
       </c>
     </row>
     <row r="105" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A105" s="1" t="s">
-        <v>377</v>
+        <v>375</v>
       </c>
     </row>
     <row r="112" spans="1:2" x14ac:dyDescent="0.25">
@@ -3469,17 +3466,20 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="A112:A142 A77 A72:A75 A1:A70">
-    <cfRule type="containsBlanks" dxfId="2" priority="2">
+    <cfRule type="containsBlanks" dxfId="1" priority="2">
       <formula>LEN(TRIM(A1))=0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A1:C1048576">
+  <conditionalFormatting sqref="A1:C89 A91:C1048576 A90 C90">
     <cfRule type="cellIs" dxfId="0" priority="1" operator="equal">
       <formula>"done"</formula>
     </cfRule>
   </conditionalFormatting>
+  <hyperlinks>
+    <hyperlink ref="B90" r:id="rId1" location="2-give-them-a-name" display="https://github.com/pret/pokecrystal/wiki/Add-a-new-trainer-class - 2-give-them-a-name" xr:uid="{0696C4C8-4149-46EA-A253-8D50317E96D3}"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId1"/>
+  <pageSetup orientation="portrait" r:id="rId2"/>
 </worksheet>
 </file>
 
@@ -5076,8 +5076,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5CCA6904-CCBA-4CF4-893E-058C20254CB5}">
   <dimension ref="A1:K39"/>
   <sheetViews>
-    <sheetView topLeftCell="A5" workbookViewId="0">
-      <selection activeCell="P17" sqref="P17"/>
+    <sheetView topLeftCell="A9" workbookViewId="0">
+      <selection activeCell="G3" sqref="G3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
@@ -5088,7 +5088,7 @@
   <sheetData>
     <row r="1" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
     </row>
     <row r="3" spans="1:11" ht="13" x14ac:dyDescent="0.3">
@@ -5099,20 +5099,18 @@
         <v>12</v>
       </c>
       <c r="C3" t="s">
-        <v>293</v>
+        <v>292</v>
       </c>
       <c r="D3" t="s">
-        <v>301</v>
+        <v>300</v>
       </c>
       <c r="E3" t="s">
         <v>160</v>
       </c>
       <c r="F3" t="s">
-        <v>302</v>
-      </c>
-      <c r="G3" s="19" t="s">
-        <v>308</v>
-      </c>
+        <v>301</v>
+      </c>
+      <c r="G3" s="19"/>
       <c r="K3" t="s">
         <v>208</v>
       </c>
@@ -5122,13 +5120,13 @@
         <v>12</v>
       </c>
       <c r="C4" t="s">
-        <v>294</v>
+        <v>293</v>
       </c>
       <c r="D4" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
       <c r="E4" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
       <c r="K4" t="s">
         <v>209</v>
@@ -5139,19 +5137,19 @@
         <v>11</v>
       </c>
       <c r="C5" t="s">
+        <v>311</v>
+      </c>
+      <c r="D5" t="s">
         <v>313</v>
       </c>
-      <c r="D5" t="s">
+      <c r="E5" t="s">
+        <v>314</v>
+      </c>
+      <c r="F5" t="s">
         <v>315</v>
       </c>
-      <c r="E5" t="s">
+      <c r="G5" t="s">
         <v>316</v>
-      </c>
-      <c r="F5" t="s">
-        <v>317</v>
-      </c>
-      <c r="G5" t="s">
-        <v>318</v>
       </c>
       <c r="K5" t="s">
         <v>210</v>
@@ -5165,19 +5163,19 @@
         <v>23</v>
       </c>
       <c r="C7" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
       <c r="D7" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
       <c r="E7" t="s">
         <v>204</v>
       </c>
       <c r="F7" t="s">
+        <v>300</v>
+      </c>
+      <c r="G7" t="s">
         <v>301</v>
-      </c>
-      <c r="G7" t="s">
-        <v>302</v>
       </c>
       <c r="K7" t="s">
         <v>208</v>
@@ -5188,16 +5186,16 @@
         <v>23</v>
       </c>
       <c r="C8" t="s">
-        <v>297</v>
+        <v>296</v>
       </c>
       <c r="D8" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
       <c r="E8" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
       <c r="F8" t="s">
-        <v>305</v>
+        <v>304</v>
       </c>
       <c r="G8" t="s">
         <v>257</v>
@@ -5211,19 +5209,19 @@
         <v>25</v>
       </c>
       <c r="C9" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
       <c r="D9" t="s">
+        <v>305</v>
+      </c>
+      <c r="E9" t="s">
         <v>306</v>
       </c>
-      <c r="E9" t="s">
+      <c r="F9" t="s">
         <v>307</v>
       </c>
-      <c r="F9" t="s">
+      <c r="G9" t="s">
         <v>308</v>
-      </c>
-      <c r="G9" t="s">
-        <v>309</v>
       </c>
       <c r="K9" s="1" t="s">
         <v>234</v>
@@ -5234,16 +5232,16 @@
         <v>25</v>
       </c>
       <c r="C10" t="s">
-        <v>313</v>
+        <v>311</v>
       </c>
       <c r="D10" t="s">
-        <v>319</v>
+        <v>317</v>
       </c>
       <c r="E10" t="s">
-        <v>320</v>
+        <v>318</v>
       </c>
       <c r="F10" t="s">
-        <v>316</v>
+        <v>314</v>
       </c>
       <c r="G10" t="s">
         <v>247</v>
@@ -5254,25 +5252,25 @@
     </row>
     <row r="12" spans="1:11" ht="13" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
-        <v>298</v>
+        <v>297</v>
       </c>
       <c r="B12">
         <v>32</v>
       </c>
       <c r="C12" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
       <c r="D12" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
       <c r="E12" s="19" t="s">
-        <v>321</v>
+        <v>319</v>
       </c>
       <c r="F12" s="19" t="s">
         <v>240</v>
       </c>
       <c r="G12" t="s">
-        <v>302</v>
+        <v>301</v>
       </c>
       <c r="K12" t="s">
         <v>208</v>
@@ -5283,16 +5281,16 @@
         <v>32</v>
       </c>
       <c r="C13" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
       <c r="D13" s="19" t="s">
-        <v>341</v>
+        <v>339</v>
       </c>
       <c r="E13" s="19" t="s">
-        <v>349</v>
+        <v>347</v>
       </c>
       <c r="F13" t="s">
-        <v>305</v>
+        <v>304</v>
       </c>
       <c r="G13" t="s">
         <v>257</v>
@@ -5306,19 +5304,19 @@
         <v>32</v>
       </c>
       <c r="C14" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
       <c r="D14" s="19" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
       <c r="E14" t="s">
-        <v>312</v>
+        <v>306</v>
       </c>
       <c r="F14" s="19" t="s">
-        <v>358</v>
+        <v>356</v>
       </c>
       <c r="G14" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
       <c r="K14" s="1" t="s">
         <v>234</v>
@@ -5329,13 +5327,13 @@
         <v>32</v>
       </c>
       <c r="C15" t="s">
-        <v>314</v>
+        <v>312</v>
       </c>
       <c r="D15" t="s">
-        <v>319</v>
+        <v>317</v>
       </c>
       <c r="E15" t="s">
-        <v>320</v>
+        <v>318</v>
       </c>
       <c r="F15" t="s">
         <v>240</v>
@@ -5354,7 +5352,7 @@
     </row>
     <row r="17" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A17" s="1" t="s">
-        <v>345</v>
+        <v>343</v>
       </c>
       <c r="D17">
         <f>COUNTIF(D19:G38, "?")</f>
@@ -5363,19 +5361,19 @@
     </row>
     <row r="19" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A19" s="1" t="s">
-        <v>336</v>
+        <v>334</v>
       </c>
       <c r="B19">
         <v>45</v>
       </c>
       <c r="C19" s="1" t="s">
-        <v>333</v>
+        <v>331</v>
       </c>
       <c r="D19" s="1" t="s">
-        <v>346</v>
+        <v>344</v>
       </c>
       <c r="E19" s="1" t="s">
-        <v>347</v>
+        <v>345</v>
       </c>
       <c r="F19" s="1" t="s">
         <v>241</v>
@@ -5392,19 +5390,19 @@
         <v>45</v>
       </c>
       <c r="C20" s="1" t="s">
-        <v>334</v>
+        <v>332</v>
       </c>
       <c r="D20" s="1" t="s">
-        <v>348</v>
+        <v>346</v>
       </c>
       <c r="E20" s="1" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
       <c r="F20" s="1" t="s">
         <v>270</v>
       </c>
       <c r="G20" s="19" t="s">
-        <v>349</v>
+        <v>347</v>
       </c>
       <c r="K20" t="s">
         <v>232</v>
@@ -5415,16 +5413,16 @@
         <v>45</v>
       </c>
       <c r="C21" s="1" t="s">
-        <v>335</v>
+        <v>333</v>
       </c>
       <c r="D21" s="19" t="s">
-        <v>341</v>
+        <v>339</v>
       </c>
       <c r="E21" s="1" t="s">
-        <v>350</v>
+        <v>348</v>
       </c>
       <c r="F21" s="1" t="s">
-        <v>351</v>
+        <v>349</v>
       </c>
       <c r="G21" s="1" t="s">
         <v>258</v>
@@ -5438,19 +5436,19 @@
         <v>45</v>
       </c>
       <c r="C22" s="1" t="s">
-        <v>326</v>
+        <v>324</v>
       </c>
       <c r="D22" s="1" t="s">
         <v>239</v>
       </c>
       <c r="E22" s="1" t="s">
-        <v>352</v>
+        <v>350</v>
       </c>
       <c r="F22" s="1" t="s">
         <v>204</v>
       </c>
       <c r="G22" s="1" t="s">
-        <v>353</v>
+        <v>351</v>
       </c>
       <c r="K22" t="s">
         <v>233</v>
@@ -5461,19 +5459,19 @@
         <v>45</v>
       </c>
       <c r="C23" s="1" t="s">
-        <v>342</v>
+        <v>340</v>
       </c>
       <c r="D23" s="1" t="s">
-        <v>341</v>
+        <v>339</v>
       </c>
       <c r="E23" s="1" t="s">
-        <v>354</v>
+        <v>352</v>
       </c>
       <c r="F23" s="1" t="s">
+        <v>353</v>
+      </c>
+      <c r="G23" s="1" t="s">
         <v>355</v>
-      </c>
-      <c r="G23" s="1" t="s">
-        <v>357</v>
       </c>
       <c r="K23" t="s">
         <v>230</v>
@@ -5487,16 +5485,16 @@
     </row>
     <row r="26" spans="1:11" ht="13" x14ac:dyDescent="0.3">
       <c r="A26" s="1" t="s">
-        <v>343</v>
+        <v>341</v>
       </c>
       <c r="B26">
         <v>48</v>
       </c>
       <c r="C26" s="1" t="s">
-        <v>328</v>
+        <v>326</v>
       </c>
       <c r="D26" s="19" t="s">
-        <v>321</v>
+        <v>319</v>
       </c>
       <c r="E26" s="19" t="s">
         <v>226</v>
@@ -5516,19 +5514,19 @@
         <v>52</v>
       </c>
       <c r="C27" s="1" t="s">
-        <v>329</v>
+        <v>327</v>
       </c>
       <c r="D27" s="19" t="s">
         <v>156</v>
       </c>
       <c r="E27" s="19" t="s">
+        <v>356</v>
+      </c>
+      <c r="F27" s="1" t="s">
         <v>358</v>
       </c>
-      <c r="F27" s="1" t="s">
-        <v>360</v>
-      </c>
       <c r="G27" s="1" t="s">
-        <v>359</v>
+        <v>357</v>
       </c>
       <c r="K27" t="s">
         <v>232</v>
@@ -5539,13 +5537,13 @@
         <v>50</v>
       </c>
       <c r="C28" s="1" t="s">
-        <v>330</v>
+        <v>328</v>
       </c>
       <c r="D28" s="19" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
       <c r="E28" s="1" t="s">
-        <v>344</v>
+        <v>342</v>
       </c>
       <c r="F28" s="1" t="s">
         <v>206</v>
@@ -5562,19 +5560,19 @@
         <v>50</v>
       </c>
       <c r="C29" s="1" t="s">
+        <v>336</v>
+      </c>
+      <c r="D29" s="1" t="s">
+        <v>337</v>
+      </c>
+      <c r="E29" s="1" t="s">
         <v>338</v>
       </c>
-      <c r="D29" s="1" t="s">
-        <v>339</v>
-      </c>
-      <c r="E29" s="1" t="s">
-        <v>340</v>
-      </c>
       <c r="F29" s="1" t="s">
-        <v>361</v>
+        <v>359</v>
       </c>
       <c r="G29" s="1" t="s">
-        <v>362</v>
+        <v>360</v>
       </c>
       <c r="K29" t="s">
         <v>233</v>
@@ -5585,13 +5583,13 @@
         <v>50</v>
       </c>
       <c r="C30" s="1" t="s">
-        <v>337</v>
+        <v>335</v>
       </c>
       <c r="D30" s="1" t="s">
-        <v>363</v>
+        <v>361</v>
       </c>
       <c r="E30" s="1" t="s">
-        <v>364</v>
+        <v>362</v>
       </c>
       <c r="F30" s="1" t="s">
         <v>249</v>
@@ -5616,7 +5614,7 @@
         <v>66</v>
       </c>
       <c r="C33" t="s">
-        <v>322</v>
+        <v>320</v>
       </c>
       <c r="D33" s="1" t="s">
         <v>270</v>
@@ -5639,10 +5637,10 @@
         <v>60</v>
       </c>
       <c r="C34" t="s">
-        <v>323</v>
+        <v>321</v>
       </c>
       <c r="D34" s="1" t="s">
-        <v>365</v>
+        <v>363</v>
       </c>
       <c r="E34" s="1" t="s">
         <v>165</v>
@@ -5651,7 +5649,7 @@
         <v>160</v>
       </c>
       <c r="G34" s="1" t="s">
-        <v>366</v>
+        <v>364</v>
       </c>
       <c r="K34" t="s">
         <v>232</v>
@@ -5662,7 +5660,7 @@
         <v>60</v>
       </c>
       <c r="C35" t="s">
-        <v>324</v>
+        <v>322</v>
       </c>
       <c r="D35" s="1" t="s">
         <v>164</v>
@@ -5674,7 +5672,7 @@
         <v>160</v>
       </c>
       <c r="G35" s="1" t="s">
-        <v>366</v>
+        <v>364</v>
       </c>
       <c r="K35" t="s">
         <v>234</v>
@@ -5685,19 +5683,19 @@
         <v>62</v>
       </c>
       <c r="C36" t="s">
-        <v>325</v>
+        <v>323</v>
       </c>
       <c r="D36" s="1" t="s">
         <v>165</v>
       </c>
       <c r="E36" s="1" t="s">
-        <v>367</v>
+        <v>365</v>
       </c>
       <c r="F36" s="1" t="s">
-        <v>364</v>
+        <v>362</v>
       </c>
       <c r="G36" s="1" t="s">
-        <v>368</v>
+        <v>366</v>
       </c>
       <c r="K36" t="s">
         <v>233</v>
@@ -5708,19 +5706,19 @@
         <v>65</v>
       </c>
       <c r="C37" t="s">
-        <v>327</v>
+        <v>325</v>
       </c>
       <c r="D37" s="1" t="s">
-        <v>350</v>
+        <v>348</v>
       </c>
       <c r="E37" s="1" t="s">
         <v>240</v>
       </c>
       <c r="F37" s="1" t="s">
-        <v>371</v>
+        <v>369</v>
       </c>
       <c r="G37" s="1" t="s">
-        <v>356</v>
+        <v>354</v>
       </c>
       <c r="K37" t="s">
         <v>230</v>
@@ -5731,16 +5729,16 @@
         <v>60</v>
       </c>
       <c r="C38" s="1" t="s">
-        <v>332</v>
+        <v>330</v>
       </c>
       <c r="D38" s="1" t="s">
         <v>165</v>
       </c>
       <c r="E38" s="1" t="s">
-        <v>369</v>
+        <v>367</v>
       </c>
       <c r="F38" s="1" t="s">
-        <v>350</v>
+        <v>348</v>
       </c>
       <c r="G38" s="19" t="s">
         <v>240</v>
@@ -5751,7 +5749,7 @@
     </row>
     <row r="39" spans="1:11" x14ac:dyDescent="0.25">
       <c r="K39" s="1" t="s">
-        <v>370</v>
+        <v>368</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
scraped sprites from crystal clear, fixed gio sprite, added gio parties
</commit_message>
<xml_diff>
--- a/Silver_Todo.xlsx
+++ b/Silver_Todo.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\dwg11\Silver\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E470D5E7-6BAC-42FD-AEAE-2CF9901EC843}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A7A43857-53DF-4E5F-B88C-A3DEC9ACC7EF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="25820" windowHeight="15500" tabRatio="788" firstSheet="1" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="12330" windowHeight="15280" tabRatio="788" firstSheet="1" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Overview and Credits" sheetId="2" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="773" uniqueCount="378">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="776" uniqueCount="380">
   <si>
     <t>Pallet Town</t>
   </si>
@@ -482,18 +482,9 @@
     <t>fishing sprite</t>
   </si>
   <si>
-    <t xml:space="preserve">remove kris </t>
-  </si>
-  <si>
     <t>biking sprite</t>
   </si>
   <si>
-    <t>gfx sprites</t>
-  </si>
-  <si>
-    <t>gfx overworld</t>
-  </si>
-  <si>
     <t>Cyndaquil</t>
   </si>
   <si>
@@ -881,15 +872,9 @@
     <t>done</t>
   </si>
   <si>
-    <t>if needed? May revise f/b and OW sprite to have this option?</t>
-  </si>
-  <si>
     <t>tutorial</t>
   </si>
   <si>
-    <t>map</t>
-  </si>
-  <si>
     <t>cribxtal</t>
   </si>
   <si>
@@ -1103,9 +1088,6 @@
     <t>Swagger</t>
   </si>
   <si>
-    <t>HP Bug</t>
-  </si>
-  <si>
     <t>Faint Attack</t>
   </si>
   <si>
@@ -1130,9 +1112,6 @@
     <t>Thunder</t>
   </si>
   <si>
-    <t>Double Kick</t>
-  </si>
-  <si>
     <t>Rock Slide</t>
   </si>
   <si>
@@ -1166,10 +1145,37 @@
     <t>intro text for giovanni</t>
   </si>
   <si>
-    <t>Add a new trainer class · pret/pokecrystal Wiki (github.com)</t>
-  </si>
-  <si>
-    <t>palfix needed at gfx/trainers/giovanni.png</t>
+    <t>remove kris?</t>
+  </si>
+  <si>
+    <t>flash gio sprite at intro</t>
+  </si>
+  <si>
+    <t>scraped, in newsprites</t>
+  </si>
+  <si>
+    <t>force "male" option</t>
+  </si>
+  <si>
+    <t>"add a new map"</t>
+  </si>
+  <si>
+    <t>edit:</t>
+  </si>
+  <si>
+    <t xml:space="preserve">engine/events/haircut, data/events/happiness_changes, dden and golderodunderground  constants/pokemon_data_constants,  </t>
+  </si>
+  <si>
+    <t>Toxic</t>
+  </si>
+  <si>
+    <t>Attract</t>
+  </si>
+  <si>
+    <t>Sludge Bomb</t>
+  </si>
+  <si>
+    <t>HP Rock</t>
   </si>
 </sst>
 </file>
@@ -1398,7 +1404,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="46">
+  <cellXfs count="45">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -1504,7 +1510,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -2587,8 +2592,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4D4D23E0-802A-4842-9CD9-587C61A270C2}">
   <dimension ref="A1:E142"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A63" workbookViewId="0">
-      <selection activeCell="B91" sqref="B91"/>
+    <sheetView topLeftCell="B77" workbookViewId="0">
+      <selection activeCell="C105" sqref="C105"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
@@ -2656,7 +2661,7 @@
         <v>32</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>271</v>
+        <v>268</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.25">
@@ -2670,7 +2675,7 @@
         <v>34</v>
       </c>
       <c r="C10" t="s">
-        <v>272</v>
+        <v>269</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.25">
@@ -2687,7 +2692,7 @@
       </c>
       <c r="B12" s="1"/>
       <c r="C12" s="1" t="s">
-        <v>273</v>
+        <v>270</v>
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.25">
@@ -2726,7 +2731,7 @@
         <v>41</v>
       </c>
       <c r="C18" s="1" t="s">
-        <v>290</v>
+        <v>285</v>
       </c>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.25">
@@ -2751,7 +2756,7 @@
         <v>44</v>
       </c>
       <c r="C21" s="1" t="s">
-        <v>277</v>
+        <v>274</v>
       </c>
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.25">
@@ -2774,7 +2779,7 @@
         <v>79</v>
       </c>
       <c r="C25" t="s">
-        <v>286</v>
+        <v>281</v>
       </c>
     </row>
     <row r="26" spans="1:5" x14ac:dyDescent="0.25">
@@ -2798,7 +2803,7 @@
         <v>68</v>
       </c>
       <c r="C28" s="1" t="s">
-        <v>275</v>
+        <v>272</v>
       </c>
     </row>
     <row r="29" spans="1:5" x14ac:dyDescent="0.25">
@@ -2868,7 +2873,7 @@
         <v>60</v>
       </c>
       <c r="C40" t="s">
-        <v>288</v>
+        <v>283</v>
       </c>
     </row>
     <row r="41" spans="1:3" x14ac:dyDescent="0.25">
@@ -2876,7 +2881,7 @@
         <v>61</v>
       </c>
       <c r="C41" t="s">
-        <v>287</v>
+        <v>282</v>
       </c>
     </row>
     <row r="42" spans="1:3" x14ac:dyDescent="0.25">
@@ -2886,10 +2891,10 @@
     </row>
     <row r="43" spans="1:3" ht="50" x14ac:dyDescent="0.25">
       <c r="A43" s="7" t="s">
-        <v>276</v>
+        <v>273</v>
       </c>
       <c r="C43" s="40" t="s">
-        <v>289</v>
+        <v>284</v>
       </c>
     </row>
     <row r="44" spans="1:3" x14ac:dyDescent="0.25">
@@ -2915,7 +2920,7 @@
         <v>65</v>
       </c>
       <c r="C47" t="s">
-        <v>371</v>
+        <v>364</v>
       </c>
     </row>
     <row r="48" spans="1:3" x14ac:dyDescent="0.25">
@@ -2951,7 +2956,7 @@
         <v>80</v>
       </c>
       <c r="C53" t="s">
-        <v>274</v>
+        <v>271</v>
       </c>
     </row>
     <row r="54" spans="1:3" ht="13" x14ac:dyDescent="0.25">
@@ -2975,7 +2980,7 @@
         <v>114</v>
       </c>
       <c r="C57" s="1" t="s">
-        <v>329</v>
+        <v>324</v>
       </c>
     </row>
     <row r="58" spans="1:3" x14ac:dyDescent="0.25">
@@ -3153,10 +3158,10 @@
     </row>
     <row r="87" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A87" t="s">
-        <v>161</v>
+        <v>158</v>
       </c>
       <c r="B87" t="s">
-        <v>278</v>
+        <v>275</v>
       </c>
     </row>
     <row r="88" spans="1:3" x14ac:dyDescent="0.25">
@@ -3164,7 +3169,7 @@
         <v>143</v>
       </c>
       <c r="B88" s="1" t="s">
-        <v>280</v>
+        <v>277</v>
       </c>
     </row>
     <row r="89" spans="1:3" x14ac:dyDescent="0.25">
@@ -3172,18 +3177,15 @@
         <v>107</v>
       </c>
       <c r="B89" t="s">
-        <v>280</v>
+        <v>277</v>
       </c>
     </row>
     <row r="90" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A90" s="1" t="s">
         <v>108</v>
       </c>
-      <c r="B90" s="45" t="s">
-        <v>376</v>
-      </c>
-      <c r="C90" t="s">
-        <v>377</v>
+      <c r="B90" t="s">
+        <v>277</v>
       </c>
     </row>
     <row r="91" spans="1:3" x14ac:dyDescent="0.25">
@@ -3191,15 +3193,15 @@
         <v>109</v>
       </c>
       <c r="B91" t="s">
-        <v>374</v>
+        <v>371</v>
       </c>
     </row>
     <row r="92" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A92" s="1" t="s">
-        <v>285</v>
+        <v>280</v>
       </c>
       <c r="B92" t="s">
-        <v>374</v>
+        <v>367</v>
       </c>
     </row>
     <row r="93" spans="1:3" x14ac:dyDescent="0.25">
@@ -3207,7 +3209,7 @@
         <v>113</v>
       </c>
       <c r="B93" t="s">
-        <v>284</v>
+        <v>279</v>
       </c>
     </row>
     <row r="94" spans="1:3" x14ac:dyDescent="0.25">
@@ -3215,7 +3217,7 @@
         <v>141</v>
       </c>
       <c r="B94" t="s">
-        <v>373</v>
+        <v>366</v>
       </c>
     </row>
     <row r="95" spans="1:3" x14ac:dyDescent="0.25">
@@ -3223,7 +3225,7 @@
         <v>142</v>
       </c>
       <c r="B95" t="s">
-        <v>282</v>
+        <v>278</v>
       </c>
     </row>
     <row r="96" spans="1:3" x14ac:dyDescent="0.25">
@@ -3231,76 +3233,90 @@
         <v>144</v>
       </c>
       <c r="B96" t="s">
-        <v>372</v>
-      </c>
-    </row>
-    <row r="97" spans="1:2" x14ac:dyDescent="0.25">
+        <v>365</v>
+      </c>
+    </row>
+    <row r="97" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A97" s="1" t="s">
         <v>145</v>
       </c>
       <c r="B97" t="s">
-        <v>282</v>
-      </c>
-    </row>
-    <row r="98" spans="1:2" x14ac:dyDescent="0.25">
+        <v>278</v>
+      </c>
+    </row>
+    <row r="98" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A98" s="1" t="s">
         <v>146</v>
       </c>
       <c r="B98" t="s">
-        <v>282</v>
-      </c>
-    </row>
-    <row r="99" spans="1:2" x14ac:dyDescent="0.25">
+        <v>278</v>
+      </c>
+    </row>
+    <row r="99" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A99" s="1" t="s">
         <v>147</v>
       </c>
       <c r="B99" t="s">
+        <v>371</v>
+      </c>
+    </row>
+    <row r="100" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A100" s="1" t="s">
+        <v>369</v>
+      </c>
+      <c r="B100" t="s">
+        <v>372</v>
+      </c>
+    </row>
+    <row r="101" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A101" s="1" t="s">
+        <v>148</v>
+      </c>
+      <c r="B101" t="s">
+        <v>371</v>
+      </c>
+    </row>
+    <row r="102" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A102" s="1" t="s">
         <v>151</v>
       </c>
-    </row>
-    <row r="100" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A100" s="1" t="s">
-        <v>148</v>
-      </c>
-      <c r="B100" t="s">
-        <v>281</v>
-      </c>
-    </row>
-    <row r="101" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A101" s="1" t="s">
-        <v>149</v>
-      </c>
-      <c r="B101" t="s">
-        <v>150</v>
-      </c>
-    </row>
-    <row r="102" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A102" s="1" t="s">
-        <v>154</v>
-      </c>
       <c r="B102" t="s">
-        <v>280</v>
-      </c>
-    </row>
-    <row r="103" spans="1:2" x14ac:dyDescent="0.25">
+        <v>277</v>
+      </c>
+    </row>
+    <row r="103" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A103" s="1" t="s">
-        <v>279</v>
+        <v>276</v>
       </c>
       <c r="B103" t="s">
-        <v>283</v>
-      </c>
-    </row>
-    <row r="104" spans="1:2" x14ac:dyDescent="0.25">
+        <v>373</v>
+      </c>
+    </row>
+    <row r="104" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A104" s="1" t="s">
+        <v>363</v>
+      </c>
+      <c r="B104" t="s">
+        <v>374</v>
+      </c>
+      <c r="C104" t="s">
+        <v>375</v>
+      </c>
+    </row>
+    <row r="105" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A105" s="1" t="s">
+        <v>368</v>
+      </c>
+    </row>
+    <row r="106" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A106" s="1" t="s">
         <v>370</v>
       </c>
-    </row>
-    <row r="105" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A105" s="1" t="s">
-        <v>375</v>
-      </c>
-    </row>
-    <row r="112" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B106" t="s">
+        <v>277</v>
+      </c>
+    </row>
+    <row r="112" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A112" s="7" t="s">
         <v>18</v>
       </c>
@@ -3470,16 +3486,13 @@
       <formula>LEN(TRIM(A1))=0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A1:C89 A91:C1048576 A90 C90">
+  <conditionalFormatting sqref="A1:C1048576">
     <cfRule type="cellIs" dxfId="0" priority="1" operator="equal">
       <formula>"done"</formula>
     </cfRule>
   </conditionalFormatting>
-  <hyperlinks>
-    <hyperlink ref="B90" r:id="rId1" location="2-give-them-a-name" display="https://github.com/pret/pokecrystal/wiki/Add-a-new-trainer-class - 2-give-them-a-name" xr:uid="{0696C4C8-4149-46EA-A253-8D50317E96D3}"/>
-  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId2"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -3518,7 +3531,7 @@
     </row>
     <row r="2" spans="1:20" x14ac:dyDescent="0.25">
       <c r="C2" s="42" t="s">
-        <v>167</v>
+        <v>164</v>
       </c>
       <c r="D2" s="43"/>
       <c r="E2" s="43"/>
@@ -3526,7 +3539,7 @@
       <c r="G2" s="43"/>
       <c r="H2" s="44"/>
       <c r="I2" s="42" t="s">
-        <v>168</v>
+        <v>165</v>
       </c>
       <c r="J2" s="43"/>
       <c r="K2" s="43"/>
@@ -3534,7 +3547,7 @@
       <c r="M2" s="43"/>
       <c r="N2" s="44"/>
       <c r="O2" s="42" t="s">
-        <v>169</v>
+        <v>166</v>
       </c>
       <c r="P2" s="43"/>
       <c r="Q2" s="43"/>
@@ -3544,10 +3557,10 @@
     </row>
     <row r="3" spans="1:20" ht="13" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>208</v>
+        <v>205</v>
       </c>
       <c r="B3" s="19" t="s">
-        <v>171</v>
+        <v>168</v>
       </c>
       <c r="C3">
         <v>5</v>
@@ -3556,34 +3569,34 @@
         <v>74</v>
       </c>
       <c r="E3" t="s">
-        <v>170</v>
+        <v>167</v>
       </c>
       <c r="F3" t="s">
-        <v>160</v>
+        <v>157</v>
       </c>
       <c r="I3">
         <v>5</v>
       </c>
       <c r="J3" t="s">
-        <v>153</v>
+        <v>150</v>
       </c>
       <c r="K3" t="s">
-        <v>207</v>
+        <v>204</v>
       </c>
       <c r="L3" t="s">
-        <v>244</v>
+        <v>241</v>
       </c>
       <c r="O3" t="s">
         <v>92</v>
       </c>
       <c r="P3" t="s">
-        <v>152</v>
+        <v>149</v>
       </c>
       <c r="Q3" t="s">
-        <v>207</v>
+        <v>204</v>
       </c>
       <c r="R3" t="s">
-        <v>160</v>
+        <v>157</v>
       </c>
     </row>
     <row r="4" spans="1:20" x14ac:dyDescent="0.25">
@@ -3609,10 +3622,10 @@
     </row>
     <row r="5" spans="1:20" ht="13" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>208</v>
+        <v>205</v>
       </c>
       <c r="B5" s="19" t="s">
-        <v>245</v>
+        <v>242</v>
       </c>
       <c r="C5">
         <v>16</v>
@@ -3621,164 +3634,164 @@
         <v>74</v>
       </c>
       <c r="E5" t="s">
-        <v>206</v>
+        <v>203</v>
       </c>
       <c r="F5" t="s">
-        <v>205</v>
+        <v>202</v>
       </c>
       <c r="G5" s="1" t="s">
-        <v>160</v>
+        <v>157</v>
       </c>
       <c r="H5" s="39" t="s">
-        <v>170</v>
+        <v>167</v>
       </c>
       <c r="I5">
         <v>16</v>
       </c>
       <c r="J5" t="s">
-        <v>176</v>
+        <v>173</v>
       </c>
       <c r="K5" t="s">
-        <v>215</v>
+        <v>212</v>
       </c>
       <c r="L5" t="s">
-        <v>213</v>
+        <v>210</v>
       </c>
       <c r="M5" t="s">
-        <v>214</v>
+        <v>211</v>
       </c>
       <c r="N5" s="39" t="s">
-        <v>207</v>
+        <v>204</v>
       </c>
       <c r="O5">
         <v>14</v>
       </c>
       <c r="P5" t="s">
-        <v>175</v>
+        <v>172</v>
       </c>
       <c r="Q5" t="s">
-        <v>216</v>
+        <v>213</v>
       </c>
       <c r="R5" t="s">
-        <v>217</v>
+        <v>214</v>
       </c>
       <c r="S5" t="s">
-        <v>207</v>
+        <v>204</v>
       </c>
       <c r="T5" s="37" t="s">
-        <v>160</v>
+        <v>157</v>
       </c>
     </row>
     <row r="6" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>209</v>
+        <v>206</v>
       </c>
       <c r="B6" t="s">
-        <v>256</v>
+        <v>253</v>
       </c>
       <c r="C6">
         <v>12</v>
       </c>
       <c r="D6" t="s">
-        <v>173</v>
+        <v>170</v>
       </c>
       <c r="E6" t="s">
-        <v>200</v>
+        <v>197</v>
       </c>
       <c r="F6" t="s">
-        <v>244</v>
+        <v>241</v>
       </c>
       <c r="G6" t="s">
-        <v>201</v>
+        <v>198</v>
       </c>
       <c r="I6">
         <v>12</v>
       </c>
       <c r="J6" t="s">
-        <v>173</v>
+        <v>170</v>
       </c>
       <c r="K6" t="s">
+        <v>197</v>
+      </c>
+      <c r="L6" t="s">
         <v>200</v>
       </c>
-      <c r="L6" t="s">
-        <v>203</v>
-      </c>
       <c r="M6" t="s">
-        <v>201</v>
+        <v>198</v>
       </c>
       <c r="N6" s="37" t="s">
-        <v>244</v>
+        <v>241</v>
       </c>
       <c r="O6">
         <v>12</v>
       </c>
       <c r="P6" t="s">
-        <v>173</v>
+        <v>170</v>
       </c>
       <c r="Q6" t="s">
+        <v>197</v>
+      </c>
+      <c r="R6" t="s">
         <v>200</v>
       </c>
-      <c r="R6" t="s">
-        <v>203</v>
-      </c>
       <c r="S6" t="s">
-        <v>201</v>
+        <v>198</v>
       </c>
       <c r="T6" s="37" t="s">
-        <v>244</v>
+        <v>241</v>
       </c>
     </row>
     <row r="7" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>210</v>
+        <v>207</v>
       </c>
       <c r="C7">
         <v>16</v>
       </c>
       <c r="D7" t="s">
-        <v>174</v>
+        <v>171</v>
       </c>
       <c r="E7" t="s">
-        <v>204</v>
+        <v>201</v>
       </c>
       <c r="F7" t="s">
-        <v>229</v>
+        <v>226</v>
       </c>
       <c r="G7" t="s">
-        <v>216</v>
+        <v>213</v>
       </c>
       <c r="I7">
         <v>16</v>
       </c>
       <c r="J7" t="s">
-        <v>177</v>
+        <v>174</v>
       </c>
       <c r="K7" t="s">
-        <v>205</v>
+        <v>202</v>
       </c>
       <c r="L7" t="s">
-        <v>218</v>
+        <v>215</v>
       </c>
       <c r="M7" t="s">
-        <v>219</v>
+        <v>216</v>
       </c>
       <c r="O7">
         <v>18</v>
       </c>
       <c r="P7" t="s">
-        <v>178</v>
+        <v>175</v>
       </c>
       <c r="Q7" s="1" t="s">
-        <v>257</v>
+        <v>254</v>
       </c>
       <c r="R7" s="1" t="s">
-        <v>258</v>
+        <v>255</v>
       </c>
       <c r="S7" s="1" t="s">
-        <v>215</v>
+        <v>212</v>
       </c>
       <c r="T7" s="39" t="s">
-        <v>207</v>
+        <v>204</v>
       </c>
     </row>
     <row r="8" spans="1:20" s="36" customFormat="1" x14ac:dyDescent="0.25">
@@ -3788,243 +3801,243 @@
     </row>
     <row r="9" spans="1:20" ht="13" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
-        <v>208</v>
+        <v>205</v>
       </c>
       <c r="B9" s="19" t="s">
-        <v>179</v>
+        <v>176</v>
       </c>
       <c r="C9">
         <v>22</v>
       </c>
       <c r="D9" t="s">
-        <v>172</v>
+        <v>169</v>
       </c>
       <c r="E9" s="1" t="s">
-        <v>158</v>
+        <v>155</v>
       </c>
       <c r="F9" s="1" t="s">
-        <v>204</v>
+        <v>201</v>
       </c>
       <c r="G9" s="1" t="s">
-        <v>160</v>
+        <v>157</v>
       </c>
       <c r="H9" s="39" t="s">
-        <v>222</v>
+        <v>219</v>
       </c>
       <c r="I9">
         <v>22</v>
       </c>
       <c r="J9" t="s">
-        <v>176</v>
+        <v>173</v>
       </c>
       <c r="K9" s="1" t="s">
-        <v>215</v>
+        <v>212</v>
       </c>
       <c r="L9" s="1" t="s">
-        <v>213</v>
+        <v>210</v>
       </c>
       <c r="M9" s="1" t="s">
-        <v>198</v>
+        <v>195</v>
       </c>
       <c r="N9" s="39" t="s">
-        <v>222</v>
+        <v>219</v>
       </c>
       <c r="O9">
         <v>22</v>
       </c>
       <c r="P9" t="s">
-        <v>175</v>
+        <v>172</v>
       </c>
       <c r="Q9" s="1" t="s">
-        <v>216</v>
+        <v>213</v>
       </c>
       <c r="R9" s="1" t="s">
-        <v>217</v>
+        <v>214</v>
       </c>
       <c r="S9" s="1" t="s">
-        <v>198</v>
+        <v>195</v>
       </c>
       <c r="T9" s="39" t="s">
-        <v>222</v>
+        <v>219</v>
       </c>
     </row>
     <row r="10" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>211</v>
+        <v>208</v>
       </c>
       <c r="B10" s="1"/>
       <c r="C10">
         <v>20</v>
       </c>
       <c r="D10" t="s">
-        <v>181</v>
+        <v>178</v>
       </c>
       <c r="E10" t="s">
-        <v>202</v>
+        <v>199</v>
       </c>
       <c r="F10" t="s">
-        <v>220</v>
+        <v>217</v>
       </c>
       <c r="G10" t="s">
-        <v>200</v>
+        <v>197</v>
       </c>
       <c r="H10" s="37" t="s">
-        <v>180</v>
+        <v>177</v>
       </c>
       <c r="I10">
         <v>20</v>
       </c>
       <c r="J10" t="s">
-        <v>181</v>
+        <v>178</v>
       </c>
       <c r="K10" t="s">
-        <v>202</v>
+        <v>199</v>
       </c>
       <c r="L10" t="s">
-        <v>220</v>
+        <v>217</v>
       </c>
       <c r="M10" t="s">
-        <v>200</v>
+        <v>197</v>
       </c>
       <c r="N10" s="37" t="s">
-        <v>180</v>
+        <v>177</v>
       </c>
       <c r="O10">
         <v>20</v>
       </c>
       <c r="P10" t="s">
-        <v>181</v>
+        <v>178</v>
       </c>
       <c r="Q10" t="s">
-        <v>202</v>
+        <v>199</v>
       </c>
       <c r="R10" t="s">
-        <v>220</v>
+        <v>217</v>
       </c>
       <c r="S10" t="s">
-        <v>200</v>
+        <v>197</v>
       </c>
       <c r="T10" s="37" t="s">
-        <v>180</v>
+        <v>177</v>
       </c>
     </row>
     <row r="11" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>210</v>
+        <v>207</v>
       </c>
       <c r="C11">
         <v>20</v>
       </c>
       <c r="D11" t="s">
-        <v>174</v>
+        <v>171</v>
       </c>
       <c r="E11" t="s">
-        <v>204</v>
+        <v>201</v>
       </c>
       <c r="F11" t="s">
-        <v>229</v>
+        <v>226</v>
       </c>
       <c r="G11" t="s">
-        <v>216</v>
+        <v>213</v>
       </c>
       <c r="H11" s="37" t="s">
-        <v>160</v>
+        <v>157</v>
       </c>
       <c r="I11">
         <v>20</v>
       </c>
       <c r="J11" t="s">
-        <v>183</v>
+        <v>180</v>
       </c>
       <c r="K11" s="1" t="s">
-        <v>205</v>
+        <v>202</v>
       </c>
       <c r="L11" s="1" t="s">
-        <v>218</v>
+        <v>215</v>
       </c>
       <c r="M11" s="1" t="s">
-        <v>246</v>
+        <v>243</v>
       </c>
       <c r="N11" s="39" t="s">
-        <v>247</v>
+        <v>244</v>
       </c>
       <c r="O11">
         <v>20</v>
       </c>
       <c r="P11" t="s">
-        <v>178</v>
+        <v>175</v>
       </c>
       <c r="Q11" s="1" t="s">
-        <v>257</v>
+        <v>254</v>
       </c>
       <c r="R11" s="1" t="s">
-        <v>258</v>
+        <v>255</v>
       </c>
       <c r="S11" s="1" t="s">
-        <v>215</v>
+        <v>212</v>
       </c>
       <c r="T11" s="39" t="s">
-        <v>207</v>
+        <v>204</v>
       </c>
     </row>
     <row r="12" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>212</v>
+        <v>209</v>
       </c>
       <c r="B12" s="1"/>
       <c r="C12">
         <v>18</v>
       </c>
       <c r="D12" t="s">
-        <v>182</v>
+        <v>179</v>
       </c>
       <c r="E12" t="s">
-        <v>237</v>
+        <v>234</v>
       </c>
       <c r="F12" t="s">
-        <v>160</v>
+        <v>157</v>
       </c>
       <c r="G12" t="s">
-        <v>238</v>
+        <v>235</v>
       </c>
       <c r="H12" s="37" t="s">
-        <v>239</v>
+        <v>236</v>
       </c>
       <c r="I12">
         <v>18</v>
       </c>
       <c r="J12" t="s">
-        <v>184</v>
+        <v>181</v>
       </c>
       <c r="K12" s="1" t="s">
-        <v>216</v>
+        <v>213</v>
       </c>
       <c r="L12" s="1" t="s">
-        <v>239</v>
+        <v>236</v>
       </c>
       <c r="M12" s="1" t="s">
-        <v>250</v>
+        <v>247</v>
       </c>
       <c r="N12" s="39" t="s">
-        <v>160</v>
+        <v>157</v>
       </c>
       <c r="O12">
         <v>18</v>
       </c>
       <c r="P12" t="s">
-        <v>185</v>
+        <v>182</v>
       </c>
       <c r="Q12" s="1" t="s">
+        <v>261</v>
+      </c>
+      <c r="R12" s="1" t="s">
+        <v>262</v>
+      </c>
+      <c r="S12" s="1" t="s">
+        <v>263</v>
+      </c>
+      <c r="T12" s="39" t="s">
         <v>264</v>
-      </c>
-      <c r="R12" s="1" t="s">
-        <v>265</v>
-      </c>
-      <c r="S12" s="1" t="s">
-        <v>266</v>
-      </c>
-      <c r="T12" s="39" t="s">
-        <v>267</v>
       </c>
     </row>
     <row r="13" spans="1:20" s="36" customFormat="1" x14ac:dyDescent="0.25">
@@ -4034,300 +4047,300 @@
     </row>
     <row r="14" spans="1:20" ht="13" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
-        <v>208</v>
+        <v>205</v>
       </c>
       <c r="B14" s="19" t="s">
-        <v>186</v>
+        <v>183</v>
       </c>
       <c r="C14">
         <v>32</v>
       </c>
       <c r="D14" t="s">
-        <v>195</v>
+        <v>192</v>
       </c>
       <c r="E14" t="s">
-        <v>180</v>
+        <v>177</v>
       </c>
       <c r="F14" s="1" t="s">
-        <v>158</v>
+        <v>155</v>
       </c>
       <c r="G14" s="1" t="s">
-        <v>204</v>
+        <v>201</v>
       </c>
       <c r="H14" s="39" t="s">
-        <v>222</v>
+        <v>219</v>
       </c>
       <c r="I14">
         <v>32</v>
       </c>
       <c r="J14" t="s">
-        <v>196</v>
+        <v>193</v>
       </c>
       <c r="K14" t="s">
-        <v>180</v>
+        <v>177</v>
       </c>
       <c r="L14" s="1" t="s">
-        <v>213</v>
+        <v>210</v>
       </c>
       <c r="M14" s="1" t="s">
-        <v>223</v>
+        <v>220</v>
       </c>
       <c r="N14" s="39" t="s">
-        <v>222</v>
+        <v>219</v>
       </c>
       <c r="O14">
         <v>36</v>
       </c>
       <c r="P14" t="s">
-        <v>197</v>
+        <v>194</v>
       </c>
       <c r="Q14" t="s">
-        <v>180</v>
+        <v>177</v>
       </c>
       <c r="R14" s="1" t="s">
-        <v>227</v>
+        <v>224</v>
       </c>
       <c r="S14" s="1" t="s">
-        <v>228</v>
+        <v>225</v>
       </c>
       <c r="T14" s="39" t="s">
-        <v>222</v>
+        <v>219</v>
       </c>
     </row>
     <row r="15" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>211</v>
+        <v>208</v>
       </c>
       <c r="C15">
         <v>32</v>
       </c>
       <c r="D15" t="s">
-        <v>181</v>
+        <v>178</v>
       </c>
       <c r="E15" t="s">
-        <v>180</v>
+        <v>177</v>
       </c>
       <c r="F15" t="s">
-        <v>220</v>
+        <v>217</v>
       </c>
       <c r="G15" t="s">
-        <v>200</v>
+        <v>197</v>
       </c>
       <c r="H15" s="39" t="s">
-        <v>221</v>
+        <v>218</v>
       </c>
       <c r="I15">
         <v>32</v>
       </c>
       <c r="J15" t="s">
-        <v>181</v>
+        <v>178</v>
       </c>
       <c r="K15" t="s">
-        <v>180</v>
+        <v>177</v>
       </c>
       <c r="L15" t="s">
-        <v>220</v>
+        <v>217</v>
       </c>
       <c r="M15" t="s">
-        <v>200</v>
+        <v>197</v>
       </c>
       <c r="N15" s="39" t="s">
-        <v>221</v>
+        <v>218</v>
       </c>
       <c r="O15">
         <v>28</v>
       </c>
       <c r="P15" t="s">
-        <v>181</v>
+        <v>178</v>
       </c>
       <c r="Q15" t="s">
-        <v>180</v>
+        <v>177</v>
       </c>
       <c r="R15" t="s">
-        <v>220</v>
+        <v>217</v>
       </c>
       <c r="S15" t="s">
-        <v>200</v>
+        <v>197</v>
       </c>
       <c r="T15" s="39" t="s">
-        <v>221</v>
+        <v>218</v>
       </c>
     </row>
     <row r="16" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>210</v>
+        <v>207</v>
       </c>
       <c r="C16">
         <v>32</v>
       </c>
       <c r="D16" t="s">
-        <v>193</v>
+        <v>190</v>
       </c>
       <c r="E16" t="s">
-        <v>204</v>
+        <v>201</v>
       </c>
       <c r="F16" t="s">
-        <v>198</v>
+        <v>195</v>
       </c>
       <c r="G16" t="s">
-        <v>216</v>
+        <v>213</v>
       </c>
       <c r="H16" s="37" t="s">
-        <v>160</v>
+        <v>157</v>
       </c>
       <c r="I16">
         <v>32</v>
       </c>
       <c r="J16" t="s">
-        <v>183</v>
+        <v>180</v>
       </c>
       <c r="K16" s="1" t="s">
-        <v>248</v>
+        <v>245</v>
       </c>
       <c r="L16" s="1" t="s">
-        <v>218</v>
+        <v>215</v>
       </c>
       <c r="M16" s="1" t="s">
-        <v>246</v>
+        <v>243</v>
       </c>
       <c r="N16" s="39" t="s">
-        <v>228</v>
+        <v>225</v>
       </c>
       <c r="O16">
         <v>32</v>
       </c>
       <c r="P16" t="s">
-        <v>192</v>
+        <v>189</v>
       </c>
       <c r="Q16" s="1" t="s">
-        <v>259</v>
+        <v>256</v>
       </c>
       <c r="R16" s="1" t="s">
-        <v>260</v>
+        <v>257</v>
       </c>
       <c r="S16" s="1" t="s">
-        <v>215</v>
+        <v>212</v>
       </c>
       <c r="T16" s="39" t="s">
-        <v>261</v>
+        <v>258</v>
       </c>
     </row>
     <row r="17" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>212</v>
+        <v>209</v>
       </c>
       <c r="C17">
         <v>30</v>
       </c>
       <c r="D17" t="s">
-        <v>187</v>
+        <v>184</v>
       </c>
       <c r="E17" t="s">
-        <v>237</v>
+        <v>234</v>
       </c>
       <c r="F17" t="s">
-        <v>160</v>
+        <v>157</v>
       </c>
       <c r="G17" t="s">
-        <v>238</v>
+        <v>235</v>
       </c>
       <c r="H17" s="37" t="s">
-        <v>239</v>
+        <v>236</v>
       </c>
       <c r="I17">
         <v>30</v>
       </c>
       <c r="J17" t="s">
-        <v>188</v>
+        <v>185</v>
       </c>
       <c r="K17" s="1" t="s">
-        <v>249</v>
+        <v>246</v>
       </c>
       <c r="L17" s="1" t="s">
-        <v>239</v>
+        <v>236</v>
       </c>
       <c r="M17" s="1" t="s">
-        <v>250</v>
+        <v>247</v>
       </c>
       <c r="N17" s="39" t="s">
-        <v>217</v>
+        <v>214</v>
       </c>
       <c r="O17">
         <v>30</v>
       </c>
       <c r="P17" t="s">
-        <v>189</v>
+        <v>186</v>
       </c>
       <c r="Q17" s="1" t="s">
-        <v>253</v>
+        <v>250</v>
       </c>
       <c r="R17" s="1" t="s">
-        <v>239</v>
+        <v>236</v>
       </c>
       <c r="S17" s="1" t="s">
-        <v>266</v>
+        <v>263</v>
       </c>
       <c r="T17" s="39" t="s">
-        <v>268</v>
+        <v>265</v>
       </c>
     </row>
     <row r="18" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>230</v>
+        <v>227</v>
       </c>
       <c r="C18">
         <v>30</v>
       </c>
       <c r="D18" t="s">
-        <v>157</v>
+        <v>154</v>
       </c>
       <c r="E18" t="s">
-        <v>158</v>
+        <v>155</v>
       </c>
       <c r="F18" t="s">
-        <v>190</v>
+        <v>187</v>
       </c>
       <c r="G18" t="s">
-        <v>159</v>
+        <v>156</v>
       </c>
       <c r="H18" s="37" t="s">
-        <v>241</v>
+        <v>238</v>
       </c>
       <c r="I18">
         <v>30</v>
       </c>
       <c r="J18" t="s">
-        <v>157</v>
+        <v>154</v>
       </c>
       <c r="K18" t="s">
-        <v>158</v>
+        <v>155</v>
       </c>
       <c r="L18" t="s">
-        <v>190</v>
+        <v>187</v>
       </c>
       <c r="M18" t="s">
-        <v>159</v>
+        <v>156</v>
       </c>
       <c r="N18" s="37" t="s">
-        <v>241</v>
+        <v>238</v>
       </c>
       <c r="O18">
         <v>30</v>
       </c>
       <c r="P18" t="s">
-        <v>157</v>
+        <v>154</v>
       </c>
       <c r="Q18" t="s">
-        <v>158</v>
+        <v>155</v>
       </c>
       <c r="R18" t="s">
-        <v>190</v>
+        <v>187</v>
       </c>
       <c r="S18" t="s">
-        <v>159</v>
+        <v>156</v>
       </c>
       <c r="T18" s="37" t="s">
-        <v>241</v>
+        <v>238</v>
       </c>
     </row>
     <row r="19" spans="1:20" s="36" customFormat="1" x14ac:dyDescent="0.25">
@@ -4337,7 +4350,7 @@
     </row>
     <row r="20" spans="1:20" ht="12.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
-        <v>208</v>
+        <v>205</v>
       </c>
       <c r="B20" s="19" t="s">
         <v>28</v>
@@ -4346,350 +4359,350 @@
         <v>38</v>
       </c>
       <c r="D20" t="s">
-        <v>195</v>
+        <v>192</v>
       </c>
       <c r="E20" s="1" t="s">
-        <v>180</v>
+        <v>177</v>
       </c>
       <c r="F20" s="1" t="s">
-        <v>158</v>
+        <v>155</v>
       </c>
       <c r="G20" s="1" t="s">
-        <v>204</v>
+        <v>201</v>
       </c>
       <c r="H20" s="39" t="s">
-        <v>228</v>
+        <v>225</v>
       </c>
       <c r="I20">
         <v>38</v>
       </c>
       <c r="J20" t="s">
-        <v>196</v>
+        <v>193</v>
       </c>
       <c r="K20" s="1" t="s">
-        <v>180</v>
+        <v>177</v>
       </c>
       <c r="L20" s="1" t="s">
-        <v>223</v>
+        <v>220</v>
       </c>
       <c r="M20" s="1" t="s">
-        <v>213</v>
+        <v>210</v>
       </c>
       <c r="N20" s="39" t="s">
-        <v>224</v>
+        <v>221</v>
       </c>
       <c r="O20">
         <v>38</v>
       </c>
       <c r="P20" t="s">
-        <v>197</v>
+        <v>194</v>
       </c>
       <c r="Q20" s="1" t="s">
-        <v>180</v>
+        <v>177</v>
       </c>
       <c r="R20" s="1" t="s">
-        <v>227</v>
+        <v>224</v>
       </c>
       <c r="S20" s="1" t="s">
-        <v>228</v>
+        <v>225</v>
       </c>
       <c r="T20" s="39" t="s">
-        <v>224</v>
+        <v>221</v>
       </c>
     </row>
     <row r="21" spans="1:20" ht="12.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>211</v>
+        <v>208</v>
       </c>
       <c r="C21">
         <v>36</v>
       </c>
       <c r="D21" t="s">
-        <v>181</v>
+        <v>178</v>
       </c>
       <c r="E21" t="s">
-        <v>180</v>
+        <v>177</v>
       </c>
       <c r="F21" t="s">
-        <v>220</v>
+        <v>217</v>
       </c>
       <c r="G21" t="s">
-        <v>200</v>
+        <v>197</v>
       </c>
       <c r="H21" s="39" t="s">
-        <v>221</v>
+        <v>218</v>
       </c>
       <c r="I21">
         <v>36</v>
       </c>
       <c r="J21" t="s">
-        <v>181</v>
+        <v>178</v>
       </c>
       <c r="K21" t="s">
-        <v>180</v>
+        <v>177</v>
       </c>
       <c r="L21" t="s">
-        <v>220</v>
+        <v>217</v>
       </c>
       <c r="M21" t="s">
-        <v>200</v>
+        <v>197</v>
       </c>
       <c r="N21" s="39" t="s">
-        <v>221</v>
+        <v>218</v>
       </c>
       <c r="O21">
         <v>36</v>
       </c>
       <c r="P21" t="s">
-        <v>181</v>
+        <v>178</v>
       </c>
       <c r="Q21" t="s">
-        <v>180</v>
+        <v>177</v>
       </c>
       <c r="R21" t="s">
-        <v>220</v>
+        <v>217</v>
       </c>
       <c r="S21" t="s">
-        <v>200</v>
+        <v>197</v>
       </c>
       <c r="T21" s="39" t="s">
-        <v>221</v>
+        <v>218</v>
       </c>
     </row>
     <row r="22" spans="1:20" ht="12.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>234</v>
+        <v>231</v>
       </c>
       <c r="C22">
         <v>35</v>
       </c>
       <c r="D22" t="s">
-        <v>193</v>
+        <v>190</v>
       </c>
       <c r="E22" t="s">
-        <v>204</v>
+        <v>201</v>
       </c>
       <c r="F22" t="s">
-        <v>198</v>
+        <v>195</v>
       </c>
       <c r="G22" t="s">
-        <v>216</v>
+        <v>213</v>
       </c>
       <c r="H22" s="37" t="s">
-        <v>236</v>
+        <v>233</v>
       </c>
       <c r="I22">
         <v>35</v>
       </c>
       <c r="J22" t="s">
-        <v>183</v>
+        <v>180</v>
       </c>
       <c r="K22" s="1" t="s">
-        <v>248</v>
+        <v>245</v>
       </c>
       <c r="L22" s="1" t="s">
-        <v>165</v>
+        <v>162</v>
       </c>
       <c r="M22" s="1" t="s">
-        <v>218</v>
+        <v>215</v>
       </c>
       <c r="N22" s="39" t="s">
-        <v>219</v>
+        <v>216</v>
       </c>
       <c r="O22">
         <v>35</v>
       </c>
       <c r="P22" t="s">
-        <v>192</v>
+        <v>189</v>
       </c>
       <c r="Q22" s="1" t="s">
-        <v>259</v>
+        <v>256</v>
       </c>
       <c r="R22" s="1" t="s">
-        <v>260</v>
+        <v>257</v>
       </c>
       <c r="S22" s="1" t="s">
-        <v>215</v>
+        <v>212</v>
       </c>
       <c r="T22" s="39" t="s">
-        <v>261</v>
+        <v>258</v>
       </c>
     </row>
     <row r="23" spans="1:20" ht="12.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>233</v>
+        <v>230</v>
       </c>
       <c r="C23">
         <v>36</v>
       </c>
       <c r="D23" t="s">
-        <v>187</v>
+        <v>184</v>
       </c>
       <c r="E23" t="s">
+        <v>234</v>
+      </c>
+      <c r="F23" t="s">
         <v>237</v>
       </c>
-      <c r="F23" t="s">
-        <v>240</v>
-      </c>
       <c r="G23" t="s">
-        <v>238</v>
+        <v>235</v>
       </c>
       <c r="H23" s="37" t="s">
-        <v>239</v>
+        <v>236</v>
       </c>
       <c r="I23">
         <v>35</v>
       </c>
       <c r="J23" t="s">
-        <v>188</v>
+        <v>185</v>
       </c>
       <c r="K23" s="1" t="s">
-        <v>249</v>
+        <v>246</v>
       </c>
       <c r="L23" s="1" t="s">
-        <v>239</v>
+        <v>236</v>
       </c>
       <c r="M23" s="1" t="s">
-        <v>251</v>
+        <v>248</v>
       </c>
       <c r="N23" s="39" t="s">
-        <v>217</v>
+        <v>214</v>
       </c>
       <c r="O23">
         <v>35</v>
       </c>
       <c r="P23" t="s">
-        <v>189</v>
+        <v>186</v>
       </c>
       <c r="Q23" s="1" t="s">
-        <v>253</v>
+        <v>250</v>
       </c>
       <c r="R23" s="1" t="s">
-        <v>239</v>
+        <v>236</v>
       </c>
       <c r="S23" s="1" t="s">
-        <v>266</v>
+        <v>263</v>
       </c>
       <c r="T23" s="39" t="s">
-        <v>268</v>
+        <v>265</v>
       </c>
     </row>
     <row r="24" spans="1:20" ht="12.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>230</v>
+        <v>227</v>
       </c>
       <c r="C24">
         <v>33</v>
       </c>
       <c r="D24" t="s">
-        <v>157</v>
+        <v>154</v>
       </c>
       <c r="E24" t="s">
-        <v>158</v>
+        <v>155</v>
       </c>
       <c r="F24" t="s">
-        <v>190</v>
+        <v>187</v>
       </c>
       <c r="G24" t="s">
-        <v>243</v>
+        <v>240</v>
       </c>
       <c r="H24" s="37" t="s">
-        <v>242</v>
+        <v>239</v>
       </c>
       <c r="I24">
         <v>35</v>
       </c>
       <c r="J24" t="s">
-        <v>157</v>
+        <v>154</v>
       </c>
       <c r="K24" t="s">
-        <v>158</v>
+        <v>155</v>
       </c>
       <c r="L24" t="s">
-        <v>190</v>
+        <v>187</v>
       </c>
       <c r="M24" t="s">
-        <v>243</v>
+        <v>240</v>
       </c>
       <c r="N24" s="37" t="s">
-        <v>242</v>
+        <v>239</v>
       </c>
       <c r="O24">
         <v>35</v>
       </c>
       <c r="P24" t="s">
-        <v>157</v>
+        <v>154</v>
       </c>
       <c r="Q24" t="s">
-        <v>158</v>
+        <v>155</v>
       </c>
       <c r="R24" t="s">
-        <v>190</v>
+        <v>187</v>
       </c>
       <c r="S24" t="s">
-        <v>243</v>
+        <v>240</v>
       </c>
       <c r="T24" s="37" t="s">
-        <v>242</v>
+        <v>239</v>
       </c>
     </row>
     <row r="25" spans="1:20" ht="12.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>231</v>
+        <v>228</v>
       </c>
       <c r="C25">
         <v>35</v>
       </c>
       <c r="D25" t="s">
-        <v>155</v>
+        <v>152</v>
       </c>
       <c r="E25" t="s">
-        <v>191</v>
+        <v>188</v>
       </c>
       <c r="F25" t="s">
-        <v>199</v>
+        <v>196</v>
       </c>
       <c r="G25" t="s">
-        <v>252</v>
+        <v>249</v>
       </c>
       <c r="H25" s="39" t="s">
-        <v>254</v>
+        <v>251</v>
       </c>
       <c r="I25">
         <v>35</v>
       </c>
       <c r="J25" t="s">
-        <v>155</v>
+        <v>152</v>
       </c>
       <c r="K25" t="s">
-        <v>191</v>
+        <v>188</v>
       </c>
       <c r="L25" t="s">
-        <v>199</v>
+        <v>196</v>
       </c>
       <c r="M25" t="s">
-        <v>252</v>
+        <v>249</v>
       </c>
       <c r="N25" s="39" t="s">
-        <v>254</v>
+        <v>251</v>
       </c>
       <c r="O25">
         <v>35</v>
       </c>
       <c r="P25" t="s">
-        <v>155</v>
+        <v>152</v>
       </c>
       <c r="Q25" t="s">
-        <v>191</v>
+        <v>188</v>
       </c>
       <c r="R25" t="s">
-        <v>199</v>
+        <v>196</v>
       </c>
       <c r="S25" t="s">
-        <v>252</v>
+        <v>249</v>
       </c>
       <c r="T25" s="39" t="s">
-        <v>254</v>
+        <v>251</v>
       </c>
     </row>
     <row r="26" spans="1:20" s="36" customFormat="1" ht="12.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -4699,7 +4712,7 @@
     </row>
     <row r="27" spans="1:20" ht="13" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
-        <v>208</v>
+        <v>205</v>
       </c>
       <c r="B27" s="19" t="s">
         <v>137</v>
@@ -4708,350 +4721,350 @@
         <v>45</v>
       </c>
       <c r="D27" s="1" t="s">
-        <v>195</v>
+        <v>192</v>
       </c>
       <c r="E27" s="1" t="s">
-        <v>180</v>
+        <v>177</v>
       </c>
       <c r="F27" s="1" t="s">
-        <v>228</v>
+        <v>225</v>
       </c>
       <c r="G27" s="1" t="s">
-        <v>162</v>
+        <v>159</v>
       </c>
       <c r="H27" s="39" t="s">
-        <v>164</v>
+        <v>161</v>
       </c>
       <c r="I27">
         <v>45</v>
       </c>
       <c r="J27" s="1" t="s">
-        <v>196</v>
+        <v>193</v>
       </c>
       <c r="K27" t="s">
-        <v>180</v>
+        <v>177</v>
       </c>
       <c r="L27" s="1" t="s">
-        <v>223</v>
+        <v>220</v>
       </c>
       <c r="M27" s="1" t="s">
-        <v>225</v>
+        <v>222</v>
       </c>
       <c r="N27" s="39" t="s">
-        <v>224</v>
+        <v>221</v>
       </c>
       <c r="O27">
         <v>45</v>
       </c>
       <c r="P27" s="1" t="s">
-        <v>197</v>
+        <v>194</v>
       </c>
       <c r="Q27" s="1" t="s">
-        <v>180</v>
+        <v>177</v>
       </c>
       <c r="R27" s="1" t="s">
-        <v>228</v>
+        <v>225</v>
       </c>
       <c r="S27" s="1" t="s">
-        <v>224</v>
+        <v>221</v>
       </c>
       <c r="T27" s="39" t="s">
-        <v>226</v>
+        <v>223</v>
       </c>
     </row>
     <row r="28" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>232</v>
+        <v>229</v>
       </c>
       <c r="C28">
         <v>43</v>
       </c>
       <c r="D28" t="s">
-        <v>181</v>
+        <v>178</v>
       </c>
       <c r="E28" t="s">
-        <v>180</v>
+        <v>177</v>
       </c>
       <c r="F28" t="s">
-        <v>220</v>
+        <v>217</v>
       </c>
       <c r="G28" t="s">
-        <v>200</v>
+        <v>197</v>
       </c>
       <c r="H28" s="39" t="s">
-        <v>221</v>
+        <v>218</v>
       </c>
       <c r="I28">
         <v>43</v>
       </c>
       <c r="J28" t="s">
-        <v>181</v>
+        <v>178</v>
       </c>
       <c r="K28" t="s">
-        <v>180</v>
+        <v>177</v>
       </c>
       <c r="L28" t="s">
-        <v>220</v>
+        <v>217</v>
       </c>
       <c r="M28" t="s">
-        <v>200</v>
+        <v>197</v>
       </c>
       <c r="N28" s="39" t="s">
-        <v>221</v>
+        <v>218</v>
       </c>
       <c r="O28">
         <v>43</v>
       </c>
       <c r="P28" t="s">
-        <v>181</v>
+        <v>178</v>
       </c>
       <c r="Q28" t="s">
-        <v>180</v>
+        <v>177</v>
       </c>
       <c r="R28" t="s">
-        <v>220</v>
+        <v>217</v>
       </c>
       <c r="S28" t="s">
-        <v>200</v>
+        <v>197</v>
       </c>
       <c r="T28" s="39" t="s">
-        <v>221</v>
+        <v>218</v>
       </c>
     </row>
     <row r="29" spans="1:20" ht="12.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>234</v>
+        <v>231</v>
       </c>
       <c r="C29">
         <v>42</v>
       </c>
       <c r="D29" t="s">
-        <v>193</v>
+        <v>190</v>
       </c>
       <c r="E29" t="s">
-        <v>204</v>
+        <v>201</v>
       </c>
       <c r="F29" t="s">
-        <v>198</v>
+        <v>195</v>
       </c>
       <c r="G29" t="s">
-        <v>166</v>
+        <v>163</v>
       </c>
       <c r="H29" s="37" t="s">
-        <v>236</v>
+        <v>233</v>
       </c>
       <c r="I29">
         <v>42</v>
       </c>
       <c r="J29" t="s">
-        <v>183</v>
+        <v>180</v>
       </c>
       <c r="K29" s="1" t="s">
-        <v>248</v>
+        <v>245</v>
       </c>
       <c r="L29" s="1" t="s">
-        <v>165</v>
+        <v>162</v>
       </c>
       <c r="M29" s="1" t="s">
-        <v>218</v>
+        <v>215</v>
       </c>
       <c r="N29" s="39" t="s">
-        <v>236</v>
+        <v>233</v>
       </c>
       <c r="O29">
         <v>44</v>
       </c>
       <c r="P29" t="s">
-        <v>192</v>
+        <v>189</v>
       </c>
       <c r="Q29" s="1" t="s">
-        <v>262</v>
+        <v>259</v>
       </c>
       <c r="R29" s="1" t="s">
-        <v>263</v>
+        <v>260</v>
       </c>
       <c r="S29" s="1" t="s">
-        <v>260</v>
+        <v>257</v>
       </c>
       <c r="T29" s="39" t="s">
-        <v>261</v>
+        <v>258</v>
       </c>
     </row>
     <row r="30" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>233</v>
+        <v>230</v>
       </c>
       <c r="C30">
         <v>47</v>
       </c>
       <c r="D30" t="s">
-        <v>187</v>
+        <v>184</v>
       </c>
       <c r="E30" t="s">
-        <v>163</v>
+        <v>160</v>
       </c>
       <c r="F30" t="s">
-        <v>240</v>
+        <v>237</v>
       </c>
       <c r="G30" t="s">
-        <v>238</v>
+        <v>235</v>
       </c>
       <c r="H30" s="37" t="s">
-        <v>239</v>
+        <v>236</v>
       </c>
       <c r="I30">
         <v>47</v>
       </c>
       <c r="J30" t="s">
-        <v>188</v>
+        <v>185</v>
       </c>
       <c r="K30" s="1" t="s">
-        <v>226</v>
+        <v>223</v>
       </c>
       <c r="L30" s="1" t="s">
-        <v>239</v>
+        <v>236</v>
       </c>
       <c r="M30" s="1" t="s">
-        <v>251</v>
+        <v>248</v>
       </c>
       <c r="N30" s="39" t="s">
-        <v>237</v>
+        <v>234</v>
       </c>
       <c r="O30">
         <v>47</v>
       </c>
       <c r="P30" t="s">
-        <v>189</v>
+        <v>186</v>
       </c>
       <c r="Q30" s="1" t="s">
-        <v>269</v>
+        <v>266</v>
       </c>
       <c r="R30" s="1" t="s">
-        <v>270</v>
+        <v>267</v>
       </c>
       <c r="S30" s="1" t="s">
-        <v>266</v>
+        <v>263</v>
       </c>
       <c r="T30" s="39" t="s">
-        <v>223</v>
+        <v>220</v>
       </c>
     </row>
     <row r="31" spans="1:20" ht="12.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
-        <v>230</v>
+        <v>227</v>
       </c>
       <c r="C31">
         <v>41</v>
       </c>
       <c r="D31" t="s">
-        <v>157</v>
+        <v>154</v>
       </c>
       <c r="E31" t="s">
-        <v>158</v>
+        <v>155</v>
       </c>
       <c r="F31" t="s">
-        <v>190</v>
+        <v>187</v>
       </c>
       <c r="G31" t="s">
-        <v>243</v>
+        <v>240</v>
       </c>
       <c r="H31" s="37" t="s">
-        <v>242</v>
+        <v>239</v>
       </c>
       <c r="I31">
         <v>41</v>
       </c>
       <c r="J31" t="s">
-        <v>157</v>
+        <v>154</v>
       </c>
       <c r="K31" t="s">
-        <v>158</v>
+        <v>155</v>
       </c>
       <c r="L31" t="s">
-        <v>190</v>
+        <v>187</v>
       </c>
       <c r="M31" t="s">
-        <v>243</v>
+        <v>240</v>
       </c>
       <c r="N31" s="37" t="s">
-        <v>242</v>
+        <v>239</v>
       </c>
       <c r="O31">
         <v>41</v>
       </c>
       <c r="P31" t="s">
-        <v>157</v>
+        <v>154</v>
       </c>
       <c r="Q31" t="s">
-        <v>158</v>
+        <v>155</v>
       </c>
       <c r="R31" t="s">
-        <v>190</v>
+        <v>187</v>
       </c>
       <c r="S31" t="s">
-        <v>243</v>
+        <v>240</v>
       </c>
       <c r="T31" s="37" t="s">
-        <v>242</v>
+        <v>239</v>
       </c>
     </row>
     <row r="32" spans="1:20" ht="12.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
-        <v>235</v>
+        <v>232</v>
       </c>
       <c r="C32">
         <v>45</v>
       </c>
       <c r="D32" t="s">
-        <v>194</v>
+        <v>191</v>
       </c>
       <c r="E32" t="s">
-        <v>191</v>
+        <v>188</v>
       </c>
       <c r="F32" t="s">
-        <v>199</v>
+        <v>196</v>
       </c>
       <c r="G32" t="s">
+        <v>249</v>
+      </c>
+      <c r="H32" s="39" t="s">
         <v>252</v>
-      </c>
-      <c r="H32" s="39" t="s">
-        <v>255</v>
       </c>
       <c r="I32">
         <v>45</v>
       </c>
       <c r="J32" t="s">
-        <v>194</v>
+        <v>191</v>
       </c>
       <c r="K32" t="s">
-        <v>191</v>
+        <v>188</v>
       </c>
       <c r="L32" t="s">
-        <v>199</v>
+        <v>196</v>
       </c>
       <c r="M32" t="s">
+        <v>249</v>
+      </c>
+      <c r="N32" s="39" t="s">
         <v>252</v>
-      </c>
-      <c r="N32" s="39" t="s">
-        <v>255</v>
       </c>
       <c r="O32">
         <v>45</v>
       </c>
       <c r="P32" t="s">
-        <v>194</v>
+        <v>191</v>
       </c>
       <c r="Q32" t="s">
-        <v>191</v>
+        <v>188</v>
       </c>
       <c r="R32" t="s">
-        <v>199</v>
+        <v>196</v>
       </c>
       <c r="S32" t="s">
+        <v>249</v>
+      </c>
+      <c r="T32" s="39" t="s">
         <v>252</v>
-      </c>
-      <c r="T32" s="39" t="s">
-        <v>255</v>
       </c>
     </row>
     <row r="33" ht="12.5" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -5076,8 +5089,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5CCA6904-CCBA-4CF4-893E-058C20254CB5}">
   <dimension ref="A1:K39"/>
   <sheetViews>
-    <sheetView topLeftCell="A9" workbookViewId="0">
-      <selection activeCell="G3" sqref="G3"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F19" sqref="F19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
@@ -5088,7 +5101,7 @@
   <sheetData>
     <row r="1" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>291</v>
+        <v>286</v>
       </c>
     </row>
     <row r="3" spans="1:11" ht="13" x14ac:dyDescent="0.3">
@@ -5099,20 +5112,20 @@
         <v>12</v>
       </c>
       <c r="C3" t="s">
-        <v>292</v>
+        <v>287</v>
       </c>
       <c r="D3" t="s">
-        <v>300</v>
+        <v>295</v>
       </c>
       <c r="E3" t="s">
-        <v>160</v>
+        <v>157</v>
       </c>
       <c r="F3" t="s">
-        <v>301</v>
+        <v>296</v>
       </c>
       <c r="G3" s="19"/>
       <c r="K3" t="s">
-        <v>208</v>
+        <v>205</v>
       </c>
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.25">
@@ -5120,16 +5133,16 @@
         <v>12</v>
       </c>
       <c r="C4" t="s">
-        <v>293</v>
+        <v>288</v>
       </c>
       <c r="D4" t="s">
-        <v>303</v>
+        <v>298</v>
       </c>
       <c r="E4" t="s">
-        <v>302</v>
+        <v>297</v>
       </c>
       <c r="K4" t="s">
-        <v>209</v>
+        <v>206</v>
       </c>
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.25">
@@ -5137,22 +5150,22 @@
         <v>11</v>
       </c>
       <c r="C5" t="s">
+        <v>306</v>
+      </c>
+      <c r="D5" t="s">
+        <v>308</v>
+      </c>
+      <c r="E5" t="s">
+        <v>309</v>
+      </c>
+      <c r="F5" t="s">
+        <v>310</v>
+      </c>
+      <c r="G5" t="s">
         <v>311</v>
       </c>
-      <c r="D5" t="s">
-        <v>313</v>
-      </c>
-      <c r="E5" t="s">
-        <v>314</v>
-      </c>
-      <c r="F5" t="s">
-        <v>315</v>
-      </c>
-      <c r="G5" t="s">
-        <v>316</v>
-      </c>
       <c r="K5" t="s">
-        <v>210</v>
+        <v>207</v>
       </c>
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.25">
@@ -5163,22 +5176,22 @@
         <v>23</v>
       </c>
       <c r="C7" t="s">
+        <v>290</v>
+      </c>
+      <c r="D7" t="s">
+        <v>294</v>
+      </c>
+      <c r="E7" t="s">
+        <v>201</v>
+      </c>
+      <c r="F7" t="s">
         <v>295</v>
       </c>
-      <c r="D7" t="s">
-        <v>299</v>
-      </c>
-      <c r="E7" t="s">
-        <v>204</v>
-      </c>
-      <c r="F7" t="s">
-        <v>300</v>
-      </c>
       <c r="G7" t="s">
-        <v>301</v>
+        <v>296</v>
       </c>
       <c r="K7" t="s">
-        <v>208</v>
+        <v>205</v>
       </c>
     </row>
     <row r="8" spans="1:11" x14ac:dyDescent="0.25">
@@ -5186,22 +5199,22 @@
         <v>23</v>
       </c>
       <c r="C8" t="s">
-        <v>296</v>
+        <v>291</v>
       </c>
       <c r="D8" t="s">
-        <v>302</v>
+        <v>297</v>
       </c>
       <c r="E8" t="s">
-        <v>309</v>
+        <v>304</v>
       </c>
       <c r="F8" t="s">
-        <v>304</v>
+        <v>299</v>
       </c>
       <c r="G8" t="s">
-        <v>257</v>
+        <v>254</v>
       </c>
       <c r="K8" t="s">
-        <v>211</v>
+        <v>208</v>
       </c>
     </row>
     <row r="9" spans="1:11" x14ac:dyDescent="0.25">
@@ -5209,22 +5222,22 @@
         <v>25</v>
       </c>
       <c r="C9" t="s">
-        <v>294</v>
+        <v>289</v>
       </c>
       <c r="D9" t="s">
-        <v>305</v>
+        <v>300</v>
       </c>
       <c r="E9" t="s">
-        <v>306</v>
+        <v>301</v>
       </c>
       <c r="F9" t="s">
-        <v>307</v>
+        <v>302</v>
       </c>
       <c r="G9" t="s">
-        <v>308</v>
+        <v>303</v>
       </c>
       <c r="K9" s="1" t="s">
-        <v>234</v>
+        <v>231</v>
       </c>
     </row>
     <row r="10" spans="1:11" x14ac:dyDescent="0.25">
@@ -5232,48 +5245,48 @@
         <v>25</v>
       </c>
       <c r="C10" t="s">
-        <v>311</v>
+        <v>306</v>
       </c>
       <c r="D10" t="s">
-        <v>317</v>
+        <v>312</v>
       </c>
       <c r="E10" t="s">
-        <v>318</v>
+        <v>313</v>
       </c>
       <c r="F10" t="s">
-        <v>314</v>
+        <v>309</v>
       </c>
       <c r="G10" t="s">
-        <v>247</v>
+        <v>244</v>
       </c>
       <c r="K10" t="s">
-        <v>212</v>
+        <v>209</v>
       </c>
     </row>
     <row r="12" spans="1:11" ht="13" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
-        <v>297</v>
+        <v>292</v>
       </c>
       <c r="B12">
         <v>32</v>
       </c>
       <c r="C12" t="s">
-        <v>295</v>
+        <v>290</v>
       </c>
       <c r="D12" t="s">
-        <v>299</v>
+        <v>294</v>
       </c>
       <c r="E12" s="19" t="s">
-        <v>319</v>
+        <v>314</v>
       </c>
       <c r="F12" s="19" t="s">
-        <v>240</v>
+        <v>237</v>
       </c>
       <c r="G12" t="s">
-        <v>301</v>
+        <v>296</v>
       </c>
       <c r="K12" t="s">
-        <v>208</v>
+        <v>205</v>
       </c>
     </row>
     <row r="13" spans="1:11" ht="13" x14ac:dyDescent="0.3">
@@ -5281,22 +5294,22 @@
         <v>32</v>
       </c>
       <c r="C13" t="s">
-        <v>298</v>
+        <v>293</v>
       </c>
       <c r="D13" s="19" t="s">
-        <v>339</v>
+        <v>334</v>
       </c>
       <c r="E13" s="19" t="s">
-        <v>347</v>
+        <v>342</v>
       </c>
       <c r="F13" t="s">
-        <v>304</v>
+        <v>299</v>
       </c>
       <c r="G13" t="s">
-        <v>257</v>
+        <v>254</v>
       </c>
       <c r="K13" t="s">
-        <v>211</v>
+        <v>208</v>
       </c>
     </row>
     <row r="14" spans="1:11" ht="13" x14ac:dyDescent="0.3">
@@ -5304,22 +5317,22 @@
         <v>32</v>
       </c>
       <c r="C14" t="s">
-        <v>294</v>
+        <v>289</v>
       </c>
       <c r="D14" s="19" t="s">
-        <v>310</v>
+        <v>305</v>
       </c>
       <c r="E14" t="s">
-        <v>306</v>
+        <v>301</v>
       </c>
       <c r="F14" s="19" t="s">
-        <v>356</v>
+        <v>350</v>
       </c>
       <c r="G14" t="s">
-        <v>308</v>
+        <v>303</v>
       </c>
       <c r="K14" s="1" t="s">
-        <v>234</v>
+        <v>231</v>
       </c>
     </row>
     <row r="15" spans="1:11" x14ac:dyDescent="0.25">
@@ -5327,283 +5340,279 @@
         <v>32</v>
       </c>
       <c r="C15" t="s">
+        <v>307</v>
+      </c>
+      <c r="D15" t="s">
         <v>312</v>
       </c>
-      <c r="D15" t="s">
-        <v>317</v>
-      </c>
       <c r="E15" t="s">
-        <v>318</v>
+        <v>313</v>
       </c>
       <c r="F15" t="s">
-        <v>240</v>
+        <v>237</v>
       </c>
       <c r="G15" t="s">
-        <v>249</v>
+        <v>246</v>
       </c>
       <c r="K15" s="1" t="s">
-        <v>233</v>
+        <v>230</v>
       </c>
     </row>
     <row r="16" spans="1:11" x14ac:dyDescent="0.25">
       <c r="K16" t="s">
-        <v>230</v>
+        <v>227</v>
       </c>
     </row>
     <row r="17" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A17" s="1" t="s">
-        <v>343</v>
-      </c>
-      <c r="D17">
-        <f>COUNTIF(D19:G38, "?")</f>
-        <v>0</v>
+        <v>338</v>
       </c>
     </row>
     <row r="19" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A19" s="1" t="s">
-        <v>334</v>
+        <v>329</v>
       </c>
       <c r="B19">
-        <v>45</v>
+        <v>50</v>
       </c>
       <c r="C19" s="1" t="s">
-        <v>331</v>
+        <v>326</v>
       </c>
       <c r="D19" s="1" t="s">
-        <v>344</v>
+        <v>339</v>
       </c>
       <c r="E19" s="1" t="s">
-        <v>345</v>
+        <v>340</v>
       </c>
       <c r="F19" s="1" t="s">
-        <v>241</v>
+        <v>238</v>
       </c>
       <c r="G19" s="1" t="s">
-        <v>255</v>
+        <v>252</v>
       </c>
       <c r="K19" t="s">
-        <v>208</v>
+        <v>205</v>
       </c>
     </row>
     <row r="20" spans="1:11" ht="13" x14ac:dyDescent="0.3">
       <c r="B20">
-        <v>45</v>
+        <v>48</v>
       </c>
       <c r="C20" s="1" t="s">
-        <v>332</v>
+        <v>327</v>
       </c>
       <c r="D20" s="1" t="s">
-        <v>346</v>
+        <v>341</v>
       </c>
       <c r="E20" s="1" t="s">
-        <v>302</v>
+        <v>297</v>
       </c>
       <c r="F20" s="1" t="s">
-        <v>270</v>
+        <v>267</v>
       </c>
       <c r="G20" s="19" t="s">
-        <v>347</v>
+        <v>342</v>
       </c>
       <c r="K20" t="s">
-        <v>232</v>
+        <v>229</v>
       </c>
     </row>
     <row r="21" spans="1:11" ht="13" x14ac:dyDescent="0.3">
       <c r="B21">
-        <v>45</v>
+        <v>48</v>
       </c>
       <c r="C21" s="1" t="s">
-        <v>333</v>
+        <v>328</v>
       </c>
       <c r="D21" s="19" t="s">
-        <v>339</v>
+        <v>334</v>
       </c>
       <c r="E21" s="1" t="s">
-        <v>348</v>
+        <v>343</v>
       </c>
       <c r="F21" s="1" t="s">
-        <v>349</v>
+        <v>344</v>
       </c>
       <c r="G21" s="1" t="s">
-        <v>258</v>
+        <v>255</v>
       </c>
       <c r="K21" t="s">
-        <v>234</v>
+        <v>231</v>
       </c>
     </row>
     <row r="22" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B22">
-        <v>45</v>
+        <v>52</v>
       </c>
       <c r="C22" s="1" t="s">
-        <v>324</v>
+        <v>319</v>
       </c>
       <c r="D22" s="1" t="s">
-        <v>239</v>
+        <v>236</v>
       </c>
       <c r="E22" s="1" t="s">
-        <v>350</v>
+        <v>345</v>
       </c>
       <c r="F22" s="1" t="s">
-        <v>204</v>
+        <v>201</v>
       </c>
       <c r="G22" s="1" t="s">
-        <v>351</v>
+        <v>346</v>
       </c>
       <c r="K22" t="s">
-        <v>233</v>
+        <v>230</v>
       </c>
     </row>
     <row r="23" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B23">
-        <v>45</v>
+        <v>48</v>
       </c>
       <c r="C23" s="1" t="s">
-        <v>340</v>
+        <v>335</v>
       </c>
       <c r="D23" s="1" t="s">
-        <v>339</v>
+        <v>334</v>
       </c>
       <c r="E23" s="1" t="s">
-        <v>352</v>
+        <v>347</v>
       </c>
       <c r="F23" s="1" t="s">
-        <v>353</v>
+        <v>348</v>
       </c>
       <c r="G23" s="1" t="s">
-        <v>355</v>
+        <v>379</v>
       </c>
       <c r="K23" t="s">
-        <v>230</v>
+        <v>227</v>
       </c>
     </row>
     <row r="24" spans="1:11" ht="13" x14ac:dyDescent="0.3">
       <c r="D24" s="19"/>
       <c r="K24" t="s">
-        <v>235</v>
+        <v>232</v>
       </c>
     </row>
     <row r="26" spans="1:11" ht="13" x14ac:dyDescent="0.3">
       <c r="A26" s="1" t="s">
-        <v>341</v>
+        <v>336</v>
       </c>
       <c r="B26">
-        <v>48</v>
+        <v>54</v>
       </c>
       <c r="C26" s="1" t="s">
-        <v>326</v>
+        <v>321</v>
       </c>
       <c r="D26" s="19" t="s">
-        <v>319</v>
+        <v>314</v>
       </c>
       <c r="E26" s="19" t="s">
+        <v>223</v>
+      </c>
+      <c r="F26" s="1" t="s">
+        <v>247</v>
+      </c>
+      <c r="G26" s="1" t="s">
         <v>226</v>
       </c>
-      <c r="F26" s="1" t="s">
-        <v>250</v>
-      </c>
-      <c r="G26" s="1" t="s">
-        <v>229</v>
-      </c>
       <c r="K26" t="s">
-        <v>208</v>
+        <v>205</v>
       </c>
     </row>
     <row r="27" spans="1:11" ht="13" x14ac:dyDescent="0.3">
       <c r="B27">
-        <v>52</v>
+        <v>54</v>
       </c>
       <c r="C27" s="1" t="s">
-        <v>327</v>
+        <v>322</v>
       </c>
       <c r="D27" s="19" t="s">
-        <v>156</v>
+        <v>153</v>
       </c>
       <c r="E27" s="19" t="s">
-        <v>356</v>
+        <v>350</v>
       </c>
       <c r="F27" s="1" t="s">
-        <v>358</v>
+        <v>352</v>
       </c>
       <c r="G27" s="1" t="s">
-        <v>357</v>
+        <v>351</v>
       </c>
       <c r="K27" t="s">
-        <v>232</v>
+        <v>229</v>
       </c>
     </row>
     <row r="28" spans="1:11" ht="13" x14ac:dyDescent="0.3">
       <c r="B28">
-        <v>50</v>
+        <v>54</v>
       </c>
       <c r="C28" s="1" t="s">
-        <v>328</v>
+        <v>323</v>
       </c>
       <c r="D28" s="19" t="s">
-        <v>307</v>
+        <v>302</v>
       </c>
       <c r="E28" s="1" t="s">
-        <v>342</v>
+        <v>337</v>
       </c>
       <c r="F28" s="1" t="s">
-        <v>206</v>
+        <v>203</v>
       </c>
       <c r="G28" s="1" t="s">
-        <v>236</v>
+        <v>233</v>
       </c>
       <c r="K28" t="s">
-        <v>234</v>
+        <v>231</v>
       </c>
     </row>
     <row r="29" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B29">
-        <v>50</v>
+        <v>56</v>
       </c>
       <c r="C29" s="1" t="s">
-        <v>336</v>
+        <v>331</v>
       </c>
       <c r="D29" s="1" t="s">
-        <v>337</v>
+        <v>332</v>
       </c>
       <c r="E29" s="1" t="s">
-        <v>338</v>
+        <v>333</v>
       </c>
       <c r="F29" s="1" t="s">
-        <v>359</v>
+        <v>353</v>
       </c>
       <c r="G29" s="1" t="s">
-        <v>360</v>
+        <v>354</v>
       </c>
       <c r="K29" t="s">
-        <v>233</v>
+        <v>230</v>
       </c>
     </row>
     <row r="30" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B30">
-        <v>50</v>
+        <v>58</v>
       </c>
       <c r="C30" s="1" t="s">
-        <v>335</v>
+        <v>330</v>
       </c>
       <c r="D30" s="1" t="s">
-        <v>361</v>
+        <v>355</v>
       </c>
       <c r="E30" s="1" t="s">
-        <v>362</v>
+        <v>356</v>
       </c>
       <c r="F30" s="1" t="s">
-        <v>249</v>
+        <v>246</v>
       </c>
       <c r="G30" s="1" t="s">
-        <v>223</v>
+        <v>220</v>
       </c>
       <c r="K30" t="s">
-        <v>230</v>
+        <v>227</v>
       </c>
     </row>
     <row r="31" spans="1:11" x14ac:dyDescent="0.25">
       <c r="K31" t="s">
-        <v>235</v>
+        <v>232</v>
       </c>
     </row>
     <row r="33" spans="1:11" x14ac:dyDescent="0.25">
@@ -5614,22 +5623,22 @@
         <v>66</v>
       </c>
       <c r="C33" t="s">
-        <v>320</v>
+        <v>315</v>
       </c>
       <c r="D33" s="1" t="s">
-        <v>270</v>
+        <v>267</v>
       </c>
       <c r="E33" s="1" t="s">
-        <v>249</v>
+        <v>246</v>
       </c>
       <c r="F33" s="1" t="s">
-        <v>237</v>
+        <v>234</v>
       </c>
       <c r="G33" s="1" t="s">
-        <v>203</v>
+        <v>200</v>
       </c>
       <c r="K33" t="s">
-        <v>208</v>
+        <v>205</v>
       </c>
     </row>
     <row r="34" spans="1:11" x14ac:dyDescent="0.25">
@@ -5637,22 +5646,22 @@
         <v>60</v>
       </c>
       <c r="C34" t="s">
-        <v>321</v>
+        <v>316</v>
       </c>
       <c r="D34" s="1" t="s">
-        <v>363</v>
+        <v>357</v>
       </c>
       <c r="E34" s="1" t="s">
-        <v>165</v>
+        <v>162</v>
       </c>
       <c r="F34" s="1" t="s">
-        <v>160</v>
+        <v>155</v>
       </c>
       <c r="G34" s="1" t="s">
-        <v>364</v>
+        <v>376</v>
       </c>
       <c r="K34" t="s">
-        <v>232</v>
+        <v>229</v>
       </c>
     </row>
     <row r="35" spans="1:11" x14ac:dyDescent="0.25">
@@ -5660,22 +5669,22 @@
         <v>60</v>
       </c>
       <c r="C35" t="s">
-        <v>322</v>
+        <v>317</v>
       </c>
       <c r="D35" s="1" t="s">
-        <v>164</v>
+        <v>161</v>
       </c>
       <c r="E35" s="1" t="s">
-        <v>165</v>
+        <v>162</v>
       </c>
       <c r="F35" s="1" t="s">
-        <v>160</v>
+        <v>377</v>
       </c>
       <c r="G35" s="1" t="s">
-        <v>364</v>
+        <v>378</v>
       </c>
       <c r="K35" t="s">
-        <v>234</v>
+        <v>231</v>
       </c>
     </row>
     <row r="36" spans="1:11" x14ac:dyDescent="0.25">
@@ -5683,22 +5692,22 @@
         <v>62</v>
       </c>
       <c r="C36" t="s">
-        <v>323</v>
+        <v>318</v>
       </c>
       <c r="D36" s="1" t="s">
-        <v>165</v>
+        <v>162</v>
       </c>
       <c r="E36" s="1" t="s">
-        <v>365</v>
+        <v>358</v>
       </c>
       <c r="F36" s="1" t="s">
-        <v>362</v>
+        <v>356</v>
       </c>
       <c r="G36" s="1" t="s">
-        <v>366</v>
+        <v>359</v>
       </c>
       <c r="K36" t="s">
-        <v>233</v>
+        <v>230</v>
       </c>
     </row>
     <row r="37" spans="1:11" x14ac:dyDescent="0.25">
@@ -5706,22 +5715,22 @@
         <v>65</v>
       </c>
       <c r="C37" t="s">
-        <v>325</v>
+        <v>320</v>
       </c>
       <c r="D37" s="1" t="s">
-        <v>348</v>
+        <v>343</v>
       </c>
       <c r="E37" s="1" t="s">
-        <v>240</v>
+        <v>237</v>
       </c>
       <c r="F37" s="1" t="s">
-        <v>369</v>
+        <v>362</v>
       </c>
       <c r="G37" s="1" t="s">
-        <v>354</v>
+        <v>349</v>
       </c>
       <c r="K37" t="s">
-        <v>230</v>
+        <v>227</v>
       </c>
     </row>
     <row r="38" spans="1:11" ht="13" x14ac:dyDescent="0.3">
@@ -5729,27 +5738,27 @@
         <v>60</v>
       </c>
       <c r="C38" s="1" t="s">
-        <v>330</v>
+        <v>325</v>
       </c>
       <c r="D38" s="1" t="s">
-        <v>165</v>
+        <v>162</v>
       </c>
       <c r="E38" s="1" t="s">
-        <v>367</v>
+        <v>360</v>
       </c>
       <c r="F38" s="1" t="s">
-        <v>348</v>
+        <v>343</v>
       </c>
       <c r="G38" s="19" t="s">
-        <v>240</v>
+        <v>237</v>
       </c>
       <c r="K38" t="s">
-        <v>235</v>
+        <v>232</v>
       </c>
     </row>
     <row r="39" spans="1:11" x14ac:dyDescent="0.25">
       <c r="K39" s="1" t="s">
-        <v>368</v>
+        <v>361</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
revised the player sprite, biking sprite, player back sprite
</commit_message>
<xml_diff>
--- a/Silver_Todo.xlsx
+++ b/Silver_Todo.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\dwg11\Silver\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A7A43857-53DF-4E5F-B88C-A3DEC9ACC7EF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6D7BDC96-C029-4F21-9EBB-031672060168}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="12330" windowHeight="15280" tabRatio="788" firstSheet="1" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="25820" windowHeight="15500" tabRatio="788" firstSheet="1" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Overview and Credits" sheetId="2" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="776" uniqueCount="380">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="777" uniqueCount="380">
   <si>
     <t>Pallet Town</t>
   </si>
@@ -1133,15 +1133,6 @@
     <t>extra rare candy at entrance</t>
   </si>
   <si>
-    <t>cal team, gio tem</t>
-  </si>
-  <si>
-    <t>m/f?</t>
-  </si>
-  <si>
-    <t>t.d.</t>
-  </si>
-  <si>
     <t>intro text for giovanni</t>
   </si>
   <si>
@@ -1157,9 +1148,6 @@
     <t>force "male" option</t>
   </si>
   <si>
-    <t>"add a new map"</t>
-  </si>
-  <si>
     <t>edit:</t>
   </si>
   <si>
@@ -1176,6 +1164,18 @@
   </si>
   <si>
     <t>HP Rock</t>
+  </si>
+  <si>
+    <t>need td cal teams</t>
+  </si>
+  <si>
+    <t>cal team</t>
+  </si>
+  <si>
+    <t>to do</t>
+  </si>
+  <si>
+    <t>"add a new map" / fix the size?</t>
   </si>
 </sst>
 </file>
@@ -2592,8 +2592,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4D4D23E0-802A-4842-9CD9-587C61A270C2}">
   <dimension ref="A1:E142"/>
   <sheetViews>
-    <sheetView topLeftCell="B77" workbookViewId="0">
-      <selection activeCell="C105" sqref="C105"/>
+    <sheetView tabSelected="1" topLeftCell="A77" workbookViewId="0">
+      <selection activeCell="B100" sqref="B100"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
@@ -3193,7 +3193,7 @@
         <v>109</v>
       </c>
       <c r="B91" t="s">
-        <v>371</v>
+        <v>277</v>
       </c>
     </row>
     <row r="92" spans="1:3" x14ac:dyDescent="0.25">
@@ -3201,7 +3201,7 @@
         <v>280</v>
       </c>
       <c r="B92" t="s">
-        <v>367</v>
+        <v>378</v>
       </c>
     </row>
     <row r="93" spans="1:3" x14ac:dyDescent="0.25">
@@ -3217,7 +3217,7 @@
         <v>141</v>
       </c>
       <c r="B94" t="s">
-        <v>366</v>
+        <v>277</v>
       </c>
     </row>
     <row r="95" spans="1:3" x14ac:dyDescent="0.25">
@@ -3233,7 +3233,10 @@
         <v>144</v>
       </c>
       <c r="B96" t="s">
-        <v>365</v>
+        <v>377</v>
+      </c>
+      <c r="C96" t="s">
+        <v>376</v>
       </c>
     </row>
     <row r="97" spans="1:3" x14ac:dyDescent="0.25">
@@ -3257,15 +3260,15 @@
         <v>147</v>
       </c>
       <c r="B99" t="s">
-        <v>371</v>
+        <v>368</v>
       </c>
     </row>
     <row r="100" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A100" s="1" t="s">
+        <v>366</v>
+      </c>
+      <c r="B100" t="s">
         <v>369</v>
-      </c>
-      <c r="B100" t="s">
-        <v>372</v>
       </c>
     </row>
     <row r="101" spans="1:3" x14ac:dyDescent="0.25">
@@ -3273,7 +3276,7 @@
         <v>148</v>
       </c>
       <c r="B101" t="s">
-        <v>371</v>
+        <v>277</v>
       </c>
     </row>
     <row r="102" spans="1:3" x14ac:dyDescent="0.25">
@@ -3289,7 +3292,7 @@
         <v>276</v>
       </c>
       <c r="B103" t="s">
-        <v>373</v>
+        <v>379</v>
       </c>
     </row>
     <row r="104" spans="1:3" x14ac:dyDescent="0.25">
@@ -3297,20 +3300,20 @@
         <v>363</v>
       </c>
       <c r="B104" t="s">
-        <v>374</v>
+        <v>370</v>
       </c>
       <c r="C104" t="s">
-        <v>375</v>
+        <v>371</v>
       </c>
     </row>
     <row r="105" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A105" s="1" t="s">
-        <v>368</v>
+        <v>365</v>
       </c>
     </row>
     <row r="106" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A106" s="1" t="s">
-        <v>370</v>
+        <v>367</v>
       </c>
       <c r="B106" t="s">
         <v>277</v>
@@ -5089,7 +5092,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5CCA6904-CCBA-4CF4-893E-058C20254CB5}">
   <dimension ref="A1:K39"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="F19" sqref="F19"/>
     </sheetView>
   </sheetViews>
@@ -5480,7 +5483,7 @@
         <v>348</v>
       </c>
       <c r="G23" s="1" t="s">
-        <v>379</v>
+        <v>375</v>
       </c>
       <c r="K23" t="s">
         <v>227</v>
@@ -5658,7 +5661,7 @@
         <v>155</v>
       </c>
       <c r="G34" s="1" t="s">
-        <v>376</v>
+        <v>372</v>
       </c>
       <c r="K34" t="s">
         <v>229</v>
@@ -5678,10 +5681,10 @@
         <v>162</v>
       </c>
       <c r="F35" s="1" t="s">
-        <v>377</v>
+        <v>373</v>
       </c>
       <c r="G35" s="1" t="s">
-        <v>378</v>
+        <v>374</v>
       </c>
       <c r="K35" t="s">
         <v>231</v>

</xml_diff>

<commit_message>
added dad phone number using wiki tutorial
</commit_message>
<xml_diff>
--- a/Silver_Todo.xlsx
+++ b/Silver_Todo.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\dwg11\Silver\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B745075C-F352-4431-AAD8-189831F697EE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BD764EE2-A6D7-46AC-BB1F-DE041321775A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="25820" windowHeight="15500" tabRatio="788" firstSheet="1" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="790" uniqueCount="390">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="791" uniqueCount="390">
   <si>
     <t>Pallet Town</t>
   </si>
@@ -1172,9 +1172,6 @@
     <t>giovanni phone</t>
   </si>
   <si>
-    <t>Add a new phone contact · pret/pokecrystal Wiki (github.com)</t>
-  </si>
-  <si>
     <t>HM mules</t>
   </si>
   <si>
@@ -1206,6 +1203,9 @@
   </si>
   <si>
     <t>scraped from crystal clear, in newsprites</t>
+  </si>
+  <si>
+    <t>need to give the number and code for the phone calls player receives</t>
   </si>
 </sst>
 </file>
@@ -1410,7 +1410,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="46">
+  <cellXfs count="43">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -1475,6 +1475,30 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1484,39 +1508,22 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="2">
+  <dxfs count="3">
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <font>
         <color rgb="FF006100"/>
@@ -2593,19 +2600,19 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4D4D23E0-802A-4842-9CD9-587C61A270C2}">
   <dimension ref="A1:E142"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A82" workbookViewId="0">
-      <selection activeCell="C119" sqref="C119"/>
+    <sheetView tabSelected="1" topLeftCell="A76" workbookViewId="0">
+      <selection activeCell="B108" sqref="B108"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="40.26953125" style="45" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="40.26953125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="11.1796875" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="83.6328125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" ht="13" x14ac:dyDescent="0.25">
-      <c r="A1" s="35" t="s">
+      <c r="A1" s="32" t="s">
         <v>87</v>
       </c>
       <c r="B1" t="s">
@@ -2619,7 +2626,7 @@
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A2" s="36" t="s">
+      <c r="A2" s="33" t="s">
         <v>98</v>
       </c>
       <c r="C2" s="1" t="s">
@@ -2627,7 +2634,7 @@
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A3" s="37" t="s">
+      <c r="A3" s="34" t="s">
         <v>29</v>
       </c>
       <c r="C3" t="s">
@@ -2635,17 +2642,17 @@
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A4" s="37" t="s">
+      <c r="A4" s="34" t="s">
         <v>30</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A5" s="37" t="s">
+      <c r="A5" s="34" t="s">
         <v>77</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A6" s="37" t="s">
+      <c r="A6" s="34" t="s">
         <v>78</v>
       </c>
       <c r="C6" s="1" t="s">
@@ -2653,12 +2660,12 @@
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A7" s="37" t="s">
+      <c r="A7" s="34" t="s">
         <v>31</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A8" s="37" t="s">
+      <c r="A8" s="34" t="s">
         <v>32</v>
       </c>
       <c r="C8" s="1" t="s">
@@ -2666,13 +2673,13 @@
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A9" s="37" t="s">
+      <c r="A9" s="34" t="s">
         <v>33</v>
       </c>
       <c r="C9" s="1"/>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A10" s="37" t="s">
+      <c r="A10" s="34" t="s">
         <v>34</v>
       </c>
       <c r="C10" t="s">
@@ -2680,7 +2687,7 @@
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A11" s="37" t="s">
+      <c r="A11" s="34" t="s">
         <v>47</v>
       </c>
       <c r="C11" s="1" t="s">
@@ -2688,7 +2695,7 @@
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A12" s="37" t="s">
+      <c r="A12" s="34" t="s">
         <v>35</v>
       </c>
       <c r="B12" s="1"/>
@@ -2697,22 +2704,22 @@
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A13" s="38" t="s">
+      <c r="A13" s="35" t="s">
         <v>36</v>
       </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A14" s="37" t="s">
+      <c r="A14" s="34" t="s">
         <v>37</v>
       </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A15" s="37" t="s">
+      <c r="A15" s="34" t="s">
         <v>38</v>
       </c>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A16" s="37" t="s">
+      <c r="A16" s="34" t="s">
         <v>39</v>
       </c>
       <c r="C16" t="s">
@@ -2720,7 +2727,7 @@
       </c>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A17" s="37" t="s">
+      <c r="A17" s="34" t="s">
         <v>40</v>
       </c>
       <c r="C17" s="1" t="s">
@@ -2728,7 +2735,7 @@
       </c>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A18" s="37" t="s">
+      <c r="A18" s="34" t="s">
         <v>41</v>
       </c>
       <c r="C18" s="1" t="s">
@@ -2736,7 +2743,7 @@
       </c>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A19" s="38" t="s">
+      <c r="A19" s="35" t="s">
         <v>42</v>
       </c>
       <c r="C19" s="1" t="s">
@@ -2745,7 +2752,7 @@
       <c r="E19" s="1"/>
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A20" s="37" t="s">
+      <c r="A20" s="34" t="s">
         <v>43</v>
       </c>
       <c r="C20" s="1" t="s">
@@ -2753,7 +2760,7 @@
       </c>
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A21" s="37" t="s">
+      <c r="A21" s="34" t="s">
         <v>44</v>
       </c>
       <c r="C21" s="1" t="s">
@@ -2761,22 +2768,22 @@
       </c>
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A22" s="37" t="s">
+      <c r="A22" s="34" t="s">
         <v>45</v>
       </c>
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A23" s="37" t="s">
+      <c r="A23" s="34" t="s">
         <v>46</v>
       </c>
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A24" s="38" t="s">
+      <c r="A24" s="35" t="s">
         <v>84</v>
       </c>
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A25" s="37" t="s">
+      <c r="A25" s="34" t="s">
         <v>79</v>
       </c>
       <c r="C25" t="s">
@@ -2784,7 +2791,7 @@
       </c>
     </row>
     <row r="26" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A26" s="37" t="s">
+      <c r="A26" s="34" t="s">
         <v>48</v>
       </c>
       <c r="C26" s="1" t="s">
@@ -2792,7 +2799,7 @@
       </c>
     </row>
     <row r="27" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A27" s="38" t="s">
+      <c r="A27" s="35" t="s">
         <v>49</v>
       </c>
       <c r="C27" s="1" t="s">
@@ -2800,7 +2807,7 @@
       </c>
     </row>
     <row r="28" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A28" s="37" t="s">
+      <c r="A28" s="34" t="s">
         <v>68</v>
       </c>
       <c r="C28" s="1" t="s">
@@ -2808,17 +2815,17 @@
       </c>
     </row>
     <row r="29" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A29" s="37" t="s">
+      <c r="A29" s="34" t="s">
         <v>51</v>
       </c>
     </row>
     <row r="30" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A30" s="37" t="s">
+      <c r="A30" s="34" t="s">
         <v>52</v>
       </c>
     </row>
     <row r="31" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A31" s="37" t="s">
+      <c r="A31" s="34" t="s">
         <v>53</v>
       </c>
       <c r="C31" s="1" t="s">
@@ -2826,22 +2833,22 @@
       </c>
     </row>
     <row r="32" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A32" s="37" t="s">
+      <c r="A32" s="34" t="s">
         <v>81</v>
       </c>
     </row>
     <row r="33" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A33" s="37" t="s">
+      <c r="A33" s="34" t="s">
         <v>54</v>
       </c>
     </row>
     <row r="34" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A34" s="37" t="s">
+      <c r="A34" s="34" t="s">
         <v>55</v>
       </c>
     </row>
     <row r="35" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A35" s="38" t="s">
+      <c r="A35" s="35" t="s">
         <v>57</v>
       </c>
       <c r="C35" s="1" t="s">
@@ -2849,36 +2856,36 @@
       </c>
     </row>
     <row r="36" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A36" s="37" t="s">
+      <c r="A36" s="34" t="s">
         <v>83</v>
       </c>
     </row>
     <row r="37" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A37" s="37" t="s">
+      <c r="A37" s="34" t="s">
         <v>76</v>
       </c>
       <c r="C37" s="1"/>
     </row>
     <row r="38" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A38" s="37" t="s">
+      <c r="A38" s="34" t="s">
         <v>58</v>
       </c>
     </row>
     <row r="39" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A39" s="37" t="s">
+      <c r="A39" s="34" t="s">
         <v>59</v>
       </c>
     </row>
     <row r="40" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A40" s="37" t="s">
+      <c r="A40" s="34" t="s">
         <v>60</v>
       </c>
       <c r="C40" t="s">
-        <v>385</v>
+        <v>384</v>
       </c>
     </row>
     <row r="41" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A41" s="38" t="s">
+      <c r="A41" s="35" t="s">
         <v>61</v>
       </c>
       <c r="C41" t="s">
@@ -2886,12 +2893,12 @@
       </c>
     </row>
     <row r="42" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A42" s="39" t="s">
+      <c r="A42" s="36" t="s">
         <v>56</v>
       </c>
     </row>
     <row r="43" spans="1:3" ht="50" x14ac:dyDescent="0.25">
-      <c r="A43" s="37" t="s">
+      <c r="A43" s="34" t="s">
         <v>272</v>
       </c>
       <c r="C43" s="29" t="s">
@@ -2899,17 +2906,17 @@
       </c>
     </row>
     <row r="44" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A44" s="37" t="s">
+      <c r="A44" s="34" t="s">
         <v>62</v>
       </c>
     </row>
     <row r="45" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A45" s="37" t="s">
+      <c r="A45" s="34" t="s">
         <v>63</v>
       </c>
     </row>
     <row r="46" spans="1:3" ht="25" x14ac:dyDescent="0.25">
-      <c r="A46" s="37" t="s">
+      <c r="A46" s="34" t="s">
         <v>64</v>
       </c>
       <c r="C46" s="30" t="s">
@@ -2917,7 +2924,7 @@
       </c>
     </row>
     <row r="47" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A47" s="37" t="s">
+      <c r="A47" s="34" t="s">
         <v>65</v>
       </c>
       <c r="C47" t="s">
@@ -2925,27 +2932,27 @@
       </c>
     </row>
     <row r="48" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A48" s="38" t="s">
+      <c r="A48" s="35" t="s">
         <v>66</v>
       </c>
     </row>
     <row r="49" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A49" s="37" t="s">
+      <c r="A49" s="34" t="s">
         <v>50</v>
       </c>
     </row>
     <row r="50" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A50" s="37" t="s">
+      <c r="A50" s="34" t="s">
         <v>67</v>
       </c>
     </row>
     <row r="51" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A51" s="37" t="s">
+      <c r="A51" s="34" t="s">
         <v>69</v>
       </c>
     </row>
     <row r="52" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A52" s="37" t="s">
+      <c r="A52" s="34" t="s">
         <v>28</v>
       </c>
       <c r="C52" s="1" t="s">
@@ -2953,7 +2960,7 @@
       </c>
     </row>
     <row r="53" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A53" s="38" t="s">
+      <c r="A53" s="35" t="s">
         <v>80</v>
       </c>
       <c r="C53" t="s">
@@ -2961,15 +2968,15 @@
       </c>
     </row>
     <row r="54" spans="1:3" ht="13" x14ac:dyDescent="0.25">
-      <c r="A54" s="40" t="s">
+      <c r="A54" s="37" t="s">
         <v>82</v>
       </c>
     </row>
     <row r="55" spans="1:3" ht="13" x14ac:dyDescent="0.25">
-      <c r="A55" s="41"/>
+      <c r="A55" s="38"/>
     </row>
     <row r="56" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A56" s="37" t="s">
+      <c r="A56" s="34" t="s">
         <v>3</v>
       </c>
       <c r="C56" s="1" t="s">
@@ -2977,7 +2984,7 @@
       </c>
     </row>
     <row r="57" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A57" s="37" t="s">
+      <c r="A57" s="34" t="s">
         <v>114</v>
       </c>
       <c r="C57" s="1" t="s">
@@ -2985,24 +2992,24 @@
       </c>
     </row>
     <row r="58" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A58" s="37" t="s">
+      <c r="A58" s="34" t="s">
         <v>70</v>
       </c>
       <c r="C58" s="1"/>
     </row>
     <row r="59" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A59" s="37" t="s">
+      <c r="A59" s="34" t="s">
         <v>71</v>
       </c>
       <c r="C59" s="1"/>
     </row>
     <row r="60" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A60" s="37" t="s">
+      <c r="A60" s="34" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="61" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A61" s="37" t="s">
+      <c r="A61" s="34" t="s">
         <v>5</v>
       </c>
       <c r="C61" s="1" t="s">
@@ -3010,27 +3017,27 @@
       </c>
     </row>
     <row r="62" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A62" s="37" t="s">
+      <c r="A62" s="34" t="s">
         <v>140</v>
       </c>
     </row>
     <row r="63" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A63" s="37" t="s">
+      <c r="A63" s="34" t="s">
         <v>1</v>
       </c>
     </row>
     <row r="64" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A64" s="37" t="s">
+      <c r="A64" s="34" t="s">
         <v>0</v>
       </c>
     </row>
     <row r="65" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A65" s="37" t="s">
+      <c r="A65" s="34" t="s">
         <v>27</v>
       </c>
     </row>
     <row r="66" spans="1:3" ht="13" x14ac:dyDescent="0.25">
-      <c r="A66" s="42" t="s">
+      <c r="A66" s="39" t="s">
         <v>115</v>
       </c>
       <c r="C66" s="1" t="s">
@@ -3038,17 +3045,17 @@
       </c>
     </row>
     <row r="67" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A67" s="37" t="s">
+      <c r="A67" s="34" t="s">
         <v>25</v>
       </c>
     </row>
     <row r="68" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A68" s="37" t="s">
+      <c r="A68" s="34" t="s">
         <v>24</v>
       </c>
     </row>
     <row r="69" spans="1:3" ht="13" x14ac:dyDescent="0.25">
-      <c r="A69" s="42" t="s">
+      <c r="A69" s="39" t="s">
         <v>116</v>
       </c>
       <c r="C69" s="1" t="s">
@@ -3056,12 +3063,12 @@
       </c>
     </row>
     <row r="70" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A70" s="37" t="s">
+      <c r="A70" s="34" t="s">
         <v>128</v>
       </c>
     </row>
     <row r="71" spans="1:3" ht="13" x14ac:dyDescent="0.3">
-      <c r="A71" s="43" t="s">
+      <c r="A71" s="13" t="s">
         <v>119</v>
       </c>
       <c r="C71" s="1" t="s">
@@ -3069,13 +3076,13 @@
       </c>
     </row>
     <row r="72" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A72" s="37" t="s">
+      <c r="A72" s="34" t="s">
         <v>17</v>
       </c>
       <c r="C72" s="1"/>
     </row>
     <row r="73" spans="1:3" ht="13" x14ac:dyDescent="0.25">
-      <c r="A73" s="42" t="s">
+      <c r="A73" s="39" t="s">
         <v>120</v>
       </c>
       <c r="C73" s="1" t="s">
@@ -3083,13 +3090,13 @@
       </c>
     </row>
     <row r="74" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A74" s="37" t="s">
+      <c r="A74" s="34" t="s">
         <v>11</v>
       </c>
       <c r="C74" s="1"/>
     </row>
     <row r="75" spans="1:3" ht="13" x14ac:dyDescent="0.25">
-      <c r="A75" s="42" t="s">
+      <c r="A75" s="39" t="s">
         <v>121</v>
       </c>
       <c r="C75" s="1" t="s">
@@ -3097,23 +3104,23 @@
       </c>
     </row>
     <row r="76" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A76" s="44" t="s">
+      <c r="A76" s="1" t="s">
         <v>130</v>
       </c>
     </row>
     <row r="77" spans="1:3" ht="13" x14ac:dyDescent="0.25">
-      <c r="A77" s="41" t="s">
+      <c r="A77" s="38" t="s">
         <v>127</v>
       </c>
     </row>
     <row r="78" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A78" s="44" t="s">
+      <c r="A78" s="1" t="s">
         <v>131</v>
       </c>
       <c r="C78" s="1"/>
     </row>
     <row r="79" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A79" s="44" t="s">
+      <c r="A79" s="1" t="s">
         <v>132</v>
       </c>
       <c r="C79" s="1" t="s">
@@ -3121,13 +3128,13 @@
       </c>
     </row>
     <row r="80" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A80" s="44" t="s">
+      <c r="A80" s="1" t="s">
         <v>10</v>
       </c>
       <c r="C80" s="1"/>
     </row>
     <row r="81" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A81" s="44" t="s">
+      <c r="A81" s="1" t="s">
         <v>117</v>
       </c>
       <c r="C81" s="1" t="s">
@@ -3135,12 +3142,12 @@
       </c>
     </row>
     <row r="82" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A82" s="44" t="s">
+      <c r="A82" s="1" t="s">
         <v>6</v>
       </c>
     </row>
     <row r="83" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A83" s="44" t="s">
+      <c r="A83" s="1" t="s">
         <v>137</v>
       </c>
       <c r="B83" s="1" t="s">
@@ -3148,25 +3155,25 @@
       </c>
     </row>
     <row r="84" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A84" s="44" t="s">
+      <c r="A84" s="1" t="s">
         <v>6</v>
       </c>
     </row>
     <row r="85" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A85" s="44" t="s">
+      <c r="A85" s="1" t="s">
         <v>138</v>
       </c>
     </row>
     <row r="87" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A87" s="45" t="s">
-        <v>386</v>
+      <c r="A87" t="s">
+        <v>385</v>
       </c>
       <c r="B87" t="s">
         <v>373</v>
       </c>
     </row>
     <row r="88" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A88" s="44" t="s">
+      <c r="A88" s="1" t="s">
         <v>143</v>
       </c>
       <c r="B88" s="1" t="s">
@@ -3174,7 +3181,7 @@
       </c>
     </row>
     <row r="89" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A89" s="44" t="s">
+      <c r="A89" s="1" t="s">
         <v>107</v>
       </c>
       <c r="B89" t="s">
@@ -3182,7 +3189,7 @@
       </c>
     </row>
     <row r="90" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A90" s="44" t="s">
+      <c r="A90" s="1" t="s">
         <v>108</v>
       </c>
       <c r="B90" t="s">
@@ -3190,7 +3197,7 @@
       </c>
     </row>
     <row r="91" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A91" s="44" t="s">
+      <c r="A91" s="1" t="s">
         <v>109</v>
       </c>
       <c r="B91" t="s">
@@ -3198,7 +3205,7 @@
       </c>
     </row>
     <row r="92" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A92" s="44" t="s">
+      <c r="A92" s="1" t="s">
         <v>278</v>
       </c>
       <c r="B92" t="s">
@@ -3206,18 +3213,18 @@
       </c>
     </row>
     <row r="93" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A93" s="44" t="s">
+      <c r="A93" s="1" t="s">
         <v>113</v>
       </c>
       <c r="B93" t="s">
         <v>277</v>
       </c>
       <c r="C93" t="s">
-        <v>384</v>
+        <v>383</v>
       </c>
     </row>
     <row r="94" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A94" s="44" t="s">
+      <c r="A94" s="1" t="s">
         <v>141</v>
       </c>
       <c r="B94" t="s">
@@ -3225,7 +3232,7 @@
       </c>
     </row>
     <row r="95" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A95" s="44" t="s">
+      <c r="A95" s="1" t="s">
         <v>142</v>
       </c>
       <c r="B95" t="s">
@@ -3233,7 +3240,7 @@
       </c>
     </row>
     <row r="96" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A96" s="44" t="s">
+      <c r="A96" s="1" t="s">
         <v>144</v>
       </c>
       <c r="B96" t="s">
@@ -3244,7 +3251,7 @@
       </c>
     </row>
     <row r="97" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A97" s="44" t="s">
+      <c r="A97" s="1" t="s">
         <v>145</v>
       </c>
       <c r="B97" t="s">
@@ -3252,29 +3259,29 @@
       </c>
     </row>
     <row r="98" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A98" s="44" t="s">
+      <c r="A98" s="1" t="s">
         <v>146</v>
       </c>
       <c r="B98" t="s">
         <v>275</v>
       </c>
       <c r="C98" t="s">
+        <v>387</v>
+      </c>
+      <c r="D98" t="s">
+        <v>386</v>
+      </c>
+    </row>
+    <row r="99" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A99" s="1" t="s">
+        <v>147</v>
+      </c>
+      <c r="B99" t="s">
         <v>388</v>
       </c>
-      <c r="D98" t="s">
-        <v>387</v>
-      </c>
-    </row>
-    <row r="99" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A99" s="44" t="s">
-        <v>147</v>
-      </c>
-      <c r="B99" t="s">
-        <v>389</v>
-      </c>
     </row>
     <row r="100" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A100" s="44" t="s">
+      <c r="A100" s="1" t="s">
         <v>363</v>
       </c>
       <c r="B100" t="s">
@@ -3282,7 +3289,7 @@
       </c>
     </row>
     <row r="101" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A101" s="44" t="s">
+      <c r="A101" s="1" t="s">
         <v>148</v>
       </c>
       <c r="B101" t="s">
@@ -3290,7 +3297,7 @@
       </c>
     </row>
     <row r="102" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A102" s="44" t="s">
+      <c r="A102" s="1" t="s">
         <v>151</v>
       </c>
       <c r="B102" t="s">
@@ -3298,7 +3305,7 @@
       </c>
     </row>
     <row r="103" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A103" s="44" t="s">
+      <c r="A103" s="1" t="s">
         <v>274</v>
       </c>
       <c r="B103" t="s">
@@ -3306,7 +3313,7 @@
       </c>
     </row>
     <row r="104" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A104" s="44" t="s">
+      <c r="A104" s="1" t="s">
         <v>360</v>
       </c>
       <c r="B104" t="s">
@@ -3317,7 +3324,7 @@
       </c>
     </row>
     <row r="105" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A105" s="44" t="s">
+      <c r="A105" s="1" t="s">
         <v>362</v>
       </c>
       <c r="B105" t="s">
@@ -3325,7 +3332,7 @@
       </c>
     </row>
     <row r="106" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A106" s="44" t="s">
+      <c r="A106" s="1" t="s">
         <v>364</v>
       </c>
       <c r="B106" t="s">
@@ -3333,7 +3340,7 @@
       </c>
     </row>
     <row r="107" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A107" s="44" t="s">
+      <c r="A107" s="1" t="s">
         <v>376</v>
       </c>
       <c r="B107" s="31" t="s">
@@ -3341,74 +3348,77 @@
       </c>
     </row>
     <row r="108" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A108" s="44" t="s">
+      <c r="A108" s="1" t="s">
         <v>377</v>
       </c>
-      <c r="B108" s="31" t="s">
+      <c r="B108" t="s">
+        <v>275</v>
+      </c>
+      <c r="C108" t="s">
+        <v>389</v>
+      </c>
+    </row>
+    <row r="109" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A109" s="1" t="s">
         <v>378</v>
       </c>
-    </row>
-    <row r="109" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A109" s="44" t="s">
+      <c r="B109" s="31" t="s">
         <v>379</v>
       </c>
-      <c r="B109" s="31" t="s">
+      <c r="C109" t="s">
         <v>380</v>
       </c>
-      <c r="C109" t="s">
+    </row>
+    <row r="110" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A110" s="1" t="s">
         <v>381</v>
       </c>
-    </row>
-    <row r="110" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A110" s="44" t="s">
+      <c r="B110" s="31" t="s">
         <v>382</v>
       </c>
-      <c r="B110" s="31" t="s">
-        <v>383</v>
-      </c>
     </row>
     <row r="112" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A112" s="37" t="s">
+      <c r="A112" s="34" t="s">
         <v>18</v>
       </c>
     </row>
     <row r="113" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A113" s="37" t="s">
+      <c r="A113" s="34" t="s">
         <v>19</v>
       </c>
     </row>
     <row r="114" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A114" s="37" t="s">
+      <c r="A114" s="34" t="s">
         <v>86</v>
       </c>
     </row>
     <row r="115" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A115" s="37" t="s">
+      <c r="A115" s="34" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="116" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A116" s="37" t="s">
+      <c r="A116" s="34" t="s">
         <v>14</v>
       </c>
     </row>
     <row r="117" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A117" s="37" t="s">
+      <c r="A117" s="34" t="s">
         <v>15</v>
       </c>
     </row>
     <row r="118" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A118" s="37" t="s">
+      <c r="A118" s="34" t="s">
         <v>16</v>
       </c>
     </row>
     <row r="119" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A119" s="37" t="s">
+      <c r="A119" s="34" t="s">
         <v>75</v>
       </c>
     </row>
     <row r="120" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A120" s="37" t="s">
+      <c r="A120" s="34" t="s">
         <v>8</v>
       </c>
       <c r="C120" s="1" t="s">
@@ -3416,7 +3426,7 @@
       </c>
     </row>
     <row r="121" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A121" s="37" t="s">
+      <c r="A121" s="34" t="s">
         <v>9</v>
       </c>
       <c r="C121" s="1" t="s">
@@ -3424,27 +3434,27 @@
       </c>
     </row>
     <row r="122" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A122" s="37" t="s">
+      <c r="A122" s="34" t="s">
         <v>6</v>
       </c>
     </row>
     <row r="123" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A123" s="37" t="s">
+      <c r="A123" s="34" t="s">
         <v>12</v>
       </c>
     </row>
     <row r="124" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A124" s="37" t="s">
+      <c r="A124" s="34" t="s">
         <v>70</v>
       </c>
     </row>
     <row r="125" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A125" s="37" t="s">
+      <c r="A125" s="34" t="s">
         <v>71</v>
       </c>
     </row>
     <row r="126" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A126" s="37" t="s">
+      <c r="A126" s="34" t="s">
         <v>5</v>
       </c>
       <c r="C126" s="1" t="s">
@@ -3452,104 +3462,108 @@
       </c>
     </row>
     <row r="127" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A127" s="37" t="s">
+      <c r="A127" s="34" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="128" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A128" s="37" t="s">
+      <c r="A128" s="34" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="129" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A129" s="37" t="s">
+      <c r="A129" s="34" t="s">
         <v>2</v>
       </c>
     </row>
     <row r="130" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A130" s="37" t="s">
+      <c r="A130" s="34" t="s">
         <v>1</v>
       </c>
     </row>
     <row r="131" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A131" s="37" t="s">
+      <c r="A131" s="34" t="s">
         <v>20</v>
       </c>
     </row>
     <row r="132" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A132" s="37" t="s">
+      <c r="A132" s="34" t="s">
         <v>21</v>
       </c>
     </row>
     <row r="133" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A133" s="37" t="s">
+      <c r="A133" s="34" t="s">
         <v>22</v>
       </c>
     </row>
     <row r="134" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A134" s="37" t="s">
+      <c r="A134" s="34" t="s">
         <v>23</v>
       </c>
     </row>
     <row r="135" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A135" s="37" t="s">
+      <c r="A135" s="34" t="s">
         <v>13</v>
       </c>
     </row>
     <row r="136" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A136" s="37" t="s">
+      <c r="A136" s="34" t="s">
         <v>0</v>
       </c>
     </row>
     <row r="137" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A137" s="37" t="s">
+      <c r="A137" s="34" t="s">
         <v>27</v>
       </c>
     </row>
     <row r="138" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A138" s="37" t="s">
+      <c r="A138" s="34" t="s">
         <v>26</v>
       </c>
     </row>
     <row r="139" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A139" s="37" t="s">
+      <c r="A139" s="34" t="s">
         <v>25</v>
       </c>
     </row>
     <row r="140" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A140" s="37" t="s">
+      <c r="A140" s="34" t="s">
         <v>24</v>
       </c>
     </row>
     <row r="141" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A141" s="37" t="s">
+      <c r="A141" s="34" t="s">
         <v>72</v>
       </c>
     </row>
     <row r="142" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A142" s="38" t="s">
+      <c r="A142" s="35" t="s">
         <v>73</v>
       </c>
     </row>
   </sheetData>
   <conditionalFormatting sqref="A112:A142 A77 A72:A75 A1:A70">
-    <cfRule type="containsBlanks" dxfId="1" priority="2">
+    <cfRule type="containsBlanks" dxfId="2" priority="3">
       <formula>LEN(TRIM(A1))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A111:C1048576 A107:A110 C107:C110 D93:E93 A1:C106 D98">
+    <cfRule type="cellIs" dxfId="1" priority="2" operator="equal">
+      <formula>"done"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B108">
     <cfRule type="cellIs" dxfId="0" priority="1" operator="equal">
       <formula>"done"</formula>
     </cfRule>
   </conditionalFormatting>
   <hyperlinks>
     <hyperlink ref="B107" r:id="rId1" display="https://github.com/pret/pokecrystal/wiki/Improve-the-event-initialization-system" xr:uid="{318A9016-A758-473A-AA4B-FB01C0425045}"/>
-    <hyperlink ref="B108" r:id="rId2" display="https://github.com/pret/pokecrystal/wiki/Add-a-new-phone-contact" xr:uid="{F33E0623-0BFD-41C3-97E6-6AE8FB8AD1E9}"/>
-    <hyperlink ref="B109" r:id="rId3" display="https://github.com/pret/pokecrystal/wiki/Allow-Using-a-Field-Move-if-the-Pokemon-Can-Learn-It" xr:uid="{3F8458B1-E8F4-4DE2-BE47-0940B3D924E8}"/>
-    <hyperlink ref="B110" r:id="rId4" display="https://github.com/pret/pokecrystal/wiki/Add-spinner-tiles-from-Generation-I-Rocket-Hideout" xr:uid="{80CD41A4-ACA1-4FA9-8AC9-03FD67A0E2C8}"/>
+    <hyperlink ref="B109" r:id="rId2" display="https://github.com/pret/pokecrystal/wiki/Allow-Using-a-Field-Move-if-the-Pokemon-Can-Learn-It" xr:uid="{3F8458B1-E8F4-4DE2-BE47-0940B3D924E8}"/>
+    <hyperlink ref="B110" r:id="rId3" display="https://github.com/pret/pokecrystal/wiki/Add-spinner-tiles-from-Generation-I-Rocket-Hideout" xr:uid="{80CD41A4-ACA1-4FA9-8AC9-03FD67A0E2C8}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId5"/>
+  <pageSetup orientation="portrait" r:id="rId4"/>
 </worksheet>
 </file>
 
@@ -3587,30 +3601,30 @@
       </c>
     </row>
     <row r="2" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="C2" s="32" t="s">
+      <c r="C2" s="40" t="s">
         <v>163</v>
       </c>
-      <c r="D2" s="33"/>
-      <c r="E2" s="33"/>
-      <c r="F2" s="33"/>
-      <c r="G2" s="33"/>
-      <c r="H2" s="34"/>
-      <c r="I2" s="32" t="s">
+      <c r="D2" s="41"/>
+      <c r="E2" s="41"/>
+      <c r="F2" s="41"/>
+      <c r="G2" s="41"/>
+      <c r="H2" s="42"/>
+      <c r="I2" s="40" t="s">
         <v>164</v>
       </c>
-      <c r="J2" s="33"/>
-      <c r="K2" s="33"/>
-      <c r="L2" s="33"/>
-      <c r="M2" s="33"/>
-      <c r="N2" s="34"/>
-      <c r="O2" s="32" t="s">
+      <c r="J2" s="41"/>
+      <c r="K2" s="41"/>
+      <c r="L2" s="41"/>
+      <c r="M2" s="41"/>
+      <c r="N2" s="42"/>
+      <c r="O2" s="40" t="s">
         <v>165</v>
       </c>
-      <c r="P2" s="33"/>
-      <c r="Q2" s="33"/>
-      <c r="R2" s="33"/>
-      <c r="S2" s="33"/>
-      <c r="T2" s="34"/>
+      <c r="P2" s="41"/>
+      <c r="Q2" s="41"/>
+      <c r="R2" s="41"/>
+      <c r="S2" s="41"/>
+      <c r="T2" s="42"/>
     </row>
     <row r="3" spans="1:20" ht="13" x14ac:dyDescent="0.3">
       <c r="A3" t="s">

</xml_diff>

<commit_message>
added dragon den team for rival and added fish sprite from crystal clear
</commit_message>
<xml_diff>
--- a/Silver_Todo.xlsx
+++ b/Silver_Todo.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\dwg11\Silver\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FEBB6DFB-181A-423F-9442-FBF177D6088A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8875C76E-E516-4A53-9A80-6BB17C648597}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="25820" windowHeight="15500" tabRatio="788" firstSheet="1" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25690" windowHeight="15280" tabRatio="788" firstSheet="1" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Overview and Credits" sheetId="2" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="791" uniqueCount="390">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="891" uniqueCount="394">
   <si>
     <t>Pallet Town</t>
   </si>
@@ -794,9 +794,6 @@
     <t>Curse</t>
   </si>
   <si>
-    <t>Moves only</t>
-  </si>
-  <si>
     <t>Sleep Powder</t>
   </si>
   <si>
@@ -866,9 +863,6 @@
     <t>done</t>
   </si>
   <si>
-    <t>tutorial</t>
-  </si>
-  <si>
     <t>cribxtal</t>
   </si>
   <si>
@@ -1181,9 +1175,6 @@
     <t>add full HM compatibility to starters</t>
   </si>
   <si>
-    <t>spinner tiles?</t>
-  </si>
-  <si>
     <t>Add spinner tiles from Generation I Rocket Hideout · pret/pokecrystal Wiki (github.com)</t>
   </si>
   <si>
@@ -1202,10 +1193,31 @@
     <t>Giovanni gives to player?</t>
   </si>
   <si>
-    <t>scraped from crystal clear, in newsprites</t>
-  </si>
-  <si>
     <t>need to give the number and code for the phone calls player receives</t>
+  </si>
+  <si>
+    <t>fixed by one of the branches?</t>
+  </si>
+  <si>
+    <t>from crystal clear</t>
+  </si>
+  <si>
+    <t>from youtube/hgss dialogue</t>
+  </si>
+  <si>
+    <t>spinner tiles, if silph map is redone</t>
+  </si>
+  <si>
+    <t>Extremespeed</t>
+  </si>
+  <si>
+    <t>Hyper Beam</t>
+  </si>
+  <si>
+    <t>Perish Song</t>
+  </si>
+  <si>
+    <t>buff these levels?</t>
   </si>
 </sst>
 </file>
@@ -1328,7 +1340,7 @@
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -1338,6 +1350,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="2" tint="-0.14999847407452621"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0" tint="-0.14999847407452621"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1410,7 +1428,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="43">
+  <cellXfs count="45">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -1508,6 +1526,8 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -2600,8 +2620,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4D4D23E0-802A-4842-9CD9-587C61A270C2}">
   <dimension ref="A1:E142"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A76" workbookViewId="0">
-      <selection activeCell="B88" sqref="B88"/>
+    <sheetView topLeftCell="A50" workbookViewId="0">
+      <selection activeCell="B1" sqref="B1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
@@ -2669,7 +2689,7 @@
         <v>32</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.25">
@@ -2683,7 +2703,7 @@
         <v>34</v>
       </c>
       <c r="C10" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.25">
@@ -2700,7 +2720,7 @@
       </c>
       <c r="B12" s="1"/>
       <c r="C12" s="1" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.25">
@@ -2739,7 +2759,7 @@
         <v>41</v>
       </c>
       <c r="C18" s="1" t="s">
-        <v>282</v>
+        <v>280</v>
       </c>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.25">
@@ -2764,7 +2784,7 @@
         <v>44</v>
       </c>
       <c r="C21" s="1" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.25">
@@ -2787,7 +2807,7 @@
         <v>79</v>
       </c>
       <c r="C25" t="s">
-        <v>279</v>
+        <v>277</v>
       </c>
     </row>
     <row r="26" spans="1:5" x14ac:dyDescent="0.25">
@@ -2811,7 +2831,7 @@
         <v>68</v>
       </c>
       <c r="C28" s="1" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
     </row>
     <row r="29" spans="1:5" x14ac:dyDescent="0.25">
@@ -2881,7 +2901,7 @@
         <v>60</v>
       </c>
       <c r="C40" t="s">
-        <v>384</v>
+        <v>381</v>
       </c>
     </row>
     <row r="41" spans="1:3" x14ac:dyDescent="0.25">
@@ -2889,7 +2909,7 @@
         <v>61</v>
       </c>
       <c r="C41" t="s">
-        <v>280</v>
+        <v>278</v>
       </c>
     </row>
     <row r="42" spans="1:3" x14ac:dyDescent="0.25">
@@ -2899,10 +2919,10 @@
     </row>
     <row r="43" spans="1:3" ht="50" x14ac:dyDescent="0.25">
       <c r="A43" s="34" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
       <c r="C43" s="29" t="s">
-        <v>281</v>
+        <v>279</v>
       </c>
     </row>
     <row r="44" spans="1:3" x14ac:dyDescent="0.25">
@@ -2928,7 +2948,7 @@
         <v>65</v>
       </c>
       <c r="C47" t="s">
-        <v>361</v>
+        <v>359</v>
       </c>
     </row>
     <row r="48" spans="1:3" x14ac:dyDescent="0.25">
@@ -2964,7 +2984,7 @@
         <v>80</v>
       </c>
       <c r="C53" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
     </row>
     <row r="54" spans="1:3" ht="13" x14ac:dyDescent="0.25">
@@ -2988,7 +3008,7 @@
         <v>114</v>
       </c>
       <c r="C57" s="1" t="s">
-        <v>321</v>
+        <v>319</v>
       </c>
     </row>
     <row r="58" spans="1:3" x14ac:dyDescent="0.25">
@@ -3166,10 +3186,10 @@
     </row>
     <row r="87" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A87" t="s">
-        <v>385</v>
+        <v>382</v>
       </c>
       <c r="B87" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
     </row>
     <row r="88" spans="1:3" x14ac:dyDescent="0.25">
@@ -3177,7 +3197,7 @@
         <v>143</v>
       </c>
       <c r="B88" s="1" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
     </row>
     <row r="89" spans="1:3" x14ac:dyDescent="0.25">
@@ -3185,7 +3205,7 @@
         <v>107</v>
       </c>
       <c r="B89" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
     </row>
     <row r="90" spans="1:3" x14ac:dyDescent="0.25">
@@ -3193,7 +3213,7 @@
         <v>108</v>
       </c>
       <c r="B90" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
     </row>
     <row r="91" spans="1:3" x14ac:dyDescent="0.25">
@@ -3201,15 +3221,15 @@
         <v>109</v>
       </c>
       <c r="B91" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
     </row>
     <row r="92" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A92" s="1" t="s">
-        <v>278</v>
+        <v>276</v>
       </c>
       <c r="B92" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
     </row>
     <row r="93" spans="1:3" x14ac:dyDescent="0.25">
@@ -3217,10 +3237,10 @@
         <v>113</v>
       </c>
       <c r="B93" t="s">
-        <v>277</v>
+        <v>275</v>
       </c>
       <c r="C93" t="s">
-        <v>383</v>
+        <v>380</v>
       </c>
     </row>
     <row r="94" spans="1:3" x14ac:dyDescent="0.25">
@@ -3228,7 +3248,7 @@
         <v>141</v>
       </c>
       <c r="B94" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
     </row>
     <row r="95" spans="1:3" x14ac:dyDescent="0.25">
@@ -3236,7 +3256,10 @@
         <v>142</v>
       </c>
       <c r="B95" t="s">
-        <v>276</v>
+        <v>274</v>
+      </c>
+      <c r="C95" t="s">
+        <v>386</v>
       </c>
     </row>
     <row r="96" spans="1:3" x14ac:dyDescent="0.25">
@@ -3244,10 +3267,10 @@
         <v>144</v>
       </c>
       <c r="B96" t="s">
-        <v>372</v>
+        <v>370</v>
       </c>
       <c r="C96" t="s">
-        <v>371</v>
+        <v>369</v>
       </c>
     </row>
     <row r="97" spans="1:4" x14ac:dyDescent="0.25">
@@ -3255,7 +3278,7 @@
         <v>145</v>
       </c>
       <c r="B97" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
     </row>
     <row r="98" spans="1:4" x14ac:dyDescent="0.25">
@@ -3263,13 +3286,13 @@
         <v>146</v>
       </c>
       <c r="B98" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
       <c r="C98" t="s">
-        <v>387</v>
+        <v>384</v>
       </c>
       <c r="D98" t="s">
-        <v>386</v>
+        <v>383</v>
       </c>
     </row>
     <row r="99" spans="1:4" x14ac:dyDescent="0.25">
@@ -3277,15 +3300,18 @@
         <v>147</v>
       </c>
       <c r="B99" t="s">
-        <v>388</v>
+        <v>274</v>
+      </c>
+      <c r="C99" t="s">
+        <v>387</v>
       </c>
     </row>
     <row r="100" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A100" s="1" t="s">
-        <v>363</v>
+        <v>361</v>
       </c>
       <c r="B100" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
     </row>
     <row r="101" spans="1:4" x14ac:dyDescent="0.25">
@@ -3293,7 +3319,7 @@
         <v>148</v>
       </c>
       <c r="B101" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
     </row>
     <row r="102" spans="1:4" x14ac:dyDescent="0.25">
@@ -3301,80 +3327,83 @@
         <v>151</v>
       </c>
       <c r="B102" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
     </row>
     <row r="103" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A103" s="1" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
       <c r="B103" t="s">
-        <v>374</v>
+        <v>372</v>
       </c>
     </row>
     <row r="104" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A104" s="1" t="s">
-        <v>360</v>
+        <v>358</v>
       </c>
       <c r="B104" t="s">
-        <v>365</v>
+        <v>363</v>
       </c>
       <c r="C104" t="s">
-        <v>366</v>
+        <v>364</v>
       </c>
     </row>
     <row r="105" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A105" s="1" t="s">
-        <v>362</v>
+        <v>360</v>
       </c>
       <c r="B105" t="s">
-        <v>373</v>
+        <v>371</v>
+      </c>
+      <c r="C105" t="s">
+        <v>388</v>
       </c>
     </row>
     <row r="106" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A106" s="1" t="s">
-        <v>364</v>
+        <v>362</v>
       </c>
       <c r="B106" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
     </row>
     <row r="107" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A107" s="1" t="s">
-        <v>376</v>
+        <v>374</v>
       </c>
       <c r="B107" s="31" t="s">
-        <v>375</v>
+        <v>373</v>
       </c>
     </row>
     <row r="108" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A108" s="1" t="s">
-        <v>377</v>
+        <v>375</v>
       </c>
       <c r="B108" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
       <c r="C108" t="s">
-        <v>389</v>
+        <v>385</v>
       </c>
     </row>
     <row r="109" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A109" s="1" t="s">
+        <v>376</v>
+      </c>
+      <c r="B109" s="31" t="s">
+        <v>377</v>
+      </c>
+      <c r="C109" t="s">
         <v>378</v>
-      </c>
-      <c r="B109" s="31" t="s">
-        <v>379</v>
-      </c>
-      <c r="C109" t="s">
-        <v>380</v>
       </c>
     </row>
     <row r="110" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A110" s="1" t="s">
-        <v>381</v>
+        <v>389</v>
       </c>
       <c r="B110" s="31" t="s">
-        <v>382</v>
+        <v>379</v>
       </c>
     </row>
     <row r="112" spans="1:4" x14ac:dyDescent="0.25">
@@ -3571,9 +3600,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DB3E0C82-6EA9-4690-9C5F-8CA3CDECAC6B}">
   <dimension ref="A1:T39"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="A27" sqref="A27:A32"/>
+      <selection pane="topRight" activeCell="B22" sqref="B22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
@@ -3757,9 +3786,6 @@
       <c r="A6" t="s">
         <v>205</v>
       </c>
-      <c r="B6" t="s">
-        <v>252</v>
-      </c>
       <c r="C6">
         <v>12</v>
       </c>
@@ -3853,10 +3879,10 @@
         <v>174</v>
       </c>
       <c r="Q7" s="1" t="s">
+        <v>252</v>
+      </c>
+      <c r="R7" s="1" t="s">
         <v>253</v>
-      </c>
-      <c r="R7" s="1" t="s">
-        <v>254</v>
       </c>
       <c r="S7" s="1" t="s">
         <v>211</v>
@@ -4039,10 +4065,10 @@
         <v>174</v>
       </c>
       <c r="Q11" s="1" t="s">
+        <v>252</v>
+      </c>
+      <c r="R11" s="1" t="s">
         <v>253</v>
-      </c>
-      <c r="R11" s="1" t="s">
-        <v>254</v>
       </c>
       <c r="S11" s="1" t="s">
         <v>211</v>
@@ -4099,16 +4125,16 @@
         <v>181</v>
       </c>
       <c r="Q12" s="1" t="s">
+        <v>259</v>
+      </c>
+      <c r="R12" s="1" t="s">
         <v>260</v>
       </c>
-      <c r="R12" s="1" t="s">
+      <c r="S12" s="1" t="s">
         <v>261</v>
       </c>
-      <c r="S12" s="1" t="s">
+      <c r="T12" s="28" t="s">
         <v>262</v>
-      </c>
-      <c r="T12" s="28" t="s">
-        <v>263</v>
       </c>
     </row>
     <row r="13" spans="1:20" s="25" customFormat="1" x14ac:dyDescent="0.25">
@@ -4284,16 +4310,16 @@
         <v>188</v>
       </c>
       <c r="Q16" s="1" t="s">
+        <v>254</v>
+      </c>
+      <c r="R16" s="1" t="s">
         <v>255</v>
-      </c>
-      <c r="R16" s="1" t="s">
-        <v>256</v>
       </c>
       <c r="S16" s="1" t="s">
         <v>211</v>
       </c>
       <c r="T16" s="28" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
     </row>
     <row r="17" spans="1:20" x14ac:dyDescent="0.25">
@@ -4349,10 +4375,10 @@
         <v>235</v>
       </c>
       <c r="S17" s="1" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
       <c r="T17" s="28" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
     </row>
     <row r="18" spans="1:20" x14ac:dyDescent="0.25">
@@ -4485,6 +4511,9 @@
       <c r="A21" t="s">
         <v>207</v>
       </c>
+      <c r="B21" s="1" t="s">
+        <v>393</v>
+      </c>
       <c r="C21">
         <v>36</v>
       </c>
@@ -4587,16 +4616,16 @@
         <v>188</v>
       </c>
       <c r="Q22" s="1" t="s">
+        <v>254</v>
+      </c>
+      <c r="R22" s="1" t="s">
         <v>255</v>
-      </c>
-      <c r="R22" s="1" t="s">
-        <v>256</v>
       </c>
       <c r="S22" s="1" t="s">
         <v>211</v>
       </c>
       <c r="T22" s="28" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
     </row>
     <row r="23" spans="1:20" ht="12.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -4652,10 +4681,10 @@
         <v>235</v>
       </c>
       <c r="S23" s="1" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
       <c r="T23" s="28" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
     </row>
     <row r="24" spans="1:20" ht="12.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -4789,7 +4818,7 @@
         <v>137</v>
       </c>
       <c r="C27">
-        <v>45</v>
+        <v>47</v>
       </c>
       <c r="D27" s="1" t="s">
         <v>191</v>
@@ -4807,7 +4836,7 @@
         <v>160</v>
       </c>
       <c r="I27">
-        <v>45</v>
+        <v>47</v>
       </c>
       <c r="J27" s="1" t="s">
         <v>192</v>
@@ -4825,7 +4854,7 @@
         <v>220</v>
       </c>
       <c r="O27">
-        <v>45</v>
+        <v>47</v>
       </c>
       <c r="P27" s="1" t="s">
         <v>193</v>
@@ -4949,16 +4978,16 @@
         <v>188</v>
       </c>
       <c r="Q29" s="1" t="s">
+        <v>257</v>
+      </c>
+      <c r="R29" s="1" t="s">
         <v>258</v>
       </c>
-      <c r="R29" s="1" t="s">
-        <v>259</v>
-      </c>
       <c r="S29" s="1" t="s">
+        <v>255</v>
+      </c>
+      <c r="T29" s="28" t="s">
         <v>256</v>
-      </c>
-      <c r="T29" s="28" t="s">
-        <v>257</v>
       </c>
     </row>
     <row r="30" spans="1:20" x14ac:dyDescent="0.25">
@@ -4966,7 +4995,7 @@
         <v>229</v>
       </c>
       <c r="C30">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="D30" t="s">
         <v>183</v>
@@ -4984,7 +5013,7 @@
         <v>235</v>
       </c>
       <c r="I30">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="J30" t="s">
         <v>184</v>
@@ -5002,19 +5031,19 @@
         <v>233</v>
       </c>
       <c r="O30">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="P30" t="s">
         <v>185</v>
       </c>
       <c r="Q30" s="1" t="s">
+        <v>264</v>
+      </c>
+      <c r="R30" s="1" t="s">
         <v>265</v>
       </c>
-      <c r="R30" s="1" t="s">
-        <v>266</v>
-      </c>
       <c r="S30" s="1" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
       <c r="T30" s="28" t="s">
         <v>219</v>
@@ -5087,10 +5116,10 @@
         <v>45</v>
       </c>
       <c r="D32" t="s">
-        <v>190</v>
-      </c>
-      <c r="E32" t="s">
-        <v>187</v>
+        <v>152</v>
+      </c>
+      <c r="E32" s="1" t="s">
+        <v>390</v>
       </c>
       <c r="F32" t="s">
         <v>195</v>
@@ -5105,10 +5134,10 @@
         <v>45</v>
       </c>
       <c r="J32" t="s">
-        <v>190</v>
-      </c>
-      <c r="K32" t="s">
-        <v>187</v>
+        <v>152</v>
+      </c>
+      <c r="K32" s="1" t="s">
+        <v>390</v>
       </c>
       <c r="L32" t="s">
         <v>195</v>
@@ -5123,10 +5152,10 @@
         <v>45</v>
       </c>
       <c r="P32" t="s">
-        <v>190</v>
-      </c>
-      <c r="Q32" t="s">
-        <v>187</v>
+        <v>152</v>
+      </c>
+      <c r="Q32" s="1" t="s">
+        <v>390</v>
       </c>
       <c r="R32" t="s">
         <v>195</v>
@@ -5138,13 +5167,368 @@
         <v>251</v>
       </c>
     </row>
-    <row r="33" ht="12.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="34" ht="12.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="35" ht="12.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="36" ht="12.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="37" ht="12.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="38" ht="12.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="39" ht="27.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="33" spans="1:20" s="44" customFormat="1" ht="12.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="H33" s="43"/>
+      <c r="N33" s="43"/>
+      <c r="T33" s="43"/>
+    </row>
+    <row r="34" spans="1:20" ht="12.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A34" t="s">
+        <v>204</v>
+      </c>
+      <c r="B34" s="13" t="s">
+        <v>65</v>
+      </c>
+      <c r="C34">
+        <v>55</v>
+      </c>
+      <c r="D34" s="1" t="s">
+        <v>191</v>
+      </c>
+      <c r="E34" s="1" t="s">
+        <v>176</v>
+      </c>
+      <c r="F34" s="1" t="s">
+        <v>224</v>
+      </c>
+      <c r="G34" s="1" t="s">
+        <v>158</v>
+      </c>
+      <c r="H34" s="28" t="s">
+        <v>160</v>
+      </c>
+      <c r="I34">
+        <v>55</v>
+      </c>
+      <c r="J34" s="1" t="s">
+        <v>192</v>
+      </c>
+      <c r="K34" t="s">
+        <v>176</v>
+      </c>
+      <c r="L34" s="1" t="s">
+        <v>219</v>
+      </c>
+      <c r="M34" s="1" t="s">
+        <v>221</v>
+      </c>
+      <c r="N34" s="28" t="s">
+        <v>220</v>
+      </c>
+      <c r="O34">
+        <v>55</v>
+      </c>
+      <c r="P34" s="1" t="s">
+        <v>193</v>
+      </c>
+      <c r="Q34" s="1" t="s">
+        <v>176</v>
+      </c>
+      <c r="R34" s="1" t="s">
+        <v>224</v>
+      </c>
+      <c r="S34" s="1" t="s">
+        <v>220</v>
+      </c>
+      <c r="T34" s="28" t="s">
+        <v>222</v>
+      </c>
+    </row>
+    <row r="35" spans="1:20" ht="12.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A35" t="s">
+        <v>228</v>
+      </c>
+      <c r="C35">
+        <v>50</v>
+      </c>
+      <c r="D35" t="s">
+        <v>177</v>
+      </c>
+      <c r="E35" t="s">
+        <v>176</v>
+      </c>
+      <c r="F35" t="s">
+        <v>216</v>
+      </c>
+      <c r="G35" t="s">
+        <v>196</v>
+      </c>
+      <c r="H35" s="28" t="s">
+        <v>217</v>
+      </c>
+      <c r="I35">
+        <v>50</v>
+      </c>
+      <c r="J35" t="s">
+        <v>177</v>
+      </c>
+      <c r="K35" t="s">
+        <v>176</v>
+      </c>
+      <c r="L35" t="s">
+        <v>216</v>
+      </c>
+      <c r="M35" t="s">
+        <v>196</v>
+      </c>
+      <c r="N35" s="28" t="s">
+        <v>217</v>
+      </c>
+      <c r="O35">
+        <v>50</v>
+      </c>
+      <c r="P35" t="s">
+        <v>177</v>
+      </c>
+      <c r="Q35" t="s">
+        <v>176</v>
+      </c>
+      <c r="R35" t="s">
+        <v>216</v>
+      </c>
+      <c r="S35" t="s">
+        <v>196</v>
+      </c>
+      <c r="T35" s="28" t="s">
+        <v>217</v>
+      </c>
+    </row>
+    <row r="36" spans="1:20" ht="12.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A36" s="1" t="s">
+        <v>317</v>
+      </c>
+      <c r="C36">
+        <v>50</v>
+      </c>
+      <c r="D36" t="s">
+        <v>189</v>
+      </c>
+      <c r="E36" t="s">
+        <v>200</v>
+      </c>
+      <c r="F36" s="1" t="s">
+        <v>390</v>
+      </c>
+      <c r="G36" t="s">
+        <v>162</v>
+      </c>
+      <c r="H36" s="26" t="s">
+        <v>232</v>
+      </c>
+      <c r="I36">
+        <v>50</v>
+      </c>
+      <c r="J36" t="s">
+        <v>179</v>
+      </c>
+      <c r="K36" s="1" t="s">
+        <v>244</v>
+      </c>
+      <c r="L36" s="1" t="s">
+        <v>161</v>
+      </c>
+      <c r="M36" s="1" t="s">
+        <v>155</v>
+      </c>
+      <c r="N36" s="28" t="s">
+        <v>232</v>
+      </c>
+      <c r="O36">
+        <v>50</v>
+      </c>
+      <c r="P36" t="s">
+        <v>188</v>
+      </c>
+      <c r="Q36" s="1" t="s">
+        <v>257</v>
+      </c>
+      <c r="R36" s="1" t="s">
+        <v>258</v>
+      </c>
+      <c r="S36" s="1" t="s">
+        <v>255</v>
+      </c>
+      <c r="T36" s="28" t="s">
+        <v>256</v>
+      </c>
+    </row>
+    <row r="37" spans="1:20" ht="12.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A37" t="s">
+        <v>229</v>
+      </c>
+      <c r="C37">
+        <v>52</v>
+      </c>
+      <c r="D37" t="s">
+        <v>183</v>
+      </c>
+      <c r="E37" t="s">
+        <v>159</v>
+      </c>
+      <c r="F37" t="s">
+        <v>236</v>
+      </c>
+      <c r="G37" t="s">
+        <v>234</v>
+      </c>
+      <c r="H37" s="26" t="s">
+        <v>235</v>
+      </c>
+      <c r="I37">
+        <v>52</v>
+      </c>
+      <c r="J37" t="s">
+        <v>184</v>
+      </c>
+      <c r="K37" s="1" t="s">
+        <v>222</v>
+      </c>
+      <c r="L37" s="1" t="s">
+        <v>235</v>
+      </c>
+      <c r="M37" s="1" t="s">
+        <v>247</v>
+      </c>
+      <c r="N37" s="28" t="s">
+        <v>233</v>
+      </c>
+      <c r="O37">
+        <v>52</v>
+      </c>
+      <c r="P37" t="s">
+        <v>185</v>
+      </c>
+      <c r="Q37" s="1" t="s">
+        <v>264</v>
+      </c>
+      <c r="R37" s="1" t="s">
+        <v>265</v>
+      </c>
+      <c r="S37" s="1" t="s">
+        <v>261</v>
+      </c>
+      <c r="T37" s="28" t="s">
+        <v>392</v>
+      </c>
+    </row>
+    <row r="38" spans="1:20" ht="12.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A38" t="s">
+        <v>226</v>
+      </c>
+      <c r="C38">
+        <v>50</v>
+      </c>
+      <c r="D38" t="s">
+        <v>154</v>
+      </c>
+      <c r="E38" t="s">
+        <v>155</v>
+      </c>
+      <c r="F38" t="s">
+        <v>186</v>
+      </c>
+      <c r="G38" s="1" t="s">
+        <v>391</v>
+      </c>
+      <c r="H38" s="26" t="s">
+        <v>238</v>
+      </c>
+      <c r="I38">
+        <v>50</v>
+      </c>
+      <c r="J38" t="s">
+        <v>154</v>
+      </c>
+      <c r="K38" s="1" t="s">
+        <v>239</v>
+      </c>
+      <c r="L38" t="s">
+        <v>186</v>
+      </c>
+      <c r="M38" s="1" t="s">
+        <v>391</v>
+      </c>
+      <c r="N38" s="26" t="s">
+        <v>238</v>
+      </c>
+      <c r="O38">
+        <v>50</v>
+      </c>
+      <c r="P38" t="s">
+        <v>154</v>
+      </c>
+      <c r="Q38" t="s">
+        <v>155</v>
+      </c>
+      <c r="R38" t="s">
+        <v>186</v>
+      </c>
+      <c r="S38" s="1" t="s">
+        <v>391</v>
+      </c>
+      <c r="T38" s="26" t="s">
+        <v>238</v>
+      </c>
+    </row>
+    <row r="39" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A39" t="s">
+        <v>231</v>
+      </c>
+      <c r="C39">
+        <v>55</v>
+      </c>
+      <c r="D39" t="s">
+        <v>190</v>
+      </c>
+      <c r="E39" s="1" t="s">
+        <v>390</v>
+      </c>
+      <c r="F39" t="s">
+        <v>195</v>
+      </c>
+      <c r="G39" t="s">
+        <v>248</v>
+      </c>
+      <c r="H39" s="28" t="s">
+        <v>251</v>
+      </c>
+      <c r="I39">
+        <v>55</v>
+      </c>
+      <c r="J39" t="s">
+        <v>190</v>
+      </c>
+      <c r="K39" s="1" t="s">
+        <v>390</v>
+      </c>
+      <c r="L39" t="s">
+        <v>195</v>
+      </c>
+      <c r="M39" t="s">
+        <v>248</v>
+      </c>
+      <c r="N39" s="28" t="s">
+        <v>251</v>
+      </c>
+      <c r="O39">
+        <v>55</v>
+      </c>
+      <c r="P39" t="s">
+        <v>190</v>
+      </c>
+      <c r="Q39" s="1" t="s">
+        <v>390</v>
+      </c>
+      <c r="R39" t="s">
+        <v>195</v>
+      </c>
+      <c r="S39" t="s">
+        <v>248</v>
+      </c>
+      <c r="T39" s="28" t="s">
+        <v>251</v>
+      </c>
+    </row>
   </sheetData>
   <mergeCells count="3">
     <mergeCell ref="C2:H2"/>
@@ -5172,7 +5556,7 @@
   <sheetData>
     <row r="1" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>283</v>
+        <v>281</v>
       </c>
     </row>
     <row r="3" spans="1:11" ht="13" x14ac:dyDescent="0.3">
@@ -5183,16 +5567,16 @@
         <v>12</v>
       </c>
       <c r="C3" t="s">
-        <v>284</v>
+        <v>282</v>
       </c>
       <c r="D3" t="s">
-        <v>292</v>
+        <v>290</v>
       </c>
       <c r="E3" t="s">
         <v>157</v>
       </c>
       <c r="F3" t="s">
-        <v>293</v>
+        <v>291</v>
       </c>
       <c r="G3" s="13"/>
       <c r="K3" t="s">
@@ -5204,13 +5588,13 @@
         <v>12</v>
       </c>
       <c r="C4" t="s">
-        <v>285</v>
+        <v>283</v>
       </c>
       <c r="D4" t="s">
-        <v>295</v>
+        <v>293</v>
       </c>
       <c r="E4" t="s">
-        <v>294</v>
+        <v>292</v>
       </c>
       <c r="K4" t="s">
         <v>205</v>
@@ -5221,19 +5605,19 @@
         <v>11</v>
       </c>
       <c r="C5" t="s">
+        <v>301</v>
+      </c>
+      <c r="D5" t="s">
         <v>303</v>
       </c>
-      <c r="D5" t="s">
+      <c r="E5" t="s">
+        <v>304</v>
+      </c>
+      <c r="F5" t="s">
         <v>305</v>
       </c>
-      <c r="E5" t="s">
+      <c r="G5" t="s">
         <v>306</v>
-      </c>
-      <c r="F5" t="s">
-        <v>307</v>
-      </c>
-      <c r="G5" t="s">
-        <v>308</v>
       </c>
       <c r="K5" t="s">
         <v>206</v>
@@ -5247,19 +5631,19 @@
         <v>23</v>
       </c>
       <c r="C7" t="s">
-        <v>287</v>
+        <v>285</v>
       </c>
       <c r="D7" t="s">
-        <v>291</v>
+        <v>289</v>
       </c>
       <c r="E7" t="s">
         <v>200</v>
       </c>
       <c r="F7" t="s">
-        <v>292</v>
+        <v>290</v>
       </c>
       <c r="G7" t="s">
-        <v>293</v>
+        <v>291</v>
       </c>
       <c r="K7" t="s">
         <v>204</v>
@@ -5270,19 +5654,19 @@
         <v>23</v>
       </c>
       <c r="C8" t="s">
-        <v>288</v>
+        <v>286</v>
       </c>
       <c r="D8" t="s">
+        <v>292</v>
+      </c>
+      <c r="E8" t="s">
+        <v>299</v>
+      </c>
+      <c r="F8" t="s">
         <v>294</v>
       </c>
-      <c r="E8" t="s">
-        <v>301</v>
-      </c>
-      <c r="F8" t="s">
-        <v>296</v>
-      </c>
       <c r="G8" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="K8" t="s">
         <v>207</v>
@@ -5293,19 +5677,19 @@
         <v>25</v>
       </c>
       <c r="C9" t="s">
-        <v>286</v>
+        <v>284</v>
       </c>
       <c r="D9" t="s">
+        <v>295</v>
+      </c>
+      <c r="E9" t="s">
+        <v>296</v>
+      </c>
+      <c r="F9" t="s">
         <v>297</v>
       </c>
-      <c r="E9" t="s">
+      <c r="G9" t="s">
         <v>298</v>
-      </c>
-      <c r="F9" t="s">
-        <v>299</v>
-      </c>
-      <c r="G9" t="s">
-        <v>300</v>
       </c>
       <c r="K9" s="1" t="s">
         <v>230</v>
@@ -5316,16 +5700,16 @@
         <v>25</v>
       </c>
       <c r="C10" t="s">
-        <v>303</v>
+        <v>301</v>
       </c>
       <c r="D10" t="s">
-        <v>309</v>
+        <v>307</v>
       </c>
       <c r="E10" t="s">
-        <v>310</v>
+        <v>308</v>
       </c>
       <c r="F10" t="s">
-        <v>306</v>
+        <v>304</v>
       </c>
       <c r="G10" t="s">
         <v>243</v>
@@ -5336,25 +5720,25 @@
     </row>
     <row r="12" spans="1:11" ht="13" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
-        <v>289</v>
+        <v>287</v>
       </c>
       <c r="B12">
         <v>32</v>
       </c>
       <c r="C12" t="s">
-        <v>287</v>
+        <v>285</v>
       </c>
       <c r="D12" t="s">
-        <v>291</v>
+        <v>289</v>
       </c>
       <c r="E12" s="13" t="s">
-        <v>311</v>
+        <v>309</v>
       </c>
       <c r="F12" s="13" t="s">
         <v>236</v>
       </c>
       <c r="G12" t="s">
-        <v>293</v>
+        <v>291</v>
       </c>
       <c r="K12" t="s">
         <v>204</v>
@@ -5365,19 +5749,19 @@
         <v>32</v>
       </c>
       <c r="C13" t="s">
-        <v>290</v>
+        <v>288</v>
       </c>
       <c r="D13" s="13" t="s">
-        <v>331</v>
+        <v>329</v>
       </c>
       <c r="E13" s="13" t="s">
-        <v>339</v>
+        <v>337</v>
       </c>
       <c r="F13" t="s">
-        <v>296</v>
+        <v>294</v>
       </c>
       <c r="G13" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="K13" t="s">
         <v>207</v>
@@ -5388,19 +5772,19 @@
         <v>32</v>
       </c>
       <c r="C14" t="s">
-        <v>286</v>
+        <v>284</v>
       </c>
       <c r="D14" s="13" t="s">
-        <v>302</v>
+        <v>300</v>
       </c>
       <c r="E14" t="s">
+        <v>296</v>
+      </c>
+      <c r="F14" s="13" t="s">
+        <v>345</v>
+      </c>
+      <c r="G14" t="s">
         <v>298</v>
-      </c>
-      <c r="F14" s="13" t="s">
-        <v>347</v>
-      </c>
-      <c r="G14" t="s">
-        <v>300</v>
       </c>
       <c r="K14" s="1" t="s">
         <v>230</v>
@@ -5411,13 +5795,13 @@
         <v>32</v>
       </c>
       <c r="C15" t="s">
-        <v>304</v>
+        <v>302</v>
       </c>
       <c r="D15" t="s">
-        <v>309</v>
+        <v>307</v>
       </c>
       <c r="E15" t="s">
-        <v>310</v>
+        <v>308</v>
       </c>
       <c r="F15" t="s">
         <v>236</v>
@@ -5436,24 +5820,24 @@
     </row>
     <row r="17" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A17" s="1" t="s">
-        <v>335</v>
+        <v>333</v>
       </c>
     </row>
     <row r="19" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A19" s="1" t="s">
-        <v>326</v>
+        <v>324</v>
       </c>
       <c r="B19">
         <v>50</v>
       </c>
       <c r="C19" s="1" t="s">
-        <v>323</v>
+        <v>321</v>
       </c>
       <c r="D19" s="1" t="s">
-        <v>336</v>
+        <v>334</v>
       </c>
       <c r="E19" s="1" t="s">
-        <v>337</v>
+        <v>335</v>
       </c>
       <c r="F19" s="1" t="s">
         <v>237</v>
@@ -5470,19 +5854,19 @@
         <v>48</v>
       </c>
       <c r="C20" s="1" t="s">
-        <v>324</v>
+        <v>322</v>
       </c>
       <c r="D20" s="1" t="s">
-        <v>338</v>
+        <v>336</v>
       </c>
       <c r="E20" s="1" t="s">
-        <v>294</v>
+        <v>292</v>
       </c>
       <c r="F20" s="1" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
       <c r="G20" s="13" t="s">
-        <v>339</v>
+        <v>337</v>
       </c>
       <c r="K20" t="s">
         <v>228</v>
@@ -5493,19 +5877,19 @@
         <v>48</v>
       </c>
       <c r="C21" s="1" t="s">
-        <v>325</v>
+        <v>323</v>
       </c>
       <c r="D21" s="13" t="s">
-        <v>331</v>
+        <v>329</v>
       </c>
       <c r="E21" s="1" t="s">
-        <v>340</v>
+        <v>338</v>
       </c>
       <c r="F21" s="1" t="s">
-        <v>341</v>
+        <v>339</v>
       </c>
       <c r="G21" s="1" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="K21" t="s">
         <v>230</v>
@@ -5516,19 +5900,19 @@
         <v>52</v>
       </c>
       <c r="C22" s="1" t="s">
-        <v>316</v>
+        <v>314</v>
       </c>
       <c r="D22" s="1" t="s">
         <v>235</v>
       </c>
       <c r="E22" s="1" t="s">
-        <v>342</v>
+        <v>340</v>
       </c>
       <c r="F22" s="1" t="s">
         <v>200</v>
       </c>
       <c r="G22" s="1" t="s">
-        <v>343</v>
+        <v>341</v>
       </c>
       <c r="K22" t="s">
         <v>229</v>
@@ -5539,19 +5923,19 @@
         <v>48</v>
       </c>
       <c r="C23" s="1" t="s">
-        <v>332</v>
+        <v>330</v>
       </c>
       <c r="D23" s="1" t="s">
-        <v>331</v>
+        <v>329</v>
       </c>
       <c r="E23" s="1" t="s">
-        <v>344</v>
+        <v>342</v>
       </c>
       <c r="F23" s="1" t="s">
-        <v>345</v>
+        <v>343</v>
       </c>
       <c r="G23" s="1" t="s">
-        <v>370</v>
+        <v>368</v>
       </c>
       <c r="K23" t="s">
         <v>226</v>
@@ -5565,16 +5949,16 @@
     </row>
     <row r="26" spans="1:11" ht="13" x14ac:dyDescent="0.3">
       <c r="A26" s="1" t="s">
-        <v>333</v>
+        <v>331</v>
       </c>
       <c r="B26">
         <v>54</v>
       </c>
       <c r="C26" s="1" t="s">
-        <v>318</v>
+        <v>316</v>
       </c>
       <c r="D26" s="13" t="s">
-        <v>311</v>
+        <v>309</v>
       </c>
       <c r="E26" s="13" t="s">
         <v>222</v>
@@ -5594,19 +5978,19 @@
         <v>54</v>
       </c>
       <c r="C27" s="1" t="s">
-        <v>319</v>
+        <v>317</v>
       </c>
       <c r="D27" s="13" t="s">
         <v>153</v>
       </c>
       <c r="E27" s="13" t="s">
+        <v>345</v>
+      </c>
+      <c r="F27" s="1" t="s">
         <v>347</v>
       </c>
-      <c r="F27" s="1" t="s">
-        <v>349</v>
-      </c>
       <c r="G27" s="1" t="s">
-        <v>348</v>
+        <v>346</v>
       </c>
       <c r="K27" t="s">
         <v>228</v>
@@ -5617,13 +6001,13 @@
         <v>54</v>
       </c>
       <c r="C28" s="1" t="s">
-        <v>320</v>
+        <v>318</v>
       </c>
       <c r="D28" s="13" t="s">
-        <v>299</v>
+        <v>297</v>
       </c>
       <c r="E28" s="1" t="s">
-        <v>334</v>
+        <v>332</v>
       </c>
       <c r="F28" s="1" t="s">
         <v>202</v>
@@ -5640,19 +6024,19 @@
         <v>56</v>
       </c>
       <c r="C29" s="1" t="s">
+        <v>326</v>
+      </c>
+      <c r="D29" s="1" t="s">
+        <v>327</v>
+      </c>
+      <c r="E29" s="1" t="s">
         <v>328</v>
       </c>
-      <c r="D29" s="1" t="s">
-        <v>329</v>
-      </c>
-      <c r="E29" s="1" t="s">
-        <v>330</v>
-      </c>
       <c r="F29" s="1" t="s">
-        <v>350</v>
+        <v>348</v>
       </c>
       <c r="G29" s="1" t="s">
-        <v>351</v>
+        <v>349</v>
       </c>
       <c r="K29" t="s">
         <v>229</v>
@@ -5663,13 +6047,13 @@
         <v>58</v>
       </c>
       <c r="C30" s="1" t="s">
-        <v>327</v>
+        <v>325</v>
       </c>
       <c r="D30" s="1" t="s">
-        <v>352</v>
+        <v>350</v>
       </c>
       <c r="E30" s="1" t="s">
-        <v>353</v>
+        <v>351</v>
       </c>
       <c r="F30" s="1" t="s">
         <v>245</v>
@@ -5694,10 +6078,10 @@
         <v>66</v>
       </c>
       <c r="C33" t="s">
-        <v>312</v>
+        <v>310</v>
       </c>
       <c r="D33" s="1" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
       <c r="E33" s="1" t="s">
         <v>245</v>
@@ -5717,10 +6101,10 @@
         <v>60</v>
       </c>
       <c r="C34" t="s">
-        <v>313</v>
+        <v>311</v>
       </c>
       <c r="D34" s="1" t="s">
-        <v>354</v>
+        <v>352</v>
       </c>
       <c r="E34" s="1" t="s">
         <v>161</v>
@@ -5729,7 +6113,7 @@
         <v>155</v>
       </c>
       <c r="G34" s="1" t="s">
-        <v>367</v>
+        <v>365</v>
       </c>
       <c r="K34" t="s">
         <v>228</v>
@@ -5740,7 +6124,7 @@
         <v>60</v>
       </c>
       <c r="C35" t="s">
-        <v>314</v>
+        <v>312</v>
       </c>
       <c r="D35" s="1" t="s">
         <v>160</v>
@@ -5749,10 +6133,10 @@
         <v>161</v>
       </c>
       <c r="F35" s="1" t="s">
-        <v>368</v>
+        <v>366</v>
       </c>
       <c r="G35" s="1" t="s">
-        <v>369</v>
+        <v>367</v>
       </c>
       <c r="K35" t="s">
         <v>230</v>
@@ -5763,19 +6147,19 @@
         <v>62</v>
       </c>
       <c r="C36" t="s">
-        <v>315</v>
+        <v>313</v>
       </c>
       <c r="D36" s="1" t="s">
         <v>161</v>
       </c>
       <c r="E36" s="1" t="s">
-        <v>355</v>
+        <v>353</v>
       </c>
       <c r="F36" s="1" t="s">
-        <v>353</v>
+        <v>351</v>
       </c>
       <c r="G36" s="1" t="s">
-        <v>356</v>
+        <v>354</v>
       </c>
       <c r="K36" t="s">
         <v>229</v>
@@ -5786,19 +6170,19 @@
         <v>65</v>
       </c>
       <c r="C37" t="s">
-        <v>317</v>
+        <v>315</v>
       </c>
       <c r="D37" s="1" t="s">
-        <v>340</v>
+        <v>338</v>
       </c>
       <c r="E37" s="1" t="s">
         <v>236</v>
       </c>
       <c r="F37" s="1" t="s">
-        <v>359</v>
+        <v>357</v>
       </c>
       <c r="G37" s="1" t="s">
-        <v>346</v>
+        <v>344</v>
       </c>
       <c r="K37" t="s">
         <v>226</v>
@@ -5809,16 +6193,16 @@
         <v>60</v>
       </c>
       <c r="C38" s="1" t="s">
-        <v>322</v>
+        <v>320</v>
       </c>
       <c r="D38" s="1" t="s">
         <v>161</v>
       </c>
       <c r="E38" s="1" t="s">
-        <v>357</v>
+        <v>355</v>
       </c>
       <c r="F38" s="1" t="s">
-        <v>340</v>
+        <v>338</v>
       </c>
       <c r="G38" s="13" t="s">
         <v>236</v>
@@ -5829,7 +6213,7 @@
     </row>
     <row r="39" spans="1:11" x14ac:dyDescent="0.25">
       <c r="K39" s="1" t="s">
-        <v>358</v>
+        <v>356</v>
       </c>
     </row>
   </sheetData>

</xml_diff>